<commit_message>
add support for multi language functionality
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -134,9 +134,6 @@
     <t>en-gb</t>
   </si>
   <si>
-    <t>en-us</t>
-  </si>
-  <si>
     <t>LITTERING_TEXT_1</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
   </si>
   <si>
     <t>LITTERING_TEXT_3</t>
-  </si>
-  <si>
-    <t>nl</t>
   </si>
   <si>
     <t>es</t>
@@ -625,24 +619,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="49.15625" customWidth="1"/>
-    <col min="2" max="2" width="58.20703125" customWidth="1"/>
-    <col min="3" max="3" width="55.83984375" customWidth="1"/>
-    <col min="4" max="4" width="54.62890625" customWidth="1"/>
-    <col min="5" max="5" width="58.9453125" customWidth="1"/>
-    <col min="6" max="6" width="55" customWidth="1"/>
-    <col min="7" max="7" width="48.47265625" customWidth="1"/>
+    <col min="2" max="2" width="62.9453125" customWidth="1"/>
+    <col min="3" max="3" width="58.9453125" customWidth="1"/>
+    <col min="4" max="4" width="55" customWidth="1"/>
+    <col min="5" max="5" width="48.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -650,24 +642,18 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="B2" s="2">
         <f>COUNTIF(A1:A10000,"*LOITERING_TEXT_*")</f>
@@ -685,18 +671,10 @@
         <f>B2</f>
         <v>3</v>
       </c>
-      <c r="F2" s="2">
-        <f>B2</f>
-        <v>3</v>
-      </c>
-      <c r="G2" s="2">
-        <f>B2</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -710,16 +688,10 @@
       <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -733,16 +705,10 @@
       <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -756,16 +722,10 @@
       <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
         <f>COUNTIF(A1:A10000,"*LITTERING_TEXT_*")</f>
@@ -783,18 +743,10 @@
         <f>B6</f>
         <v>4</v>
       </c>
-      <c r="F6" s="1">
-        <f>B6</f>
-        <v>4</v>
-      </c>
-      <c r="G6" s="1">
-        <f>B6</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -808,16 +760,10 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -831,16 +777,10 @@
       <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -854,16 +794,10 @@
       <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -877,16 +811,10 @@
       <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1">
         <f>COUNTIF(A1:A10000,"*NOISECOMPLAINT_TEXT_*")</f>
@@ -904,18 +832,10 @@
         <f t="shared" ref="E11:E42" si="2">B11</f>
         <v>6</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" ref="F11:F42" si="3">B11</f>
-        <v>6</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" ref="G11:G42" si="4">B11</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -929,16 +849,10 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -952,16 +866,10 @@
       <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -975,16 +883,10 @@
       <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -998,16 +900,10 @@
       <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1021,16 +917,10 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -1044,16 +934,10 @@
       <c r="E17" t="s">
         <v>33</v>
       </c>
-      <c r="F17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1">
         <f>COUNTIF(A1:A10000,"*LANDARGUMENT_TEXT_*")</f>
@@ -1071,18 +955,10 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F18" s="1">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
@@ -1096,16 +972,10 @@
       <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -1119,16 +989,10 @@
       <c r="E20" t="s">
         <v>33</v>
       </c>
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -1142,16 +1006,10 @@
       <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1">
         <f>COUNTIF(A1:A10000,"*DISCRIMINATION_TEXT_*")</f>
@@ -1169,18 +1027,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F22" s="1">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
@@ -1194,16 +1044,10 @@
       <c r="E23" t="s">
         <v>33</v>
       </c>
-      <c r="F23" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1">
         <f>COUNTIF(A1:A10000,"*DOMESTICABUSE_TEXT_*")</f>
@@ -1221,18 +1065,10 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="F24" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -1246,16 +1082,10 @@
       <c r="E25" t="s">
         <v>33</v>
       </c>
-      <c r="F25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -1269,16 +1099,10 @@
       <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="F26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1">
         <f>COUNTIF(A1:A10000,"*ASSAULT_TEXT_*")</f>
@@ -1296,18 +1120,10 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="F27" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G27" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
@@ -1321,16 +1137,10 @@
       <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="F28" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
@@ -1344,16 +1154,10 @@
       <c r="E29" t="s">
         <v>33</v>
       </c>
-      <c r="F29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -1367,16 +1171,10 @@
       <c r="E30" t="s">
         <v>33</v>
       </c>
-      <c r="F30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
         <v>22</v>
@@ -1390,16 +1188,10 @@
       <c r="E31" t="s">
         <v>33</v>
       </c>
-      <c r="F31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -1413,16 +1205,10 @@
       <c r="E32" t="s">
         <v>33</v>
       </c>
-      <c r="F32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1">
         <f>COUNTIF(A1:A10000,"*MULTIPLEASSAULTS_TEXT_*")</f>
@@ -1440,18 +1226,10 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F33" s="1">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="G33" s="1">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
         <v>24</v>
@@ -1465,16 +1243,10 @@
       <c r="E34" t="s">
         <v>33</v>
       </c>
-      <c r="F34" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
@@ -1488,16 +1260,10 @@
       <c r="E35" t="s">
         <v>33</v>
       </c>
-      <c r="F35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
@@ -1511,16 +1277,10 @@
       <c r="E36" t="s">
         <v>33</v>
       </c>
-      <c r="F36" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" s="1">
         <f>COUNTIF(A1:A10000,"*TRAFFICINCIDENT_TEXT_*")</f>
@@ -1538,18 +1298,10 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="F37" s="1">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="G37" s="1">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="11.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="38" spans="1:5" ht="11.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
         <v>27</v>
@@ -1563,16 +1315,10 @@
       <c r="E38" t="s">
         <v>33</v>
       </c>
-      <c r="F38" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
@@ -1586,16 +1332,10 @@
       <c r="E39" t="s">
         <v>33</v>
       </c>
-      <c r="F39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
@@ -1609,16 +1349,10 @@
       <c r="E40" t="s">
         <v>33</v>
       </c>
-      <c r="F40" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
@@ -1632,16 +1366,10 @@
       <c r="E41" t="s">
         <v>33</v>
       </c>
-      <c r="F41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1">
         <f>COUNTIF(A1:A10000,"*FATALITY_TEXT_*")</f>
@@ -1659,18 +1387,10 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="F42" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G42" s="1">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
@@ -1684,16 +1404,10 @@
       <c r="E43" t="s">
         <v>33</v>
       </c>
-      <c r="F43" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
         <v>32</v>
@@ -1705,12 +1419,6 @@
         <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" t="s">
-        <v>33</v>
-      </c>
-      <c r="G44" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update localization script to use the language index to get the max number in case there are varying values
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="82">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>LANDARGUMENT_TEXT_3</t>
+  </si>
+  <si>
+    <t>LITTERING_LENGTH</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -725,7 +728,7 @@
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1">
         <f>COUNTIF(A1:A10000,"*LITTERING_TEXT_*")</f>

</xml_diff>

<commit_message>
start to prepare to move all strings to be got from the strings file
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580"/>
   </bookViews>
   <sheets>
-    <sheet name="IncidentSpreadsheet" sheetId="3" r:id="rId1"/>
+    <sheet name="StringLocalizations" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -270,6 +270,24 @@
   </si>
   <si>
     <t>LITTERING_LENGTH</t>
+  </si>
+  <si>
+    <t>START_SCREEN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. You must use your resources carefully to solve cases and keep civilians happy and feeling safe.\nBut be careful, officers are limited so use them wisely</t>
+  </si>
+  <si>
+    <t>APP_NAME</t>
+  </si>
+  <si>
+    <t>ResourceForce</t>
+  </si>
+  <si>
+    <t>START_SCREEN_TAP</t>
+  </si>
+  <si>
+    <t>Tap to start!</t>
   </si>
 </sst>
 </file>
@@ -333,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -341,6 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1425,6 +1444,57 @@
         <v>33</v>
       </c>
     </row>
+    <row r="45" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
localize all strings in game and hook them up to the script
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="138">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -275,9 +275,6 @@
     <t>START_SCREEN_DESCRIPTION</t>
   </si>
   <si>
-    <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. You must use your resources carefully to solve cases and keep civilians happy and feeling safe.\nBut be careful, officers are limited so use them wisely</t>
-  </si>
-  <si>
     <t>APP_NAME</t>
   </si>
   <si>
@@ -288,6 +285,159 @@
   </si>
   <si>
     <t>Tap to start!</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_OK</t>
+  </si>
+  <si>
+    <t>OK!</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_WAIT</t>
+  </si>
+  <si>
+    <t>Wait!</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_DEVELOPED</t>
+  </si>
+  <si>
+    <t>Developed Case</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SEND_ONE</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SEND_MANY</t>
+  </si>
+  <si>
+    <t>Send {0} officers for {1} turns</t>
+  </si>
+  <si>
+    <t>Send 1 officer for {0} turns</t>
+  </si>
+  <si>
+    <t>Arrests have been made</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_ARREST_FAIL</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_ARREST_SUCCESS</t>
+  </si>
+  <si>
+    <t>Officers fail to make any arrests regarding the case</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CITIZEN_SUCCESS</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CITIZEN_FAIL</t>
+  </si>
+  <si>
+    <t>Citizens provide evidence through the INSPEC2T app, 2 have been charged</t>
+  </si>
+  <si>
+    <t>Citizen fails to provide any solid evidence for the case</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_NO_MORE_INCIDENTS</t>
+  </si>
+  <si>
+    <t>No more incidents to check this turn</t>
+  </si>
+  <si>
+    <t>INCIDENT_NEW</t>
+  </si>
+  <si>
+    <t>INCIDENT_ONGOING</t>
+  </si>
+  <si>
+    <t>INCIDENT_RESOLVED</t>
+  </si>
+  <si>
+    <t>INCIDENT_CASE</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>INCIDENT_CASE_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_RESOLVED_CASES</t>
+  </si>
+  <si>
+    <t>Arrests</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_ACTIVE_CASES</t>
+  </si>
+  <si>
+    <t>Active Cases</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_TURN</t>
+  </si>
+  <si>
+    <t>Turn</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_GAMEOVER</t>
+  </si>
+  <si>
+    <t>INCIDENT_OFFICERS</t>
+  </si>
+  <si>
+    <t>Officers</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_AVAILABLE</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_TURNS_UNTIL_AVAILABLE</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>turns until available</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_ASK_CITIZEN</t>
+  </si>
+  <si>
+    <t>Ask citizen for help</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_NEXT_TURN</t>
+  </si>
+  <si>
+    <t>Next Turn</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_GAMEOVER_BODY</t>
+  </si>
+  <si>
+    <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. You must use your resources carefully to solve cases and keep civilians happy and feeling safe.*n*But be careful, officers are limited so use them wisely</t>
+  </si>
+  <si>
+    <t>Game Over*n*Too many unresolved cases</t>
+  </si>
+  <si>
+    <t>You Survived {0} Turns*n*And Made Arrests for {1}% of Cases</t>
   </si>
 </sst>
 </file>
@@ -641,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -678,7 +828,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="2">
-        <f>COUNTIF(A1:A10000,"*LOITERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*LOITERING_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C2" s="2">
@@ -750,7 +900,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="1">
-        <f>COUNTIF(A1:A10000,"*LITTERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*LITTERING_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C6" s="1">
@@ -839,7 +989,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="1">
-        <f>COUNTIF(A1:A10000,"*NOISECOMPLAINT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*NOISECOMPLAINT_TEXT_*")</f>
         <v>6</v>
       </c>
       <c r="C11" s="1">
@@ -962,7 +1112,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="1">
-        <f>COUNTIF(A1:A10000,"*LANDARGUMENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*LANDARGUMENT_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C18" s="1">
@@ -1034,7 +1184,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="1">
-        <f>COUNTIF(A1:A10000,"*DISCRIMINATION_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*DISCRIMINATION_TEXT_*")</f>
         <v>1</v>
       </c>
       <c r="C22" s="1">
@@ -1072,7 +1222,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="1">
-        <f>COUNTIF(A1:A10000,"*DOMESTICABUSE_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*DOMESTICABUSE_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C24" s="1">
@@ -1127,7 +1277,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="1">
-        <f>COUNTIF(A1:A10000,"*ASSAULT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*ASSAULT_TEXT_*")</f>
         <v>5</v>
       </c>
       <c r="C27" s="1">
@@ -1233,7 +1383,7 @@
         <v>51</v>
       </c>
       <c r="B33" s="1">
-        <f>COUNTIF(A1:A10000,"*MULTIPLEASSAULTS_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*MULTIPLEASSAULTS_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C33" s="1">
@@ -1305,7 +1455,7 @@
         <v>52</v>
       </c>
       <c r="B37" s="1">
-        <f>COUNTIF(A1:A10000,"*TRAFFICINCIDENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*TRAFFICINCIDENT_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C37" s="1">
@@ -1394,7 +1544,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="1">
-        <f>COUNTIF(A1:A10000,"*FATALITY_TEXT_*")</f>
+        <f>COUNTIF(A1:A10005,"*FATALITY_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C42" s="1">
@@ -1449,7 +1599,7 @@
         <v>82</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>33</v>
@@ -1463,10 +1613,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
         <v>84</v>
-      </c>
-      <c r="B46" t="s">
-        <v>85</v>
       </c>
       <c r="C46" t="s">
         <v>33</v>
@@ -1480,18 +1630,443 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" t="s">
         <v>86</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
         <v>87</v>
       </c>
-      <c r="C47" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" t="s">
+        <v>131</v>
+      </c>
+      <c r="C55" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>132</v>
+      </c>
+      <c r="B59" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" t="s">
+        <v>120</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" t="s">
+        <v>33</v>
+      </c>
+      <c r="E67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>127</v>
+      </c>
+      <c r="B72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change localization script to use a dictiojnary rather than using an array to search throug
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -431,13 +431,13 @@
     <t>BASIC_TEXT_GAMEOVER_BODY</t>
   </si>
   <si>
-    <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. You must use your resources carefully to solve cases and keep civilians happy and feeling safe.*n*But be careful, officers are limited so use them wisely</t>
-  </si>
-  <si>
-    <t>Game Over*n*Too many unresolved cases</t>
-  </si>
-  <si>
-    <t>You Survived {0} Turns*n*And Made Arrests for {1}% of Cases</t>
+    <t>You Survived {0} Turns*2n*And Made Arrests for {1}% of Cases</t>
+  </si>
+  <si>
+    <t>Game Over*2n*Too many unresolved cases</t>
+  </si>
+  <si>
+    <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. You must use your resources carefully to solve cases and keep civilians happy and feeling safe.*2n*But be careful, officers are limited so use them wisely</t>
   </si>
 </sst>
 </file>
@@ -794,7 +794,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1471,7 +1471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="11.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>82</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>33</v>
@@ -2024,7 +2024,7 @@
         <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
add officer requirement number to incident text and also add case number and icon to headers
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="140">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. You must use your resources carefully to solve cases and keep civilians happy and feeling safe.*2n*But be careful, officers are limited so use them wisely</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_OFFICERS_REQUIRED</t>
+  </si>
+  <si>
+    <t>Officers required</t>
   </si>
 </sst>
 </file>
@@ -790,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2069,6 +2075,23 @@
         <v>33</v>
       </c>
     </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
change end game condition and update strings to match
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="142">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -431,12 +431,6 @@
     <t>BASIC_TEXT_GAMEOVER_BODY</t>
   </si>
   <si>
-    <t>You Survived {0} Turns*2n*And Made Arrests for {1}% of Cases</t>
-  </si>
-  <si>
-    <t>Game Over*2n*Too many unresolved cases</t>
-  </si>
-  <si>
     <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. You must use your resources carefully to solve cases and keep civilians happy and feeling safe.*2n*But be careful, officers are limited so use them wisely</t>
   </si>
   <si>
@@ -444,6 +438,18 @@
   </si>
   <si>
     <t>Officers required</t>
+  </si>
+  <si>
+    <t>Citizen Happines</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CITIZEN_HAPPINESS</t>
+  </si>
+  <si>
+    <t>You Survived {0} Turns*2n*Before citizen happiness fell too low, Citizens no longer feel safe under your control</t>
+  </si>
+  <si>
+    <t>Game Over*2n*Citizens not happy with your performance</t>
   </si>
 </sst>
 </file>
@@ -796,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1604,7 +1610,7 @@
         <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
         <v>33</v>
@@ -2012,7 +2018,7 @@
         <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C69" t="s">
         <v>33</v>
@@ -2029,7 +2035,7 @@
         <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>
@@ -2077,18 +2083,35 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" t="s">
         <v>138</v>
       </c>
-      <c r="B73" t="s">
-        <v>139</v>
-      </c>
-      <c r="C73" t="s">
-        <v>33</v>
-      </c>
-      <c r="D73" t="s">
-        <v>33</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="C74" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change game over message and add in high scores
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="146">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -446,10 +446,22 @@
     <t>BASIC_TEXT_CITIZEN_HAPPINESS</t>
   </si>
   <si>
-    <t>You Survived {0} Turns*2n*Before citizen happiness fell too low, Citizens no longer feel safe under your control</t>
-  </si>
-  <si>
-    <t>Game Over*2n*Citizens not happy with your performance</t>
+    <t>BASIC_TEXT_SCORE</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_BEST</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Game Over</t>
+  </si>
+  <si>
+    <t>You Survived {0} Turns*2n*Citizen happiness fallen below 20%, citizens no longer feel safe under your control</t>
   </si>
 </sst>
 </file>
@@ -802,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2018,7 +2030,7 @@
         <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C69" t="s">
         <v>33</v>
@@ -2035,7 +2047,7 @@
         <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>
@@ -2112,6 +2124,40 @@
         <v>33</v>
       </c>
       <c r="E74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make the game more challenging to survive for many turns
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="148">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -311,24 +311,12 @@
     <t>BASIC_TEXT_SEND_MANY</t>
   </si>
   <si>
-    <t>Send {0} officers for {1} turns</t>
-  </si>
-  <si>
-    <t>Send 1 officer for {0} turns</t>
-  </si>
-  <si>
-    <t>Arrests have been made</t>
-  </si>
-  <si>
     <t>BASIC_TEXT_ARREST_FAIL</t>
   </si>
   <si>
     <t>BASIC_TEXT_ARREST_SUCCESS</t>
   </si>
   <si>
-    <t>Officers fail to make any arrests regarding the case</t>
-  </si>
-  <si>
     <t>BASIC_TEXT_CITIZEN_SUCCESS</t>
   </si>
   <si>
@@ -462,6 +450,24 @@
   </si>
   <si>
     <t>You Survived {0} Turns*2n*Citizen happiness fallen below 20%, citizens no longer feel safe under your control</t>
+  </si>
+  <si>
+    <t>Arrests have been made for the following case:</t>
+  </si>
+  <si>
+    <t>Officers fail to make any arrests regarding the case:</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_TURNS_REQUIRED</t>
+  </si>
+  <si>
+    <t>Turns required</t>
+  </si>
+  <si>
+    <t>Send officers</t>
+  </si>
+  <si>
+    <t>Send officer</t>
   </si>
 </sst>
 </file>
@@ -814,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -851,7 +857,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="2">
-        <f>COUNTIF(A1:A10005,"*LOITERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*LOITERING_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C2" s="2">
@@ -923,7 +929,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="1">
-        <f>COUNTIF(A1:A10005,"*LITTERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*LITTERING_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C6" s="1">
@@ -1012,7 +1018,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="1">
-        <f>COUNTIF(A1:A10005,"*NOISECOMPLAINT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*NOISECOMPLAINT_TEXT_*")</f>
         <v>6</v>
       </c>
       <c r="C11" s="1">
@@ -1135,7 +1141,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="1">
-        <f>COUNTIF(A1:A10005,"*LANDARGUMENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*LANDARGUMENT_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C18" s="1">
@@ -1207,7 +1213,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="1">
-        <f>COUNTIF(A1:A10005,"*DISCRIMINATION_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*DISCRIMINATION_TEXT_*")</f>
         <v>1</v>
       </c>
       <c r="C22" s="1">
@@ -1245,7 +1251,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="1">
-        <f>COUNTIF(A1:A10005,"*DOMESTICABUSE_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*DOMESTICABUSE_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C24" s="1">
@@ -1300,7 +1306,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="1">
-        <f>COUNTIF(A1:A10005,"*ASSAULT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*ASSAULT_TEXT_*")</f>
         <v>5</v>
       </c>
       <c r="C27" s="1">
@@ -1406,7 +1412,7 @@
         <v>51</v>
       </c>
       <c r="B33" s="1">
-        <f>COUNTIF(A1:A10005,"*MULTIPLEASSAULTS_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*MULTIPLEASSAULTS_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C33" s="1">
@@ -1478,7 +1484,7 @@
         <v>52</v>
       </c>
       <c r="B37" s="1">
-        <f>COUNTIF(A1:A10005,"*TRAFFICINCIDENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*TRAFFICINCIDENT_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C37" s="1">
@@ -1567,7 +1573,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="1">
-        <f>COUNTIF(A1:A10005,"*FATALITY_TEXT_*")</f>
+        <f>COUNTIF(A1:A10006,"*FATALITY_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C42" s="1">
@@ -1622,7 +1628,7 @@
         <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
         <v>33</v>
@@ -1707,7 +1713,7 @@
         <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="C50" t="s">
         <v>33</v>
@@ -1724,7 +1730,7 @@
         <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
         <v>33</v>
@@ -1755,10 +1761,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
         <v>33</v>
@@ -1772,10 +1778,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
         <v>33</v>
@@ -1789,10 +1795,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C55" t="s">
         <v>33</v>
@@ -1806,10 +1812,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s">
         <v>33</v>
@@ -1823,10 +1829,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
@@ -1840,10 +1846,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C58" t="s">
         <v>33</v>
@@ -1857,10 +1863,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C59" t="s">
         <v>33</v>
@@ -1874,10 +1880,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" t="s">
         <v>107</v>
-      </c>
-      <c r="B60" t="s">
-        <v>111</v>
       </c>
       <c r="C60" t="s">
         <v>33</v>
@@ -1891,10 +1897,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" t="s">
         <v>108</v>
-      </c>
-      <c r="B61" t="s">
-        <v>112</v>
       </c>
       <c r="C61" t="s">
         <v>33</v>
@@ -1908,10 +1914,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" t="s">
         <v>109</v>
-      </c>
-      <c r="B62" t="s">
-        <v>113</v>
       </c>
       <c r="C62" t="s">
         <v>33</v>
@@ -1925,10 +1931,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" t="s">
         <v>110</v>
-      </c>
-      <c r="B63" t="s">
-        <v>114</v>
       </c>
       <c r="C63" t="s">
         <v>33</v>
@@ -1942,10 +1948,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C64" t="s">
         <v>33</v>
@@ -1959,10 +1965,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C65" t="s">
         <v>33</v>
@@ -1976,10 +1982,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B66" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C66" t="s">
         <v>33</v>
@@ -1993,10 +1999,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
         <v>33</v>
@@ -2010,10 +2016,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C68" t="s">
         <v>33</v>
@@ -2027,10 +2033,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B69" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C69" t="s">
         <v>33</v>
@@ -2044,10 +2050,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>
@@ -2061,10 +2067,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B71" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C71" t="s">
         <v>33</v>
@@ -2078,10 +2084,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B72" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C72" t="s">
         <v>33</v>
@@ -2095,10 +2101,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C73" t="s">
         <v>33</v>
@@ -2112,10 +2118,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C74" t="s">
         <v>33</v>
@@ -2129,10 +2135,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C75" t="s">
         <v>33</v>
@@ -2146,10 +2152,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C76" t="s">
         <v>33</v>
@@ -2158,6 +2164,23 @@
         <v>33</v>
       </c>
       <c r="E76" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>138</v>
+      </c>
+      <c r="B77" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update UI to be the same layout as designs ready for sprites to be provided
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="196">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -594,6 +594,24 @@
   </si>
   <si>
     <t>Using citizen information, the officers manage to locate the man and arrest him</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_LOCATION</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_STATUS</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -958,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -996,7 +1014,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3">
-        <f>COUNTIF(A1:A10006,"*LOITERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*LOITERING_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C2" s="3">
@@ -1068,7 +1086,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="2">
-        <f>COUNTIF(A1:A10006,"*LITTERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*LITTERING_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C6" s="2">
@@ -1157,7 +1175,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="2">
-        <f>COUNTIF(A1:A10006,"*NOISECOMPLAINT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*NOISECOMPLAINT_TEXT_*")</f>
         <v>6</v>
       </c>
       <c r="C11" s="2">
@@ -1280,7 +1298,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="2">
-        <f>COUNTIF(A1:A10006,"*LANDARGUMENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*LANDARGUMENT_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C18" s="2">
@@ -1352,7 +1370,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="2">
-        <f>COUNTIF(A1:A10006,"*DISCRIMINATION_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*DISCRIMINATION_TEXT_*")</f>
         <v>1</v>
       </c>
       <c r="C22" s="2">
@@ -1390,7 +1408,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="2">
-        <f>COUNTIF(A1:A10006,"*DOMESTICABUSE_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*DOMESTICABUSE_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C24" s="2">
@@ -1445,7 +1463,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="2">
-        <f>COUNTIF(A1:A10006,"*ASSAULT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*ASSAULT_TEXT_*")</f>
         <v>5</v>
       </c>
       <c r="C27" s="2">
@@ -1551,7 +1569,7 @@
         <v>51</v>
       </c>
       <c r="B33" s="2">
-        <f>COUNTIF(A1:A10006,"*MULTIPLEASSAULTS_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*MULTIPLEASSAULTS_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C33" s="2">
@@ -1623,7 +1641,7 @@
         <v>52</v>
       </c>
       <c r="B37" s="2">
-        <f>COUNTIF(A1:A10006,"*TRAFFICINCIDENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*TRAFFICINCIDENT_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C37" s="2">
@@ -1712,7 +1730,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="2">
-        <f>COUNTIF(A1:A10006,"*FATALITY_TEXT_*")</f>
+        <f>COUNTIF(A1:A10009,"*FATALITY_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C42" s="2">
@@ -2342,61 +2360,61 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>33</v>
@@ -2410,61 +2428,61 @@
     </row>
     <row r="83" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>33</v>
@@ -2478,10 +2496,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>33</v>
@@ -2495,10 +2513,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
@@ -2510,12 +2528,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
@@ -2529,10 +2547,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
@@ -2546,10 +2564,10 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>33</v>
@@ -2563,10 +2581,10 @@
     </row>
     <row r="92" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>33</v>
@@ -2580,10 +2598,10 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>33</v>
@@ -2595,12 +2613,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>33</v>
@@ -2614,10 +2632,10 @@
     </row>
     <row r="95" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>33</v>
@@ -2631,52 +2649,103 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="1" t="s">
+      <c r="C99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="1" t="s">
+      <c r="C100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E98" s="1" t="s">
+      <c r="C101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add background to badgeto allow for customisation of different badge sizes
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="198">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -612,6 +612,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_TYPE</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -976,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="C65" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1014,7 +1020,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3">
-        <f>COUNTIF(A1:A10009,"*LOITERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*LOITERING_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C2" s="3">
@@ -1086,7 +1092,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="2">
-        <f>COUNTIF(A1:A10009,"*LITTERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*LITTERING_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C6" s="2">
@@ -1175,7 +1181,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="2">
-        <f>COUNTIF(A1:A10009,"*NOISECOMPLAINT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*NOISECOMPLAINT_TEXT_*")</f>
         <v>6</v>
       </c>
       <c r="C11" s="2">
@@ -1298,7 +1304,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="2">
-        <f>COUNTIF(A1:A10009,"*LANDARGUMENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*LANDARGUMENT_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C18" s="2">
@@ -1370,7 +1376,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="2">
-        <f>COUNTIF(A1:A10009,"*DISCRIMINATION_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*DISCRIMINATION_TEXT_*")</f>
         <v>1</v>
       </c>
       <c r="C22" s="2">
@@ -1408,7 +1414,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="2">
-        <f>COUNTIF(A1:A10009,"*DOMESTICABUSE_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*DOMESTICABUSE_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C24" s="2">
@@ -1463,7 +1469,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="2">
-        <f>COUNTIF(A1:A10009,"*ASSAULT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*ASSAULT_TEXT_*")</f>
         <v>5</v>
       </c>
       <c r="C27" s="2">
@@ -1569,7 +1575,7 @@
         <v>51</v>
       </c>
       <c r="B33" s="2">
-        <f>COUNTIF(A1:A10009,"*MULTIPLEASSAULTS_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*MULTIPLEASSAULTS_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C33" s="2">
@@ -1641,7 +1647,7 @@
         <v>52</v>
       </c>
       <c r="B37" s="2">
-        <f>COUNTIF(A1:A10009,"*TRAFFICINCIDENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*TRAFFICINCIDENT_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C37" s="2">
@@ -1730,7 +1736,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="2">
-        <f>COUNTIF(A1:A10009,"*FATALITY_TEXT_*")</f>
+        <f>COUNTIF(A1:A10010,"*FATALITY_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C42" s="2">
@@ -2377,10 +2383,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>33</v>
@@ -2394,10 +2400,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>33</v>
@@ -2411,27 +2417,27 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>33</v>
@@ -2445,10 +2451,10 @@
     </row>
     <row r="84" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>33</v>
@@ -2462,10 +2468,10 @@
     </row>
     <row r="85" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>33</v>
@@ -2479,27 +2485,27 @@
     </row>
     <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>33</v>
@@ -2513,10 +2519,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
@@ -2530,10 +2536,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
@@ -2547,10 +2553,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
@@ -2564,44 +2570,44 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="1" t="s">
+      <c r="C92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>33</v>
@@ -2615,61 +2621,61 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="1" t="s">
+      <c r="C95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="1" t="s">
+      <c r="C96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>33</v>
@@ -2683,27 +2689,27 @@
     </row>
     <row r="98" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>33</v>
@@ -2717,10 +2723,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>33</v>
@@ -2734,18 +2740,35 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E101" s="1" t="s">
+      <c r="C102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add try again button to game over and remove automatic restart
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="200">
   <si>
     <t>A group of people have been reported loitering in {0} area</t>
   </si>
@@ -618,6 +618,12 @@
   </si>
   <si>
     <t>Ask citizens for help!</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_TRY_AGAIN</t>
+  </si>
+  <si>
+    <t>Try Again</t>
   </si>
 </sst>
 </file>
@@ -982,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1020,7 +1026,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3">
-        <f>COUNTIF(A1:A10010,"*LOITERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*LOITERING_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C2" s="3">
@@ -1092,7 +1098,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="2">
-        <f>COUNTIF(A1:A10010,"*LITTERING_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*LITTERING_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C6" s="2">
@@ -1181,7 +1187,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="2">
-        <f>COUNTIF(A1:A10010,"*NOISECOMPLAINT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*NOISECOMPLAINT_TEXT_*")</f>
         <v>6</v>
       </c>
       <c r="C11" s="2">
@@ -1304,7 +1310,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="2">
-        <f>COUNTIF(A1:A10010,"*LANDARGUMENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*LANDARGUMENT_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C18" s="2">
@@ -1376,7 +1382,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="2">
-        <f>COUNTIF(A1:A10010,"*DISCRIMINATION_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*DISCRIMINATION_TEXT_*")</f>
         <v>1</v>
       </c>
       <c r="C22" s="2">
@@ -1414,7 +1420,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="2">
-        <f>COUNTIF(A1:A10010,"*DOMESTICABUSE_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*DOMESTICABUSE_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C24" s="2">
@@ -1469,7 +1475,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="2">
-        <f>COUNTIF(A1:A10010,"*ASSAULT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*ASSAULT_TEXT_*")</f>
         <v>5</v>
       </c>
       <c r="C27" s="2">
@@ -1575,7 +1581,7 @@
         <v>51</v>
       </c>
       <c r="B33" s="2">
-        <f>COUNTIF(A1:A10010,"*MULTIPLEASSAULTS_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*MULTIPLEASSAULTS_TEXT_*")</f>
         <v>3</v>
       </c>
       <c r="C33" s="2">
@@ -1647,7 +1653,7 @@
         <v>52</v>
       </c>
       <c r="B37" s="2">
-        <f>COUNTIF(A1:A10010,"*TRAFFICINCIDENT_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*TRAFFICINCIDENT_TEXT_*")</f>
         <v>4</v>
       </c>
       <c r="C37" s="2">
@@ -1736,7 +1742,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="2">
-        <f>COUNTIF(A1:A10010,"*FATALITY_TEXT_*")</f>
+        <f>COUNTIF(A1:A10011,"*FATALITY_TEXT_*")</f>
         <v>2</v>
       </c>
       <c r="C42" s="2">
@@ -1873,10 +1879,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>93</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>33</v>
@@ -1890,10 +1896,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>33</v>
@@ -1907,10 +1913,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>33</v>
@@ -1924,10 +1930,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>33</v>
@@ -1941,10 +1947,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>33</v>
@@ -1958,10 +1964,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>33</v>
@@ -1975,10 +1981,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>33</v>
@@ -1992,10 +1998,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>33</v>
@@ -2009,10 +2015,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>33</v>
@@ -2026,10 +2032,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>33</v>
@@ -2043,10 +2049,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>33</v>
@@ -2060,10 +2066,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>33</v>
@@ -2077,10 +2083,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>33</v>
@@ -2094,10 +2100,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>33</v>
@@ -2111,10 +2117,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>33</v>
@@ -2128,10 +2134,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>33</v>
@@ -2145,10 +2151,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>33</v>
@@ -2162,10 +2168,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>33</v>
@@ -2179,10 +2185,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>33</v>
@@ -2196,44 +2202,44 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>33</v>
@@ -2247,10 +2253,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>33</v>
@@ -2264,10 +2270,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>33</v>
@@ -2281,10 +2287,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>33</v>
@@ -2298,10 +2304,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>196</v>
+        <v>142</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>33</v>
@@ -2315,10 +2321,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>135</v>
+        <v>196</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>33</v>
@@ -2332,10 +2338,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>33</v>
@@ -2349,10 +2355,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>33</v>
@@ -2366,10 +2372,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>33</v>
@@ -2383,10 +2389,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>33</v>
@@ -2400,10 +2406,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>33</v>
@@ -2417,10 +2423,10 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>33</v>
@@ -2434,27 +2440,27 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>33</v>
@@ -2468,10 +2474,10 @@
     </row>
     <row r="85" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>33</v>
@@ -2485,10 +2491,10 @@
     </row>
     <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>33</v>
@@ -2502,27 +2508,27 @@
     </row>
     <row r="87" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
@@ -2536,10 +2542,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
@@ -2553,10 +2559,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
@@ -2570,10 +2576,10 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>33</v>
@@ -2587,44 +2593,44 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="1" t="s">
+      <c r="C93" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>33</v>
@@ -2638,61 +2644,61 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="1" t="s">
+      <c r="C96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="1" t="s">
+      <c r="C97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>33</v>
@@ -2706,27 +2712,27 @@
     </row>
     <row r="99" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>33</v>
@@ -2740,10 +2746,10 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>33</v>
@@ -2757,18 +2763,35 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E102" s="1" t="s">
+      <c r="C103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update strings and add padding to the text boxes
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -419,9 +419,6 @@
     <t>TUTORIAL_TEXT_OFFICERS</t>
   </si>
   <si>
-    <t>The officer indicatior informs you how many officers are available and how many turns until officers in the field return</t>
-  </si>
-  <si>
     <t>TUTORIAL_TEXT_INFORMATION</t>
   </si>
   <si>
@@ -444,6 +441,9 @@
   </si>
   <si>
     <t>Each case will need a number of officers to attend  for a set number of turns</t>
+  </si>
+  <si>
+    <t>The officer indicator informs you how many officers are available and how many turns until officers in the field return and become available again</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1865,7 +1865,7 @@
         <v>130</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -1879,10 +1879,10 @@
     </row>
     <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>0</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -1913,10 +1913,10 @@
     </row>
     <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -1930,10 +1930,10 @@
     </row>
     <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
add warning when incidents expire and made sure incidents do expire correctly
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="142">
   <si>
     <t>XXXX</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>The officer indicator informs you how many officers are available and how many turns until officers in the field return and become available again</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_IGNORE_WARNING</t>
+  </si>
+  <si>
+    <t>WARNING! Selecting wait will cause the case to expire, reducing citizen satisfaction</t>
   </si>
 </sst>
 </file>
@@ -773,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1469,29 +1475,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -1505,10 +1511,10 @@
     </row>
     <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
@@ -1522,10 +1528,10 @@
     </row>
     <row r="44" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
@@ -1539,27 +1545,27 @@
     </row>
     <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -1573,10 +1579,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -1590,10 +1596,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -1607,10 +1613,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -1624,44 +1630,44 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -1675,61 +1681,61 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="1" t="s">
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -1743,27 +1749,27 @@
     </row>
     <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>0</v>
@@ -1777,10 +1783,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>0</v>
@@ -1794,10 +1800,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>0</v>
@@ -1811,27 +1817,27 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>0</v>
@@ -1845,10 +1851,10 @@
     </row>
     <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -1862,10 +1868,10 @@
     </row>
     <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -1879,44 +1885,44 @@
     </row>
     <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="1" t="s">
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -1930,18 +1936,35 @@
     </row>
     <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="1" t="s">
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add support for multiple locations
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,10 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="StringLocalizations" sheetId="3" r:id="rId1"/>
+    <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
+    <sheet name="StringLocalizations_Belfast" sheetId="4" r:id="rId2"/>
+    <sheet name="StringLocalizations_Nicosia" sheetId="5" r:id="rId3"/>
+    <sheet name="StringLocalizations_Groningen" sheetId="6" r:id="rId4"/>
+    <sheet name="StringLocalizations_Valencia" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="142">
   <si>
     <t>XXXX</t>
   </si>
@@ -781,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1972,4 +1976,4788 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.9453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.47265625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.9453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.47265625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.9453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.47265625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.9453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.47265625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update back end to include new scenarios as provided Current Count: Preston - 12 Valencia - 9 Cyprus - 3 Belfast - 0 Groningen - 0
Also addition of initial sprites provided by hajee and the design team
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="413">
   <si>
     <t>XXXX</t>
   </si>
@@ -466,13 +466,1044 @@
   </si>
   <si>
     <t>Please set your location below to get the best experience!</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_6</t>
+  </si>
+  <si>
+    <t>Report of a young female running through the city centre partially clothed and appears distressed.</t>
+  </si>
+  <si>
+    <t>Resolution due to delay in rape being reported vital evidence is lost no arrests made.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Officer eventually locates female who discloses that she has been raped. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait to start rape investigation leading to evidence being lost and although suspect arrested not enough evidence to secure a charge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information allows officers to locate female quickly who discloses that she has been raped </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rape investigation conducted and offender identified and arrested </t>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_5</t>
+  </si>
+  <si>
+    <t>Report of a vehicle being park in an inconsiderate manner on a residential street.</t>
+  </si>
+  <si>
+    <t>Patrol attends and fines that vehicle is not causing an obstruction &amp; cannot do anything refers the matter to council parking services.</t>
+  </si>
+  <si>
+    <t>Information allows dispatch to determine that the matter is not a police one &amp; issue is referred to council parking services.</t>
+  </si>
+  <si>
+    <t>Public are asking for police to dispatch officers to the location</t>
+  </si>
+  <si>
+    <t>Information allows dispatch to determine that the matter is not a police one &amp; issue is referred to council parking services. However due to the delay in resolving matter confidence is lost.</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_7</t>
+  </si>
+  <si>
+    <t>Report of a disabled female in a wheelchair being verbally abused by a young male in the street, there are no cctv cameras in the area.</t>
+  </si>
+  <si>
+    <t>Due to lack of deployment not enough evidence can be obtained to identify &amp; prosecute the offender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Officer attends and take statement from victim and witnesses. Using information suspect is identified </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrest the suspect, using victim &amp; witness statements suspect is successfully prosecuted </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspect eventually arrested and successfully prosecuted at the cost of public confidence </t>
+  </si>
+  <si>
+    <t>Information allows officers to quickly identify the suspect who is arrested a short distance away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspect is successfully prosecuted </t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_INDEX_8</t>
+  </si>
+  <si>
+    <t>Report of two homeless males fighting over a bottle of wine in the city centre.</t>
+  </si>
+  <si>
+    <t>Fight escalates resulting in one of the males smashing the bottle and stabbing the other.</t>
+  </si>
+  <si>
+    <t>Victim bleeds out &amp; dies due to lack of deployment</t>
+  </si>
+  <si>
+    <t>Deploy officers, arrest the offender. Due to the severity of the injury a scene is identified and officers allocated to staff it awaiting CSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forensic evidence allows offender to be successfully prosecuted </t>
+  </si>
+  <si>
+    <t>Information allows officers to identify which of the males was the aggressor. Officer attends and arrests aggressor thus preventing situation escalating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggressor is successfully prosecuted </t>
+  </si>
+  <si>
+    <t>Officer attends and defuses the situation before it gets out of hand however unable to identify who was the aggressor. Both males warned and go their separate ways</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_8</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_9</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_10</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_11</t>
+  </si>
+  <si>
+    <t>Report from a drunk male stating that he has been assaulted inside a busy nightclub. Male refuses an ambulance as he is not seriously injured.</t>
+  </si>
+  <si>
+    <t>Drunk male becomes aggressive with doorstaff and tries picking a fight</t>
+  </si>
+  <si>
+    <t>Drunk male has started attacking a member of doorstaff</t>
+  </si>
+  <si>
+    <t>Deploy an officer, male is arrested for assault after attacking a member of doorstaff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male is successfully prosecuted however still wants to report assault inside the club </t>
+  </si>
+  <si>
+    <t>Male reporting assault inside the club is unable to provide full information and no further arrests can be made</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploy an officer male is arrested for drunk &amp; disorderly however still wanting to report assault once sober in the morning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to drunken state male isn’t able to provide full information and no arrests can be made </t>
+  </si>
+  <si>
+    <t>Drunk male becomes aggressive with officers which results in him being arrested disorderly however still wanting to report assault once sober in the morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information allows officers to identify a suspect and make an arrest </t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_8</t>
+  </si>
+  <si>
+    <t>Report of a group of 10-15 youths gathering outside a fast food restaurant causing a nuisance</t>
+  </si>
+  <si>
+    <t>Officer attends resolves current problem but fails to address long term issues.</t>
+  </si>
+  <si>
+    <t>Information leads to finding identity of youths and reason for them causing problems</t>
+  </si>
+  <si>
+    <t>Officer attends, resolves current issue &amp; long term issues.</t>
+  </si>
+  <si>
+    <t>Nuisance escalates into criminal damage leading to window being smashed.</t>
+  </si>
+  <si>
+    <t>Groups behaviour escalates further &amp; staff member gets assaulted whilst challenging them</t>
+  </si>
+  <si>
+    <t>Offenders identified and arrested</t>
+  </si>
+  <si>
+    <t>Due to time taken key evidence is lost meaning arrests cannot be made</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_6</t>
+  </si>
+  <si>
+    <t>Report of an elderly male being found in a confused state by staff on the train station.</t>
+  </si>
+  <si>
+    <t>Officer attend and discovers that male has been reported missing</t>
+  </si>
+  <si>
+    <t>Officer returns male to family address &amp; submits reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male is eventually returned home however becomes increasingly distressed during the wait and requires officer to spend additional time calming him down </t>
+  </si>
+  <si>
+    <t>Officer calms down the elderly man who was distressed</t>
+  </si>
+  <si>
+    <t>Information obtained identify man as a missing person</t>
+  </si>
+  <si>
+    <t>SCENARIO_10_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_10_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_10_INDEX_3</t>
+  </si>
+  <si>
+    <t>Report of a collision between two vehicles on a busy road, report states that no persons are injured.</t>
+  </si>
+  <si>
+    <t>Report resolved without police deployment. Slight lose of happiness.</t>
+  </si>
+  <si>
+    <t>Officer attends no offences have taken place advices both parties to exchange details. Report resolved</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_INDEX_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_INDEX_6</t>
+  </si>
+  <si>
+    <t>Report of a collision involving two vehicles on a busy road, report is unable to give a specific junction &amp; states that one of the drivers is complaining of neck pain.</t>
+  </si>
+  <si>
+    <t>Delay in reporting causes problems with congestion leading to several incidents of road rage.</t>
+  </si>
+  <si>
+    <t>Officers attend &amp; closes part of the road and take details. One of the drivers smells of alcohol.</t>
+  </si>
+  <si>
+    <t>Driver successfully charged with drink driving.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 driver arrested at scene but wait until additional resources are available to transport into custody </t>
+  </si>
+  <si>
+    <t>Driver eventually transported to custody, due to delay in driver getting into custody alcohol level reduced and driver released without being charged</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_INDEX_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_INDEX_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_INDEX_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_INDEX_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_INDEX_5</t>
+  </si>
+  <si>
+    <t>Report of a shoplifter being detained by security staff at a large retailer</t>
+  </si>
+  <si>
+    <t>Male becomes aggressive and runs away from security, assaulting them in the process</t>
+  </si>
+  <si>
+    <t>Male eventually arrested and prosecuted for theft and assault</t>
+  </si>
+  <si>
+    <t>Due to delay in deployment key evidence is lost &amp; prosecution no longer possible</t>
+  </si>
+  <si>
+    <t>Information reveals that shoplifter has never been in trouble previously and can issued a fixed penalty for the theft. Report concluded</t>
+  </si>
+  <si>
+    <t>A neighbor complains about noise from nearby house</t>
+  </si>
+  <si>
+    <t>A neighbor's dog is barking</t>
+  </si>
+  <si>
+    <t>As a result of the fight a woman is screaming out of her lungs to her husband regarding a difference they had related to their child.</t>
+  </si>
+  <si>
+    <t>A citizen reports that a kid is heard crying produsely from the back side of the house looking through the slightly open door</t>
+  </si>
+  <si>
+    <t>As soon as the parents realise the absense of the kid they decide to file a report through the INSPEC2T app.</t>
+  </si>
+  <si>
+    <t>The woman rushes out of the house gets in the car and starts looking for the kid; she is in panic mode and drives recklessly. As a result she hits an electricity pillar</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_8</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_9</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_11</t>
+  </si>
+  <si>
+    <t>The police surrounds the area to avoid any chances of electrocution or the generation of fire</t>
+  </si>
+  <si>
+    <t>returned to the nearby police station</t>
+  </si>
+  <si>
+    <t>The officer visited the reported location and resolved the issue. A couple was arguing in the precense of a 9 yr old kid. None of the parents wanted to file the incident.</t>
+  </si>
+  <si>
+    <t>The officer visited the reported location and resolved the issue. A couple was arguing in the precense of a 9 yr old kid. However the officer needed to transfer the child to the social services and ensure that everything is ok</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_10</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_12</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_13</t>
+  </si>
+  <si>
+    <t>Officers find the kid and they immediately contact hs parents</t>
+  </si>
+  <si>
+    <t>The situation escalated with no reason. The woman was saved by miracle and the boy was found by citizens</t>
+  </si>
+  <si>
+    <t>The situation escalated with no reason. The woman was saved by miracle and the boy was found by officers</t>
+  </si>
+  <si>
+    <t>A citizen reported littering in around his neighbourhood. His newly moved neighbors do not seem to respect others' space</t>
+  </si>
+  <si>
+    <t>The citizen's trust in police is decreased</t>
+  </si>
+  <si>
+    <t>A citizen reported littering in around his neighbourhood for the second time</t>
+  </si>
+  <si>
+    <t>The two neighbours are involved in an argument</t>
+  </si>
+  <si>
+    <t>The argument escalated on a fight which required the intervention of the police. The two neighbours seem to be unfriendly with each other with the issue between them still unresolved</t>
+  </si>
+  <si>
+    <t>A police officer resolves the issue and the two neighbours restored their trust in police and managed to build a strong relationship</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_INDEX_8</t>
+  </si>
+  <si>
+    <t>A citizen reported that her dog got sick after their walk around the neighbourhood and claimed the existence of pet poison around the area</t>
+  </si>
+  <si>
+    <t>Multiple citizens reported the existense of pet poison through the use of the INSPEC2T app. Some of them also associated the event with a number of locations. Thanks to the spatiotemporal processing in INSPEC2T. The system suggested the correlation of some reports and provided an estimation of the location.</t>
+  </si>
+  <si>
+    <t>Thanks to system indications and the contribution of citizens the officer managed to find and remove the poison within the area</t>
+  </si>
+  <si>
+    <t>The officers spent a long time on this but it paid off. They have managed to identify the poison and cleared the area.</t>
+  </si>
+  <si>
+    <t>Broadcasted a message to the area and urged anyone knowing anything about the event to contact the police or file a report. The case is not closed until the perpetrator is found</t>
+  </si>
+  <si>
+    <t>Multiple citizens provided key information to the police about a person that seems to be responsible for putting the poison to the area</t>
+  </si>
+  <si>
+    <t>The suspect is being arrested and is sent for questioning</t>
+  </si>
+  <si>
+    <t>The public seems to be losing trust in the police. They feel that the system does not work and get discouraged in providing input in the future</t>
+  </si>
+  <si>
+    <t>Youth group making graffiti</t>
+  </si>
+  <si>
+    <t>The group makes more damage by throwing stones to the windows of the library</t>
+  </si>
+  <si>
+    <t>When the patrol arrives, the group escapes</t>
+  </si>
+  <si>
+    <t>The patrol localizes one suspect, but is not sure that is implicated</t>
+  </si>
+  <si>
+    <r>
+      <t>A citizen sends in a recording of the incident via the INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T app</t>
+    </r>
+  </si>
+  <si>
+    <t>The supervisor recognizes one of the teenagers as a user of the library, making possible to catch the group</t>
+  </si>
+  <si>
+    <t>Two drug-addicts are injecting heroine near the school</t>
+  </si>
+  <si>
+    <t>One of the fathers reprimands for their actions and starts arguing. He gets injured.</t>
+  </si>
+  <si>
+    <t>A school-boy founds the syringe used by drug-addicts and pinches himself with a needle.</t>
+  </si>
+  <si>
+    <t>A witness records drug-addicts and the place where they leave their syringes</t>
+  </si>
+  <si>
+    <t>Drug-addicts are identified, fined and the syringes are localized</t>
+  </si>
+  <si>
+    <t>The injured receive medical assistance; one of the drug-addicts is arrested for the result of his aggression.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the drag-addicts is identified, but the other one tries to run, throwing away the syringes. </t>
+  </si>
+  <si>
+    <t>Two cars had an accident inside of the tunnel. The drivers started an argument</t>
+  </si>
+  <si>
+    <t>Other drivers are inattentive watching the scene; and another accident happen, this time with serious injuries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the injured dies without having been attended. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The incident is reported, seriously wounded are taken to the hospital. One of the culprits runs. </t>
+  </si>
+  <si>
+    <t>The incident is reported, the traffic is brought back to normal, but one of the drivers involved managed to run.</t>
+  </si>
+  <si>
+    <t>The incident is reported the victims are taken to the hospital if necessary, the traffic is brought back to normal, but one of the of the drivers involved ran and there was one death.</t>
+  </si>
+  <si>
+    <t>The accident is taken care of and however one of the drivers ran, it was possible to localize him knowing license plate numbers of his car</t>
+  </si>
+  <si>
+    <r>
+      <t>One of the witnesses shares a photo of the incident with plates of the vehicles involved via INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T.</t>
+    </r>
+  </si>
+  <si>
+    <t>Grupo de jóvenes haciendo grafitis</t>
+  </si>
+  <si>
+    <t>El encargado de la biblioteca no puede ser localizado</t>
+  </si>
+  <si>
+    <t>El grupo causa más daños lanzando piedras a las ventanas de la biblioteca</t>
+  </si>
+  <si>
+    <t>Cuando las patrullas llegan, el grupo escapa</t>
+  </si>
+  <si>
+    <t>La patrulla localiza a un sospechoso, pero no es seguro que esté implicado</t>
+  </si>
+  <si>
+    <t>El supervisor reconoce a uno de los jóvenes como usuario de la biblioteca, haciendo posible identificar al resto del grupo</t>
+  </si>
+  <si>
+    <t>Dos toxicómanos inyectándose heroína junto a un colegio</t>
+  </si>
+  <si>
+    <t>El padre de un alumno les reprocha su actitud y se inicia una pelea. Es herido</t>
+  </si>
+  <si>
+    <t>Un menor escolar se pincha con una aguja de una jeringuilla de los toxicómanos</t>
+  </si>
+  <si>
+    <t>Un testigo graba a los toxicómanos y dónde dejan las jeringuillas</t>
+  </si>
+  <si>
+    <t>Los toxicómanos son identificados y multados y las jeringuillas localizadas</t>
+  </si>
+  <si>
+    <t>Los heridos son atendidos y uno de los toxicómanos es detenidos por el resultado de la agresión</t>
+  </si>
+  <si>
+    <t>Uno de los toxicómanos es identificado pero el otro emprende la huida, tirando la jeringuill</t>
+  </si>
+  <si>
+    <t>Accidente entre dos turismos en el interior de un túnel. Los conductores se enzarzan en una discusión.</t>
+  </si>
+  <si>
+    <t>Debido al efecto “mirón”, se produce otro accidente, esta vez con heridos graves.</t>
+  </si>
+  <si>
+    <t>Uno de los heridos fallece al no ser atendido urgentemente</t>
+  </si>
+  <si>
+    <t>Se instruye atestado y varios heridos graves son trasladados al hospital. Fuga de uno de los implicados en el accidente.</t>
+  </si>
+  <si>
+    <t>Se instruye atestado y se normaliza el tráfico, pero una unidad implicada en el accidente ha huido.</t>
+  </si>
+  <si>
+    <t>Se instruye atestado, se atiende a los heridos y se normaliza el tráfico, pero una unidad implicada en el accidente ha huido y hay un fallecido.</t>
+  </si>
+  <si>
+    <t>Se logra atender el accidente, y pese a que un conductor ha huido, es localizado a través de la placa de matrícula de su vehículo.</t>
+  </si>
+  <si>
+    <r>
+      <t>Un ciudadano envía una grabación a través de la App de INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Un conductor testigo de los hechos comparte a través de INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T una foto con la matrícula de los vehículos implicados.</t>
+    </r>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_7</t>
+  </si>
+  <si>
+    <t>A group of young people is drinking alcohol in residential area with the music blasting from one of their cars</t>
+  </si>
+  <si>
+    <t>Upon seeing the patrol, they turn the music down. One of the vehicles tries to flee</t>
+  </si>
+  <si>
+    <t>A taxi driver is returning home sees the situation and reprimands the culprits, which causes a fight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The claimant has photos of the whole situation and of license plates of cars involved taken. </t>
+  </si>
+  <si>
+    <t>The police is able to intercept the fled vehicle and detains the driver for previous charges. The others, though, go on consuming alcohol and blasting music</t>
+  </si>
+  <si>
+    <t>The fight was stopped, but two officers had been injured.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They could intercept the fled car and detain the driver. Thanks to the INSPEC2T they manage to find the rest of the group. </t>
+  </si>
+  <si>
+    <t>SCENARIO_5_INDEX_8</t>
+  </si>
+  <si>
+    <t>A man hits his wife in presence of their child.</t>
+  </si>
+  <si>
+    <t>The victim and the minor receive assistance from the CP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The aggressor takes the minor somewhere. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trace the aggressor, but not provide the victim with proper medical assistance. </t>
+  </si>
+  <si>
+    <t>They provide medical assistance for the victim and her child. The police couldn´t find the aggressor</t>
+  </si>
+  <si>
+    <t>Guarantee medical assistance for the victim and prevent the aggression against the minor due to his prompt localization.</t>
+  </si>
+  <si>
+    <r>
+      <t>Via INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T a witness uploads the recording of the escape of the aggressor and his location</t>
+    </r>
+  </si>
+  <si>
+    <t>They are able to localize the minor, but he is injured and his mother has irreversible head injuries since she never was given medical assistance</t>
+  </si>
+  <si>
+    <t>The owner of the dog was injured while trying to stop the fight between his dog and another one on the dog beach</t>
+  </si>
+  <si>
+    <t>After having searched the area, the police wasn’t able to find neither the aggressor dog, nor his owner.</t>
+  </si>
+  <si>
+    <t>They provided medical assistance for the injured person. The aggressor dog is still being sought. The injured dog dies</t>
+  </si>
+  <si>
+    <t>The aggressor dog is still being sought, but the injured person and his dog receive medical assistance on time</t>
+  </si>
+  <si>
+    <t>The injured person received medical assistance, the wounded dog was saved and due to the photo that added to the verbal description provided, the police was able to localize the owner of the aggressor dog with his pet</t>
+  </si>
+  <si>
+    <t>In the surrounding area of the Mestalla football stadium broke windows and robbed from the inside few vehicles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide deterrent police presence and help and guidance for victims. </t>
+  </si>
+  <si>
+    <t>A witness shares through INSPEC2T the picture of a suspect who he has seen trying to force the lock of the vehicle.</t>
+  </si>
+  <si>
+    <t>New robberies in another area occurred, one of them with physical violence. The suspect is still missing</t>
+  </si>
+  <si>
+    <t>The author of the robberies is found and more damages are avoided. The owners of the damaged vehicles aren’t attended or advised</t>
+  </si>
+  <si>
+    <t>The affected people are attended; however the thief is missing</t>
+  </si>
+  <si>
+    <r>
+      <t>Via INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">T a swimmer shares a panoramic photo of the area. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The police officer that coordinates theINSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T compares the information from the ID from the wallet with the photo of the suspect and deduces that this is the same man. Later he found and detained due to the photos and documents..</t>
+    </r>
+  </si>
+  <si>
+    <t>Un grupo de jóvenes se encuentra con sus vehículos en zona residencial con la música alta y bebiendo alcohol</t>
+  </si>
+  <si>
+    <t>Un taxista que finaliza su turno de trabajo les llama la atención  y se inicia una pelea</t>
+  </si>
+  <si>
+    <t>El reclamante ha grabado la escena y posee imágenes de las matrículas de los  vehículos  que se encuentran allí</t>
+  </si>
+  <si>
+    <t>Se logra interceptar al vehículo fugado y se detiene a su conductor al tener antecedentes. El resto de los jóvenes vuelve a poner música y consumir alcohol</t>
+  </si>
+  <si>
+    <t>Se intercede en la pelea con el resultado de varios heridos</t>
+  </si>
+  <si>
+    <t>Se logra interceptar al vehículo fugado y se detiene a su conductor al tener antecedentes. El resto del grupo es localizado a posteriori gracias a INSPEC2T</t>
+  </si>
+  <si>
+    <t>Un varón golpea a su pareja en presencia del hijo de ambos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atención a la víctima y al menor por parte del PB de la zona </t>
+  </si>
+  <si>
+    <t>El agresor se lleva al menor del lugar</t>
+  </si>
+  <si>
+    <t>Localización del agresor pero asistencia de la víctima deficiente</t>
+  </si>
+  <si>
+    <t>El menor ha sido localizado pero presenta lesiones de consideración, y la madre ha sufrido daños irreversibles por la demora en su atención sanitaria</t>
+  </si>
+  <si>
+    <t>No se localiza al agresor pero se atiende a las víctimas</t>
+  </si>
+  <si>
+    <t>Atención adecuada de la víctima y prevención de la agresión al menor al ser localizado con prontitud.</t>
+  </si>
+  <si>
+    <t>El dueño de un can ha sufrido heridas al interceder en una pelea entre su perro y otro, en la zona de baño para animales de la playa</t>
+  </si>
+  <si>
+    <t>Tras realizar batidas por la zona no se consigue localizar al perro agresor ni a su dueño</t>
+  </si>
+  <si>
+    <t>Se atiende a la persona lesionada y no se localiza al perro agresor. El perro agredido fallece.</t>
+  </si>
+  <si>
+    <t>No se localiza al perro agresor pero la víctima es tratada y el perro herido es tratado a tiempo y no fallece.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanto la persona que ha sufrido  el mordisco como su perro son atendidos a tiempo y gracias a la imagen compartida se logra contrastar la descripción verbal de los testigos , capturándose acto seguido al dueño y a su perro. </t>
+  </si>
+  <si>
+    <t>dEn la zona de estacionamiento contigua al estadio de fútbol de Mestalla varios vehículos han sufrido robo de enseres por el 
+método de fractura de luna</t>
+  </si>
+  <si>
+    <t>Presencia disuasoria policial y atención y asesoramiento a los afectados</t>
+  </si>
+  <si>
+    <t>Un aficionado localiza una cartera con documentación junto a uno de los vehículos dañados y lo comparte a través de INSPEC2T</t>
+  </si>
+  <si>
+    <t>localizada a posteriori gracias a la documentación y arrestada</t>
+  </si>
+  <si>
+    <t>Se localiza al autor de los daños y se evitan nuevos robos, pero no se asesora a los afectados</t>
+  </si>
+  <si>
+    <t>Se atiende y asiste a los afectados pero no se localiza al autor.</t>
+  </si>
+  <si>
+    <r>
+      <t>A través de INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T un testigo de los hechos graba la huida del agresor y su localización</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A través de INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">T un bañista comparte una imagen panorámica de la zona </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Un testigo comparte a través de INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">T una imagen de un sospechoso que ha visto intentando abrir un vehículo </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>El agente de policía coordinador de INSPEC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T coteja la información de la documentación hallada con la imagen subida a INSPEC2T y deduce que es la misma persona. Es localizada a posteriori gracias a la documentación y arrestada</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,13 +1517,62 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA7C0DE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -507,12 +1587,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -795,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132:B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1544,10 +2651,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>77</v>
+        <v>124</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
@@ -1559,12 +2666,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>78</v>
+        <v>126</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -1576,12 +2683,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>79</v>
+        <v>128</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -1593,12 +2700,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>80</v>
+        <v>130</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -1610,12 +2717,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>81</v>
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -1629,10 +2736,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>82</v>
+        <v>137</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -1644,12 +2751,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>133</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -1661,12 +2768,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>98</v>
+        <v>135</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -1678,29 +2785,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -1714,10 +2821,10 @@
     </row>
     <row r="54" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -1729,12 +2836,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -1746,12 +2853,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -1763,12 +2870,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
@@ -1780,29 +2887,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>0</v>
@@ -1814,12 +2921,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>0</v>
@@ -1833,10 +2940,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>0</v>
@@ -1848,12 +2955,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>0</v>
@@ -1867,10 +2974,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -1884,10 +2991,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>125</v>
+        <v>89</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -1899,12 +3006,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>127</v>
+        <v>90</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>0</v>
@@ -1916,12 +3023,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>129</v>
+        <v>91</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -1933,12 +3040,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>139</v>
+        <v>92</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -1950,12 +3057,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>132</v>
+        <v>93</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -1969,10 +3076,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>94</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
@@ -1984,12 +3091,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>134</v>
+        <v>95</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>0</v>
@@ -2001,12 +3108,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>136</v>
+        <v>96</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>0</v>
@@ -2015,6 +3122,1111 @@
         <v>0</v>
       </c>
       <c r="E71" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E136" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3256,10 +5468,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B68" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4005,10 +6217,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>77</v>
+        <v>124</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
@@ -4020,12 +6232,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>78</v>
+        <v>126</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -4037,12 +6249,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>79</v>
+        <v>128</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -4054,12 +6266,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>80</v>
+        <v>130</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -4071,12 +6283,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>81</v>
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -4090,10 +6302,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>82</v>
+        <v>137</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -4105,12 +6317,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>133</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -4122,12 +6334,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>98</v>
+        <v>135</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -4139,29 +6351,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="1" t="s">
-        <v>85</v>
+    <row r="52" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>100</v>
+        <v>276</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -4175,10 +6387,10 @@
     </row>
     <row r="54" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>101</v>
+        <v>277</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -4190,12 +6402,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>102</v>
+        <v>278</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -4207,12 +6419,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" ht="26.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>103</v>
+        <v>75</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -4226,10 +6438,10 @@
     </row>
     <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>104</v>
+        <v>280</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
@@ -4241,12 +6453,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
-        <v>91</v>
+        <v>281</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>0</v>
@@ -4258,12 +6470,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
-        <v>92</v>
+        <v>282</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>106</v>
+        <v>286</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>0</v>
@@ -4275,12 +6487,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>93</v>
+        <v>283</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>107</v>
+        <v>287</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>0</v>
@@ -4292,12 +6504,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>94</v>
+        <v>289</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>108</v>
+        <v>288</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>0</v>
@@ -4311,10 +6523,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>95</v>
+        <v>284</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>109</v>
+        <v>292</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>0</v>
@@ -4326,12 +6538,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>290</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>110</v>
+        <v>293</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -4343,12 +6555,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>125</v>
+        <v>291</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -4360,29 +6572,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>129</v>
+        <v>84</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>296</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -4394,12 +6606,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>139</v>
+        <v>85</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -4411,12 +6623,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>132</v>
+        <v>86</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -4428,12 +6640,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>87</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>299</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
@@ -4445,12 +6657,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>134</v>
+        <v>88</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>300</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>0</v>
@@ -4462,20 +6674,139 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="1" t="s">
+    <row r="71" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5716,18 +8047,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B105" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="58.9453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.89453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="48.47265625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
@@ -6465,367 +8796,368 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="1" t="s">
+      <c r="B52" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="1" t="s">
+      <c r="B53" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="1" t="s">
+      <c r="B54" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="1" t="s">
+      <c r="B55" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="1" t="s">
+      <c r="B56" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="1" t="s">
+      <c r="B57" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="1" t="s">
+      <c r="B59" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="1" t="s">
+      <c r="B60" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="1" t="s">
+      <c r="B61" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="1" t="s">
+      <c r="B62" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="1" t="s">
+      <c r="B63" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="1" t="s">
+      <c r="B64" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>127</v>
+      <c r="B65" s="11" t="s">
+        <v>323</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>0</v>
@@ -6833,33 +9165,33 @@
       <c r="D65" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E65" s="10" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>325</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -6867,16 +9199,16 @@
       <c r="D67" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E67" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>132</v>
+        <v>148</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>326</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -6884,16 +9216,16 @@
       <c r="D68" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E68" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="39.299999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>149</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>331</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
@@ -6901,16 +9233,16 @@
       <c r="D69" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E69" s="11" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>134</v>
+        <v>150</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>327</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>0</v>
@@ -6918,16 +9250,16 @@
       <c r="D70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E70" s="11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>136</v>
+        <v>151</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>328</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>0</v>
@@ -6935,8 +9267,535 @@
       <c r="D71" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>0</v>
+      <c r="E71" s="11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="49.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="50.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add game over screeen art assets
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2295" uniqueCount="415">
   <si>
     <t>XXXX</t>
   </si>
@@ -1497,6 +1497,12 @@
       </rPr>
       <t>T coteja la información de la documentación hallada con la imagen subida a INSPEC2T y deduce que es la misma persona. Es localizada a posteriori gracias a la documentación y arrestada</t>
     </r>
+  </si>
+  <si>
+    <t>BASIC_TEXT_DOWNLOAD</t>
+  </si>
+  <si>
+    <t>Download the INSPEC2T App Now!</t>
   </si>
 </sst>
 </file>
@@ -8047,10 +8053,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B105" sqref="A1:XFD1048576"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8745,44 +8751,44 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
@@ -8796,27 +8802,27 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -8830,10 +8836,10 @@
     </row>
     <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -8847,10 +8853,10 @@
     </row>
     <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -8864,44 +8870,44 @@
     </row>
     <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="1" t="s">
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -8915,232 +8921,232 @@
     </row>
     <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="3" t="s">
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1" t="s">
+      <c r="C53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E53" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:6" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="11" t="s">
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="11" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="11" t="s">
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="11" t="s">
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B58" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="10" t="s">
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="F57" s="7"/>
-    </row>
-    <row r="58" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="1" t="s">
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B59" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="11" t="s">
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="3" t="s">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B60" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="11" t="s">
+      <c r="C60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="11" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B61" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="10" t="s">
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="10" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B62" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="11" t="s">
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="11" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B63" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="10" t="s">
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="10" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -9149,190 +9155,190 @@
         <v>0</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B66" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="10" t="s">
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="3" t="s">
+    <row r="67" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B67" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="11" t="s">
+      <c r="C67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B68" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" s="11" t="s">
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="11" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B69" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="10" t="s">
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="10" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="39.299999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:5" ht="39.299999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B70" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="11" t="s">
+      <c r="C70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B72" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="11" t="s">
+      <c r="C72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="11" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>329</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B74" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="11" t="s">
+      <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="11" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="3" t="s">
+    <row r="75" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="1" t="s">
+      <c r="C75" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E75" s="11" t="s">
@@ -9341,10 +9347,10 @@
     </row>
     <row r="76" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>0</v>
@@ -9353,352 +9359,352 @@
         <v>0</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="10" t="s">
+      <c r="C78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="10" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="10" t="s">
+      <c r="C79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="10" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="11" t="s">
+      <c r="C80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="10" t="s">
+      <c r="C81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="10" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="3" t="s">
+    <row r="82" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B82" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="C81" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="11" t="s">
+      <c r="C82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="11" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B84" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="11" t="s">
+      <c r="C84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="11" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="B85" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="11" t="s">
+      <c r="C85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="11" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="B86" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="11" t="s">
+      <c r="C86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="11" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B87" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E86" s="11" t="s">
+      <c r="C87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="11" t="s">
         <v>395</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B89" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="11" t="s">
+      <c r="C89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="11" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="3" t="s">
+    <row r="90" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="11" t="s">
+      <c r="C90" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="11" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="11" t="s">
+      <c r="C91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="11" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="11" t="s">
+      <c r="C92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="11" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E92" s="11" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E93" s="11" t="s">
+      <c r="C94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="11" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="49.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:5" ht="49.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="10" t="s">
+      <c r="C95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="3" t="s">
+    <row r="96" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="11" t="s">
+      <c r="C96" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="11" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="11" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>378</v>
@@ -9709,92 +9715,109 @@
       <c r="D97" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="E97" s="11" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="10" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E98" s="11" t="s">
+      <c r="C99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="11" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="50.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:5" ht="50.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E99" s="10" t="s">
+      <c r="C100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="10" t="s">
         <v>412</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="10" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E101" s="10" t="s">
+      <c r="C102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="10" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="11" t="s">
+      <c r="C103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="11" t="s">
         <v>408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add settings menu to game
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="422">
   <si>
     <t>XXXX</t>
   </si>
@@ -1507,6 +1507,24 @@
   </si>
   <si>
     <t>No officers available!</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_RESUME</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_QUIT</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SOUND</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Resume Game</t>
+  </si>
+  <si>
+    <t>Quit to Menu</t>
   </si>
 </sst>
 </file>
@@ -4396,10 +4414,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5161,10 +5179,10 @@
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>142</v>
+        <v>416</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>143</v>
+        <v>420</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -5178,61 +5196,61 @@
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -5246,10 +5264,10 @@
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -5261,12 +5279,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -5280,10 +5298,10 @@
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -5297,18 +5315,69 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update strings to include the download link on the start screen move icon to its own folder fade out settings button to make it less imposing
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="424">
   <si>
     <t>XXXX</t>
   </si>
@@ -1525,6 +1525,12 @@
   </si>
   <si>
     <t>Quit to Menu</t>
+  </si>
+  <si>
+    <t>START_SCREEN_INSPECT_TEXT</t>
+  </si>
+  <si>
+    <t>Help your local police force to solve real crimes with the Inspec2t app</t>
   </si>
 </sst>
 </file>
@@ -4414,10 +4420,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5247,27 +5253,27 @@
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -5281,10 +5287,10 @@
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -5298,10 +5304,10 @@
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -5315,44 +5321,44 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="1" t="s">
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -5366,18 +5372,35 @@
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5907,7 +5930,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
change audio  in game set up build for release to publish on google play
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="426">
   <si>
     <t>XXXX</t>
   </si>
@@ -1531,6 +1531,12 @@
   </si>
   <si>
     <t>Help your local police force to solve real crimes with the Inspec2t app</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_BACK</t>
+  </si>
+  <si>
+    <t>Back</t>
   </si>
 </sst>
 </file>
@@ -4420,10 +4426,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4743,10 +4749,10 @@
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>424</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>425</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -4760,10 +4766,10 @@
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>0</v>
@@ -4777,10 +4783,10 @@
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -4794,10 +4800,10 @@
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -4811,10 +4817,10 @@
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
@@ -4828,10 +4834,10 @@
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
@@ -4845,10 +4851,10 @@
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -4862,10 +4868,10 @@
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -4879,10 +4885,10 @@
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -4896,44 +4902,44 @@
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>0</v>
@@ -4947,10 +4953,10 @@
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>0</v>
@@ -4964,10 +4970,10 @@
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>0</v>
@@ -4981,10 +4987,10 @@
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>0</v>
@@ -4998,10 +5004,10 @@
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
@@ -5015,10 +5021,10 @@
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>412</v>
+        <v>118</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
@@ -5032,10 +5038,10 @@
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -5049,10 +5055,10 @@
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>117</v>
+        <v>413</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -5066,10 +5072,10 @@
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -5083,10 +5089,10 @@
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>0</v>
@@ -5100,10 +5106,10 @@
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
@@ -5117,10 +5123,10 @@
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>410</v>
+        <v>109</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>411</v>
+        <v>110</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
@@ -5134,44 +5140,44 @@
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
@@ -5185,10 +5191,10 @@
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -5202,10 +5208,10 @@
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -5219,10 +5225,10 @@
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -5236,10 +5242,10 @@
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>142</v>
+        <v>418</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>143</v>
+        <v>419</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -5253,10 +5259,10 @@
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>422</v>
+        <v>142</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>423</v>
+        <v>143</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -5270,27 +5276,27 @@
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -5304,10 +5310,10 @@
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -5321,10 +5327,10 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -5338,44 +5344,44 @@
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -5389,18 +5395,35 @@
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move back button to be simple text, start to implement credits screen
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="430">
   <si>
     <t>XXXX</t>
   </si>
@@ -1537,6 +1537,18 @@
   </si>
   <si>
     <t>Back</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SETTINGS</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CREDITS</t>
+  </si>
+  <si>
+    <t>Credits</t>
   </si>
 </sst>
 </file>
@@ -4426,10 +4438,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5259,10 +5271,10 @@
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>142</v>
+        <v>426</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>143</v>
+        <v>427</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -5276,10 +5288,10 @@
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -5293,44 +5305,44 @@
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -5344,10 +5356,10 @@
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -5361,10 +5373,10 @@
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -5376,12 +5388,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -5395,35 +5407,69 @@
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="1" t="s">
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Add ability to change location after initial selection. - General bug fixing - Improve quality of buttons - Force language to English for testing
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="432">
   <si>
     <t>XXXX</t>
   </si>
@@ -1549,6 +1549,12 @@
   </si>
   <si>
     <t>Credits</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CHANGE_LOCATION</t>
+  </si>
+  <si>
+    <t>Change Location</t>
   </si>
 </sst>
 </file>
@@ -4438,10 +4444,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5305,10 +5311,10 @@
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>142</v>
+        <v>430</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>143</v>
+        <v>431</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -5322,10 +5328,10 @@
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>422</v>
+        <v>142</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>423</v>
+        <v>143</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -5339,27 +5345,27 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -5373,10 +5379,10 @@
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -5390,10 +5396,10 @@
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -5407,44 +5413,44 @@
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>0</v>
@@ -5458,18 +5464,35 @@
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add how to play text to tutorial to make it clear that it is a tutorial
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="434">
   <si>
     <t>XXXX</t>
   </si>
@@ -1555,6 +1555,12 @@
   </si>
   <si>
     <t>Change Location</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_HOW_TO_PLAY</t>
+  </si>
+  <si>
+    <t>How To Play</t>
   </si>
 </sst>
 </file>
@@ -4444,10 +4450,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5362,27 +5368,27 @@
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -5396,10 +5402,10 @@
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -5413,10 +5419,10 @@
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
@@ -5430,44 +5436,44 @@
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="1" t="s">
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>0</v>
@@ -5481,18 +5487,35 @@
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change inspect link to a feedback button so that users can email their feedback of the apps currently the feedback link is set to felix@playgen,com as placeholder
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="438">
   <si>
     <t>XXXX</t>
   </si>
@@ -1561,6 +1561,18 @@
   </si>
   <si>
     <t>How To Play</t>
+  </si>
+  <si>
+    <t>START_SCREEN_FEEDBACK_TEXT</t>
+  </si>
+  <si>
+    <t>START_SCREEN_SEND_FEEDBACK</t>
+  </si>
+  <si>
+    <t>Send Feedback!</t>
+  </si>
+  <si>
+    <t>Help us to make the app better, by sending us your feedback!</t>
   </si>
 </sst>
 </file>
@@ -4450,10 +4462,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5516,6 +5528,40 @@
         <v>0</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Various fixes from bug list: - Added new screen for resolution - Made it clearer which incident is currently being shown - Change available officers not to say 5/5 but just 5 - Added satisfaction impact to ok and next turn buttons - change satisfaction impact at end of turn to be fpr ignored cases only
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="445">
   <si>
     <t>XXXX</t>
   </si>
@@ -1573,6 +1573,27 @@
   </si>
   <si>
     <t>Help us to make the app better, by sending us your feedback!</t>
+  </si>
+  <si>
+    <t>INCIDENT_AVAILABLE</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SATISFACTION</t>
+  </si>
+  <si>
+    <t>{0}% Satisfaction</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SATISFACTION_END_TURN</t>
+  </si>
+  <si>
+    <t>{0} Ignored Case{1}, -{2}% Satisfaction</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_NO_IGNORED_CASES</t>
+  </si>
+  <si>
+    <t>0 Ignored Cases, No Satisfaction Change</t>
   </si>
 </sst>
 </file>
@@ -4462,10 +4483,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5562,6 +5583,74 @@
         <v>0</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>438</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More changes to UI
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\ResourceForce\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\INSPEC2T\ResourceForce\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -514,9 +514,6 @@
     <t>SCENARIO_4_INDEX_5</t>
   </si>
   <si>
-    <t>Report of a vehicle being park in an inconsiderate manner on a residential street.</t>
-  </si>
-  <si>
     <t>Patrol attends and fines that vehicle is not causing an obstruction &amp; cannot do anything refers the matter to council parking services.</t>
   </si>
   <si>
@@ -565,9 +562,6 @@
     <t xml:space="preserve">Suspect eventually arrested and successfully prosecuted at the cost of public confidence </t>
   </si>
   <si>
-    <t>Information allows officers to quickly identify the suspect who is arrested a short distance away</t>
-  </si>
-  <si>
     <t xml:space="preserve">Suspect is successfully prosecuted </t>
   </si>
   <si>
@@ -778,9 +772,6 @@
     <t>Report of a collision between two vehicles on a busy road, report states that no persons are injured.</t>
   </si>
   <si>
-    <t>Report resolved without police deployment. Slight lose of happiness.</t>
-  </si>
-  <si>
     <t>Officer attends no offences have taken place advices both parties to exchange details. Report resolved</t>
   </si>
   <si>
@@ -845,9 +836,6 @@
   </si>
   <si>
     <t>Due to delay in deployment key evidence is lost &amp; prosecution no longer possible</t>
-  </si>
-  <si>
-    <t>Information reveals that shoplifter has never been in trouble previously and can issued a fixed penalty for the theft. Report concluded</t>
   </si>
   <si>
     <t>A neighbor complains about noise from nearby house</t>
@@ -1594,6 +1582,18 @@
   </si>
   <si>
     <t>0 Ignored Cases, No Satisfaction Change</t>
+  </si>
+  <si>
+    <t>Report of a vehicle being parked in an inconsiderate manner on a residential street.</t>
+  </si>
+  <si>
+    <t>Information allows officers to quickly identify the suspect who is can be arrested a short distance away</t>
+  </si>
+  <si>
+    <t>Report resolved without police deployment. Slight loss of happiness.</t>
+  </si>
+  <si>
+    <t>Information reveals that shoplifter has never been in trouble previously and was issued a fixed penalty for the theft. Report concluded</t>
   </si>
 </sst>
 </file>
@@ -2001,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A2:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2474,12 +2474,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>161</v>
+        <v>441</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>0</v>
@@ -2496,7 +2496,7 @@
         <v>157</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
@@ -2513,7 +2513,7 @@
         <v>158</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>0</v>
@@ -2530,7 +2530,7 @@
         <v>159</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>0</v>
@@ -2547,7 +2547,7 @@
         <v>160</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>0</v>
@@ -2561,10 +2561,10 @@
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>0</v>
@@ -2578,10 +2578,10 @@
     </row>
     <row r="34" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
@@ -2595,10 +2595,10 @@
     </row>
     <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
@@ -2612,10 +2612,10 @@
     </row>
     <row r="36" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -2629,10 +2629,10 @@
     </row>
     <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -2646,10 +2646,10 @@
     </row>
     <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>178</v>
+        <v>442</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -2663,10 +2663,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>0</v>
@@ -2680,10 +2680,10 @@
     </row>
     <row r="40" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>0</v>
@@ -2697,10 +2697,10 @@
     </row>
     <row r="41" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -2731,10 +2731,10 @@
     </row>
     <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
@@ -2765,10 +2765,10 @@
     </row>
     <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -2782,10 +2782,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -2799,10 +2799,10 @@
     </row>
     <row r="47" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -2816,10 +2816,10 @@
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>0</v>
@@ -2833,10 +2833,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -2850,10 +2850,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -2867,10 +2867,10 @@
     </row>
     <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -2884,10 +2884,10 @@
     </row>
     <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="53" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -2918,10 +2918,10 @@
     </row>
     <row r="54" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -2935,10 +2935,10 @@
     </row>
     <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
@@ -2952,10 +2952,10 @@
     </row>
     <row r="56" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -2969,10 +2969,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
@@ -2986,10 +2986,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>0</v>
@@ -3003,10 +3003,10 @@
     </row>
     <row r="59" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>0</v>
@@ -3020,10 +3020,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>0</v>
@@ -3037,10 +3037,10 @@
     </row>
     <row r="61" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>0</v>
@@ -3054,10 +3054,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>0</v>
@@ -3071,10 +3071,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="64" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -3105,10 +3105,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>0</v>
@@ -3122,10 +3122,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -3139,10 +3139,10 @@
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -3173,10 +3173,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
@@ -3190,10 +3190,10 @@
     </row>
     <row r="70" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>0</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>0</v>
@@ -3224,10 +3224,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>0</v>
@@ -3241,10 +3241,10 @@
     </row>
     <row r="73" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>0</v>
@@ -3258,10 +3258,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>249</v>
+        <v>443</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>0</v>
@@ -3275,10 +3275,10 @@
     </row>
     <row r="75" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>250</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>0</v>
@@ -3292,10 +3292,10 @@
     </row>
     <row r="76" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>0</v>
@@ -3309,10 +3309,10 @@
     </row>
     <row r="77" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>0</v>
@@ -3326,10 +3326,10 @@
     </row>
     <row r="78" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>0</v>
@@ -3343,10 +3343,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>0</v>
@@ -3360,10 +3360,10 @@
     </row>
     <row r="80" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>0</v>
@@ -3377,10 +3377,10 @@
     </row>
     <row r="81" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>0</v>
@@ -3394,10 +3394,10 @@
     </row>
     <row r="82" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>0</v>
@@ -3411,10 +3411,10 @@
     </row>
     <row r="83" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>0</v>
@@ -3428,10 +3428,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>0</v>
@@ -3445,10 +3445,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>0</v>
@@ -3462,10 +3462,10 @@
     </row>
     <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>272</v>
+        <v>444</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>0</v>
@@ -3488,7 +3488,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A2:XFD43"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4039,7 +4039,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -4056,7 +4056,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -4073,7 +4073,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -4090,7 +4090,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -4107,7 +4107,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -4124,7 +4124,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -4138,10 +4138,10 @@
     </row>
     <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -4155,10 +4155,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
@@ -4172,10 +4172,10 @@
     </row>
     <row r="10" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -4189,10 +4189,10 @@
     </row>
     <row r="11" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
@@ -4206,10 +4206,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -4223,10 +4223,10 @@
     </row>
     <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -4240,10 +4240,10 @@
     </row>
     <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -4260,7 +4260,7 @@
         <v>81</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>0</v>
@@ -4277,7 +4277,7 @@
         <v>82</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
@@ -4294,7 +4294,7 @@
         <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
@@ -4311,7 +4311,7 @@
         <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>0</v>
@@ -4328,7 +4328,7 @@
         <v>85</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -4345,7 +4345,7 @@
         <v>144</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>0</v>
@@ -4362,7 +4362,7 @@
         <v>145</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -4379,7 +4379,7 @@
         <v>146</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -4396,7 +4396,7 @@
         <v>147</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
@@ -4413,7 +4413,7 @@
         <v>148</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -4444,10 +4444,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -4461,10 +4461,10 @@
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -4485,7 +4485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
@@ -4806,10 +4806,10 @@
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -5098,7 +5098,7 @@
         <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -5115,7 +5115,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -5197,10 +5197,10 @@
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -5248,10 +5248,10 @@
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -5265,10 +5265,10 @@
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -5282,10 +5282,10 @@
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -5299,10 +5299,10 @@
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -5316,10 +5316,10 @@
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -5333,10 +5333,10 @@
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -5350,10 +5350,10 @@
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -5384,10 +5384,10 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -5401,10 +5401,10 @@
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -5571,10 +5571,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>48</v>
@@ -5605,10 +5605,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -5622,10 +5622,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -5639,10 +5639,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -6215,7 +6215,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -6224,7 +6224,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6232,7 +6232,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -6241,7 +6241,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -6249,7 +6249,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -6258,7 +6258,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6266,7 +6266,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -6275,7 +6275,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6283,7 +6283,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -6292,7 +6292,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
@@ -6300,7 +6300,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -6309,16 +6309,16 @@
         <v>0</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -6327,7 +6327,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6335,7 +6335,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -6344,7 +6344,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
@@ -6352,7 +6352,7 @@
         <v>82</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -6361,7 +6361,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6369,7 +6369,7 @@
         <v>83</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
@@ -6378,7 +6378,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
@@ -6386,7 +6386,7 @@
         <v>84</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -6395,7 +6395,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6403,7 +6403,7 @@
         <v>85</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -6412,7 +6412,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6420,7 +6420,7 @@
         <v>86</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -6429,7 +6429,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6437,7 +6437,7 @@
         <v>87</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -6446,7 +6446,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6454,7 +6454,7 @@
         <v>144</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>0</v>
@@ -6463,7 +6463,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6471,7 +6471,7 @@
         <v>145</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
@@ -6480,7 +6480,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -6488,7 +6488,7 @@
         <v>146</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>0</v>
@@ -6497,7 +6497,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="39.299999999999997" x14ac:dyDescent="0.55000000000000004">
@@ -6505,7 +6505,7 @@
         <v>147</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -6514,7 +6514,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6522,7 +6522,7 @@
         <v>148</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>0</v>
@@ -6531,7 +6531,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6539,7 +6539,7 @@
         <v>149</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -6548,15 +6548,15 @@
         <v>0</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -6565,15 +6565,15 @@
         <v>0</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
@@ -6582,7 +6582,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6590,7 +6590,7 @@
         <v>156</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>0</v>
@@ -6599,7 +6599,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6607,7 +6607,7 @@
         <v>157</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -6616,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6624,7 +6624,7 @@
         <v>158</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -6633,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6641,7 +6641,7 @@
         <v>159</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -6650,7 +6650,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
@@ -6658,7 +6658,7 @@
         <v>160</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>0</v>
@@ -6667,15 +6667,15 @@
         <v>0</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
@@ -6684,15 +6684,15 @@
         <v>0</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>0</v>
@@ -6701,15 +6701,15 @@
         <v>0</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>0</v>
@@ -6718,15 +6718,15 @@
         <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>0</v>
@@ -6735,15 +6735,15 @@
         <v>0</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>0</v>
@@ -6752,15 +6752,15 @@
         <v>0</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
@@ -6769,15 +6769,15 @@
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
@@ -6786,15 +6786,15 @@
         <v>0</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -6803,15 +6803,15 @@
         <v>0</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -6820,15 +6820,15 @@
         <v>0</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -6837,15 +6837,15 @@
         <v>0</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>0</v>
@@ -6854,15 +6854,15 @@
         <v>0</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
@@ -6871,15 +6871,15 @@
         <v>0</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
@@ -6888,15 +6888,15 @@
         <v>0</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -6905,15 +6905,15 @@
         <v>0</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
@@ -6922,15 +6922,15 @@
         <v>0</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="49.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
@@ -6939,15 +6939,15 @@
         <v>0</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>0</v>
@@ -6956,15 +6956,15 @@
         <v>0</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -6973,15 +6973,15 @@
         <v>0</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -6990,15 +6990,15 @@
         <v>0</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -7007,15 +7007,15 @@
         <v>0</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="50.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -7024,15 +7024,15 @@
         <v>0</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -7041,15 +7041,15 @@
         <v>0</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -7058,15 +7058,15 @@
         <v>0</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -7075,7 +7075,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update grammatical errors in scenarios
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -670,9 +670,6 @@
     <t xml:space="preserve">Due to drunken state male isn’t able to provide full information and no arrests can be made </t>
   </si>
   <si>
-    <t>Drunk male becomes aggressive with officers which results in him being arrested disorderly however still wanting to report assault once sober in the morning</t>
-  </si>
-  <si>
     <t xml:space="preserve">Information allows officers to identify a suspect and make an arrest </t>
   </si>
   <si>
@@ -1594,6 +1591,9 @@
   </si>
   <si>
     <t>Information reveals that shoplifter has never been in trouble previously and was issued a fixed penalty for the theft. Report concluded</t>
+  </si>
+  <si>
+    <t>Drunk male becomes aggressive with officers which results in him being arrested, however he still wants to report assault once sober in the morning</t>
   </si>
 </sst>
 </file>
@@ -2001,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2479,7 +2479,7 @@
         <v>156</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>0</v>
@@ -2649,7 +2649,7 @@
         <v>170</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -2955,7 +2955,7 @@
         <v>202</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>213</v>
+        <v>444</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -2972,7 +2972,7 @@
         <v>203</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
@@ -3003,10 +3003,10 @@
     </row>
     <row r="59" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>0</v>
@@ -3020,10 +3020,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>0</v>
@@ -3037,10 +3037,10 @@
     </row>
     <row r="61" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>0</v>
@@ -3054,10 +3054,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>0</v>
@@ -3071,10 +3071,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="64" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -3105,10 +3105,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>0</v>
@@ -3122,10 +3122,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -3139,10 +3139,10 @@
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>0</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -3173,10 +3173,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
@@ -3190,10 +3190,10 @@
     </row>
     <row r="70" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>0</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>0</v>
@@ -3224,10 +3224,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>0</v>
@@ -3241,10 +3241,10 @@
     </row>
     <row r="73" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>0</v>
@@ -3258,10 +3258,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>0</v>
@@ -3275,10 +3275,10 @@
     </row>
     <row r="75" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>0</v>
@@ -3292,10 +3292,10 @@
     </row>
     <row r="76" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>0</v>
@@ -3309,10 +3309,10 @@
     </row>
     <row r="77" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>0</v>
@@ -3326,10 +3326,10 @@
     </row>
     <row r="78" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>0</v>
@@ -3343,10 +3343,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>0</v>
@@ -3360,10 +3360,10 @@
     </row>
     <row r="80" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>0</v>
@@ -3377,10 +3377,10 @@
     </row>
     <row r="81" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>0</v>
@@ -3394,10 +3394,10 @@
     </row>
     <row r="82" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>0</v>
@@ -3411,10 +3411,10 @@
     </row>
     <row r="83" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>0</v>
@@ -3428,10 +3428,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>0</v>
@@ -3445,10 +3445,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>0</v>
@@ -3462,10 +3462,10 @@
     </row>
     <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>0</v>
@@ -4039,7 +4039,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -4056,7 +4056,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -4073,7 +4073,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -4090,7 +4090,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -4107,7 +4107,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -4124,7 +4124,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -4138,10 +4138,10 @@
     </row>
     <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -4155,10 +4155,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
@@ -4172,10 +4172,10 @@
     </row>
     <row r="10" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -4189,10 +4189,10 @@
     </row>
     <row r="11" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
@@ -4206,10 +4206,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -4223,10 +4223,10 @@
     </row>
     <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -4240,10 +4240,10 @@
     </row>
     <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -4260,7 +4260,7 @@
         <v>81</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>0</v>
@@ -4277,7 +4277,7 @@
         <v>82</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
@@ -4294,7 +4294,7 @@
         <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
@@ -4311,7 +4311,7 @@
         <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>0</v>
@@ -4328,7 +4328,7 @@
         <v>85</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -4345,7 +4345,7 @@
         <v>144</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>0</v>
@@ -4362,7 +4362,7 @@
         <v>145</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -4379,7 +4379,7 @@
         <v>146</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -4396,7 +4396,7 @@
         <v>147</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
@@ -4413,7 +4413,7 @@
         <v>148</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -4444,10 +4444,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -4461,10 +4461,10 @@
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -4806,10 +4806,10 @@
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -5098,7 +5098,7 @@
         <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -5115,7 +5115,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -5197,10 +5197,10 @@
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>407</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -5248,10 +5248,10 @@
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -5265,10 +5265,10 @@
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -5282,10 +5282,10 @@
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -5299,10 +5299,10 @@
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -5316,10 +5316,10 @@
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>423</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -5333,10 +5333,10 @@
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>425</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -5350,10 +5350,10 @@
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>427</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -5384,10 +5384,10 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -5401,10 +5401,10 @@
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>429</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -5571,10 +5571,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>0</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>48</v>
@@ -5605,10 +5605,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -5622,10 +5622,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -5639,10 +5639,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -6215,7 +6215,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -6224,7 +6224,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6232,7 +6232,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -6241,7 +6241,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -6249,7 +6249,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -6258,7 +6258,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6266,7 +6266,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -6275,7 +6275,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6283,7 +6283,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -6292,7 +6292,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
@@ -6300,7 +6300,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -6309,16 +6309,16 @@
         <v>0</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -6327,7 +6327,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6335,7 +6335,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -6344,7 +6344,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
@@ -6352,7 +6352,7 @@
         <v>82</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -6361,7 +6361,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6369,7 +6369,7 @@
         <v>83</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
@@ -6378,7 +6378,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
@@ -6386,7 +6386,7 @@
         <v>84</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -6395,7 +6395,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6403,7 +6403,7 @@
         <v>85</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -6412,7 +6412,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6420,7 +6420,7 @@
         <v>86</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -6429,7 +6429,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6437,7 +6437,7 @@
         <v>87</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -6446,7 +6446,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6454,7 +6454,7 @@
         <v>144</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>0</v>
@@ -6463,7 +6463,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6471,7 +6471,7 @@
         <v>145</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
@@ -6480,7 +6480,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -6488,7 +6488,7 @@
         <v>146</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>0</v>
@@ -6497,7 +6497,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="39.299999999999997" x14ac:dyDescent="0.55000000000000004">
@@ -6505,7 +6505,7 @@
         <v>147</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -6514,7 +6514,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6522,7 +6522,7 @@
         <v>148</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>0</v>
@@ -6531,7 +6531,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6539,7 +6539,7 @@
         <v>149</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -6548,15 +6548,15 @@
         <v>0</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -6565,15 +6565,15 @@
         <v>0</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
@@ -6582,7 +6582,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6590,7 +6590,7 @@
         <v>156</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>0</v>
@@ -6599,7 +6599,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6607,7 +6607,7 @@
         <v>157</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -6616,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6624,7 +6624,7 @@
         <v>158</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -6633,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6641,7 +6641,7 @@
         <v>159</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -6650,7 +6650,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
@@ -6658,7 +6658,7 @@
         <v>160</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>0</v>
@@ -6667,15 +6667,15 @@
         <v>0</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
@@ -6684,15 +6684,15 @@
         <v>0</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>0</v>
@@ -6701,7 +6701,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6709,7 +6709,7 @@
         <v>165</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>0</v>
@@ -6718,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -6726,7 +6726,7 @@
         <v>166</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>0</v>
@@ -6735,7 +6735,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -6743,7 +6743,7 @@
         <v>167</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>0</v>
@@ -6752,7 +6752,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -6760,7 +6760,7 @@
         <v>168</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
@@ -6769,7 +6769,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6777,7 +6777,7 @@
         <v>169</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
@@ -6786,7 +6786,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
@@ -6794,7 +6794,7 @@
         <v>170</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -6803,7 +6803,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6811,7 +6811,7 @@
         <v>171</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -6820,15 +6820,15 @@
         <v>0</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -6837,7 +6837,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
@@ -6845,7 +6845,7 @@
         <v>178</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>0</v>
@@ -6854,7 +6854,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6862,7 +6862,7 @@
         <v>180</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
@@ -6871,7 +6871,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -6879,7 +6879,7 @@
         <v>181</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
@@ -6888,7 +6888,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6896,7 +6896,7 @@
         <v>179</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -6905,7 +6905,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6913,7 +6913,7 @@
         <v>182</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
@@ -6922,7 +6922,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="49.2" x14ac:dyDescent="0.55000000000000004">
@@ -6930,7 +6930,7 @@
         <v>183</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
@@ -6939,7 +6939,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
@@ -6947,7 +6947,7 @@
         <v>194</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>0</v>
@@ -6956,7 +6956,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -6964,7 +6964,7 @@
         <v>195</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -6973,7 +6973,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
@@ -6981,7 +6981,7 @@
         <v>196</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -6990,7 +6990,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -6998,7 +6998,7 @@
         <v>197</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -7007,7 +7007,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="50.7" x14ac:dyDescent="0.55000000000000004">
@@ -7015,7 +7015,7 @@
         <v>198</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -7024,7 +7024,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -7032,7 +7032,7 @@
         <v>199</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -7041,7 +7041,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -7049,7 +7049,7 @@
         <v>200</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -7058,7 +7058,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -7066,7 +7066,7 @@
         <v>201</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -7075,7 +7075,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tips for when the citizen button is not pressed
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="455">
   <si>
     <t>XXXX</t>
   </si>
@@ -1594,6 +1594,36 @@
   </si>
   <si>
     <t>Drunk male becomes aggressive with officers which results in him being arrested, however he still wants to report assault once sober in the morning</t>
+  </si>
+  <si>
+    <t>TIPS_CITIZEN_1</t>
+  </si>
+  <si>
+    <t>TIPS_CITIZEN_2</t>
+  </si>
+  <si>
+    <t>TIPS_CITIZEN_3</t>
+  </si>
+  <si>
+    <t>TIPS_CITIZEN_4</t>
+  </si>
+  <si>
+    <t>TIPS_CITIZEN_5</t>
+  </si>
+  <si>
+    <t>TIP:*n*You can save resources by asking citizens for more information!</t>
+  </si>
+  <si>
+    <t>TIP:*n*Citizens using the INSPEC2T app can help to identify key suspects</t>
+  </si>
+  <si>
+    <t>TIP:*n*Citizens may be able to help with cases with information or evidence, make the most of the option</t>
+  </si>
+  <si>
+    <t>TIP:*n*Maybe next time ask citizens for information, it could cut down the required officers</t>
+  </si>
+  <si>
+    <t>TIP:*n*Maybe next time ask for citizen help from the INSPEC2T app, it could reduce the number of turns required</t>
   </si>
 </sst>
 </file>
@@ -2001,7 +2031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -4483,10 +4513,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5651,6 +5681,91 @@
         <v>0</v>
       </c>
       <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add tips when interacting with the app
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="473">
   <si>
     <t>XXXX</t>
   </si>
@@ -1611,19 +1611,73 @@
     <t>TIPS_CITIZEN_5</t>
   </si>
   <si>
-    <t>TIP:*n*You can save resources by asking citizens for more information!</t>
-  </si>
-  <si>
-    <t>TIP:*n*Citizens using the INSPEC2T app can help to identify key suspects</t>
-  </si>
-  <si>
-    <t>TIP:*n*Citizens may be able to help with cases with information or evidence, make the most of the option</t>
-  </si>
-  <si>
-    <t>TIP:*n*Maybe next time ask citizens for information, it could cut down the required officers</t>
-  </si>
-  <si>
-    <t>TIP:*n*Maybe next time ask for citizen help from the INSPEC2T app, it could reduce the number of turns required</t>
+    <t>TIPS_WAIT_1</t>
+  </si>
+  <si>
+    <t>Ignoring a case will lower satisfaction at the end of the turn, try to close as many cases as possible</t>
+  </si>
+  <si>
+    <t>TIPS_WAIT_2</t>
+  </si>
+  <si>
+    <t>Sometimes it is better to save officers for a more severe case</t>
+  </si>
+  <si>
+    <t>TIPS_WAIT_3</t>
+  </si>
+  <si>
+    <t>TIPS_WAIT_4</t>
+  </si>
+  <si>
+    <t>TIPS_WAIT_5</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER_1</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER_2</t>
+  </si>
+  <si>
+    <t>Remember to keep an eye on upcoming incidents to keep officers for potentially more severe incidents</t>
+  </si>
+  <si>
+    <t>Ignoring incidents is more likely to give negative resolutions for incidents, try not to ignore cases</t>
+  </si>
+  <si>
+    <t>Some incidents will develop less than others, remember to evaluate the information provided carefully</t>
+  </si>
+  <si>
+    <t>Sending officers will always lead to a positive resolution, but at the cost of resources, make decisions carefully</t>
+  </si>
+  <si>
+    <t>Be Careful, sometimes ignoring incidents will cause them to develop.</t>
+  </si>
+  <si>
+    <t>Maybe next time ask for citizen help from the INSPEC2T app, it could reduce the number of turns required</t>
+  </si>
+  <si>
+    <t>Maybe next time ask citizens for information, it could cut down the required officers</t>
+  </si>
+  <si>
+    <t>Citizens may be able to help with cases with information or evidence, make the most of the option</t>
+  </si>
+  <si>
+    <t>Citizens using the INSPEC2T app can help to identify key suspects</t>
+  </si>
+  <si>
+    <t>You can save resources by asking citizens for more information!</t>
+  </si>
+  <si>
+    <t>Great Job!</t>
+  </si>
+  <si>
+    <t>Remember thet officers sent to incidents requiring just 1 turn will return at the start of the next turn</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER_POSITIVE_1</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER_NEGATIVE_1</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1749,6 +1803,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4513,10 +4568,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5689,7 +5744,7 @@
         <v>445</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
@@ -5706,7 +5761,7 @@
         <v>446</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>451</v>
+        <v>467</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>0</v>
@@ -5723,7 +5778,7 @@
         <v>447</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>0</v>
@@ -5740,7 +5795,7 @@
         <v>448</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>0</v>
@@ -5757,18 +5812,173 @@
         <v>449</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="B76" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="84" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add more tips to the game bases on player decisions
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="487">
   <si>
     <t>XXXX</t>
   </si>
@@ -1674,10 +1674,52 @@
     <t>Remember thet officers sent to incidents requiring just 1 turn will return at the start of the next turn</t>
   </si>
   <si>
-    <t>TIPS_OFFICER_POSITIVE_1</t>
-  </si>
-  <si>
-    <t>TIPS_OFFICER_NEGATIVE_1</t>
+    <t>TIPS_OFFICER_ONE_TURN_NEGATIVE_1</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER_HIGH_SEVERITY_NEGATIVE_1</t>
+  </si>
+  <si>
+    <t>Well Done!</t>
+  </si>
+  <si>
+    <t>Ignoring high severity cases will have a large impact on satisfaction.</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER_HIGH_SEVERITY_NEGATIVE_2</t>
+  </si>
+  <si>
+    <t>Make sure to give high severity cases priority, failing to resolve will give a big satisfaction penalty!</t>
+  </si>
+  <si>
+    <t>Awesome!</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER_ONE_TURN_NEGATIVE_2</t>
+  </si>
+  <si>
+    <t>Good Choice!</t>
+  </si>
+  <si>
+    <t>Sending officers to incidents that only require 1 turn is a great way to clear active cases</t>
+  </si>
+  <si>
+    <t>TIPS_POSITIVE_1</t>
+  </si>
+  <si>
+    <t>TIPS_POSITIVE_2</t>
+  </si>
+  <si>
+    <t>TIPS_POSITIVE_3</t>
+  </si>
+  <si>
+    <t>TIPS_POSITIVE_4</t>
+  </si>
+  <si>
+    <t>TIPS_POSITIVE_5</t>
+  </si>
+  <si>
+    <t>Nice!</t>
   </si>
 </sst>
 </file>
@@ -4568,10 +4610,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5943,42 +5985,164 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>471</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="84" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+      <c r="C87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
make text larger where possible Generate more incidents per turn Remove time out on incidents as it does not work with current setup add tap to continue to tips to automatically continue without needing to wait the alotted time
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="489">
   <si>
     <t>XXXX</t>
   </si>
@@ -1572,15 +1572,9 @@
     <t>BASIC_TEXT_SATISFACTION_END_TURN</t>
   </si>
   <si>
-    <t>{0} Ignored Case{1}, -{2}% Satisfaction</t>
-  </si>
-  <si>
     <t>BASIC_TEXT_NO_IGNORED_CASES</t>
   </si>
   <si>
-    <t>0 Ignored Cases, No Satisfaction Change</t>
-  </si>
-  <si>
     <t>Report of a vehicle being parked in an inconsiderate manner on a residential street.</t>
   </si>
   <si>
@@ -1720,6 +1714,18 @@
   </si>
   <si>
     <t>Nice!</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_IGNORE</t>
+  </si>
+  <si>
+    <t>Ignore!</t>
+  </si>
+  <si>
+    <t>0 Ignored Cases*2n*No Satisfaction Change</t>
+  </si>
+  <si>
+    <t>{0} Ignored Case{1}*2n*-{2}% Satisfaction</t>
   </si>
 </sst>
 </file>
@@ -2606,7 +2612,7 @@
         <v>156</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>0</v>
@@ -2776,7 +2782,7 @@
         <v>170</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -3082,7 +3088,7 @@
         <v>202</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -3388,7 +3394,7 @@
         <v>243</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>0</v>
@@ -3592,7 +3598,7 @@
         <v>263</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>0</v>
@@ -4610,10 +4616,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4729,27 +4735,27 @@
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -4763,10 +4769,10 @@
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
@@ -4780,10 +4786,10 @@
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -4797,10 +4803,10 @@
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
@@ -4814,10 +4820,10 @@
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -4831,10 +4837,10 @@
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -4848,10 +4854,10 @@
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -4865,10 +4871,10 @@
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -4882,10 +4888,10 @@
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
@@ -4899,10 +4905,10 @@
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>140</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
@@ -4916,10 +4922,10 @@
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>0</v>
@@ -4933,10 +4939,10 @@
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>419</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>420</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -4950,10 +4956,10 @@
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>419</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>420</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>0</v>
@@ -4967,10 +4973,10 @@
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -4984,10 +4990,10 @@
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -5001,10 +5007,10 @@
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
@@ -5018,10 +5024,10 @@
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
@@ -5035,10 +5041,10 @@
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -5052,10 +5058,10 @@
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -5069,10 +5075,10 @@
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -5086,10 +5092,10 @@
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>0</v>
@@ -5103,44 +5109,44 @@
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>0</v>
@@ -5154,10 +5160,10 @@
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>0</v>
@@ -5171,10 +5177,10 @@
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>0</v>
@@ -5188,10 +5194,10 @@
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
@@ -5205,10 +5211,10 @@
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
@@ -5222,10 +5228,10 @@
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>407</v>
+        <v>118</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
@@ -5239,10 +5245,10 @@
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -5256,10 +5262,10 @@
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>408</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -5273,10 +5279,10 @@
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>0</v>
@@ -5290,10 +5296,10 @@
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
@@ -5307,10 +5313,10 @@
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
@@ -5324,10 +5330,10 @@
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>405</v>
+        <v>109</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>406</v>
+        <v>110</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -5341,44 +5347,44 @@
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -5392,10 +5398,10 @@
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
@@ -5409,10 +5415,10 @@
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
@@ -5426,10 +5432,10 @@
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
@@ -5443,10 +5449,10 @@
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
@@ -5460,10 +5466,10 @@
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
@@ -5477,10 +5483,10 @@
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
@@ -5494,10 +5500,10 @@
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>142</v>
+        <v>425</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>143</v>
+        <v>426</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
@@ -5511,10 +5517,10 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>417</v>
+        <v>142</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>418</v>
+        <v>143</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
@@ -5528,10 +5534,10 @@
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
@@ -5545,27 +5551,27 @@
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -5579,10 +5585,10 @@
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
@@ -5596,10 +5602,10 @@
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>0</v>
@@ -5613,44 +5619,44 @@
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>0</v>
@@ -5664,27 +5670,27 @@
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>0</v>
@@ -5698,44 +5704,44 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="s">
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
         <v>433</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>435</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>0</v>
@@ -5749,10 +5755,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
@@ -5766,10 +5772,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>439</v>
+        <v>488</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
@@ -5783,10 +5789,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>468</v>
+        <v>487</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
@@ -5800,10 +5806,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>0</v>
@@ -5815,12 +5821,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>0</v>
@@ -5834,10 +5840,10 @@
     </row>
     <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>0</v>
@@ -5851,10 +5857,10 @@
     </row>
     <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>0</v>
@@ -5868,44 +5874,44 @@
     </row>
     <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>0</v>
@@ -5919,44 +5925,44 @@
     </row>
     <row r="77" spans="1:5" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="12" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="12" t="s">
-        <v>456</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>0</v>
@@ -5970,10 +5976,10 @@
     </row>
     <row r="80" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>0</v>
@@ -5987,10 +5993,10 @@
     </row>
     <row r="81" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>0</v>
@@ -6004,62 +6010,62 @@
     </row>
     <row r="82" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="1" t="s">
+      <c r="C83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>473</v>
-      </c>
       <c r="C85" s="1" t="s">
         <v>0</v>
       </c>
@@ -6069,14 +6075,13 @@
       <c r="E85" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>0</v>
@@ -6091,10 +6096,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>0</v>
@@ -6109,10 +6114,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>0</v>
@@ -6127,10 +6132,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>0</v>
@@ -6142,6 +6147,24 @@
         <v>0</v>
       </c>
       <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F90" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refine alternate language screen and appropriate text
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="495">
   <si>
     <t>XXXX</t>
   </si>
@@ -1727,12 +1727,30 @@
   <si>
     <t>{0} Ignored Case{1}*2n*-{2}% Satisfaction</t>
   </si>
+  <si>
+    <t>BASIC_TEXT_SELECT_LANGUAGE</t>
+  </si>
+  <si>
+    <t>Multiple Scenario Languages available. Select a language</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_ENGLISH</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SPANISH</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1777,6 +1795,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri   "/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1816,7 +1839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1852,6 +1875,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2138,7 +2164,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
@@ -2148,7 +2174,7 @@
     <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2165,7 +2191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
@@ -2182,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -2199,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -2216,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -2233,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -2250,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -2267,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
@@ -2284,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
@@ -2301,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -2318,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -2335,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="25.5">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -2352,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -2369,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>87</v>
       </c>
@@ -2386,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="25.5">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -2403,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -2420,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="25.5">
       <c r="A17" s="1" t="s">
         <v>90</v>
       </c>
@@ -2437,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" ht="25.5">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
@@ -2454,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>92</v>
       </c>
@@ -2471,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>93</v>
       </c>
@@ -2488,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>94</v>
       </c>
@@ -2505,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A22" s="3" t="s">
         <v>144</v>
       </c>
@@ -2522,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="25.5">
       <c r="A23" s="1" t="s">
         <v>145</v>
       </c>
@@ -2539,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>146</v>
       </c>
@@ -2556,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" ht="25.5">
       <c r="A25" s="1" t="s">
         <v>147</v>
       </c>
@@ -2573,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" ht="25.5">
       <c r="A26" s="1" t="s">
         <v>148</v>
       </c>
@@ -2590,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>149</v>
       </c>
@@ -2607,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A28" s="3" t="s">
         <v>156</v>
       </c>
@@ -2624,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="1" t="s">
         <v>157</v>
       </c>
@@ -2641,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" ht="25.5">
       <c r="A30" s="1" t="s">
         <v>158</v>
       </c>
@@ -2658,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>159</v>
       </c>
@@ -2675,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" ht="37.799999999999997">
       <c r="A32" s="1" t="s">
         <v>160</v>
       </c>
@@ -2692,7 +2718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A33" s="3" t="s">
         <v>165</v>
       </c>
@@ -2709,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" ht="25.5">
       <c r="A34" s="1" t="s">
         <v>166</v>
       </c>
@@ -2726,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" ht="25.5">
       <c r="A35" s="1" t="s">
         <v>167</v>
       </c>
@@ -2743,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" ht="25.5">
       <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
@@ -2760,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" ht="25.5">
       <c r="A37" s="1" t="s">
         <v>169</v>
       </c>
@@ -2777,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="1" t="s">
         <v>170</v>
       </c>
@@ -2794,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>171</v>
       </c>
@@ -2811,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" s="3" customFormat="1">
       <c r="A40" s="3" t="s">
         <v>178</v>
       </c>
@@ -2828,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="25.5">
       <c r="A41" s="1" t="s">
         <v>179</v>
       </c>
@@ -2845,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>180</v>
       </c>
@@ -2862,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" ht="25.5">
       <c r="A43" s="1" t="s">
         <v>181</v>
       </c>
@@ -2879,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>182</v>
       </c>
@@ -2896,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" ht="25.5">
       <c r="A45" s="1" t="s">
         <v>183</v>
       </c>
@@ -2913,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>184</v>
       </c>
@@ -2930,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" ht="37.799999999999997">
       <c r="A47" s="1" t="s">
         <v>185</v>
       </c>
@@ -2947,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A48" s="3" t="s">
         <v>194</v>
       </c>
@@ -2964,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>195</v>
       </c>
@@ -2981,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
         <v>196</v>
       </c>
@@ -2998,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" ht="25.5">
       <c r="A51" s="1" t="s">
         <v>197</v>
       </c>
@@ -3015,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" ht="25.5">
       <c r="A52" s="1" t="s">
         <v>198</v>
       </c>
@@ -3032,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" ht="25.5">
       <c r="A53" s="1" t="s">
         <v>199</v>
       </c>
@@ -3049,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" ht="25.5">
       <c r="A54" s="1" t="s">
         <v>200</v>
       </c>
@@ -3066,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" ht="25.5">
       <c r="A55" s="1" t="s">
         <v>201</v>
       </c>
@@ -3083,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" ht="25.5">
       <c r="A56" s="1" t="s">
         <v>202</v>
       </c>
@@ -3100,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>203</v>
       </c>
@@ -3117,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>204</v>
       </c>
@@ -3134,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A59" s="3" t="s">
         <v>214</v>
       </c>
@@ -3151,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>215</v>
       </c>
@@ -3168,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" ht="25.5">
       <c r="A61" s="1" t="s">
         <v>216</v>
       </c>
@@ -3185,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>217</v>
       </c>
@@ -3202,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
         <v>218</v>
       </c>
@@ -3219,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5" ht="25.5">
       <c r="A64" s="1" t="s">
         <v>219</v>
       </c>
@@ -3236,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>220</v>
       </c>
@@ -3253,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
         <v>221</v>
       </c>
@@ -3270,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A67" s="3" t="s">
         <v>230</v>
       </c>
@@ -3287,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>231</v>
       </c>
@@ -3304,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>232</v>
       </c>
@@ -3321,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" ht="25.5">
       <c r="A70" s="1" t="s">
         <v>233</v>
       </c>
@@ -3338,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
         <v>234</v>
       </c>
@@ -3355,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
         <v>235</v>
       </c>
@@ -3372,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A73" s="3" t="s">
         <v>242</v>
       </c>
@@ -3389,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
         <v>243</v>
       </c>
@@ -3406,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" ht="25.5">
       <c r="A75" s="1" t="s">
         <v>244</v>
       </c>
@@ -3423,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A76" s="3" t="s">
         <v>247</v>
       </c>
@@ -3440,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" ht="25.5">
       <c r="A77" s="1" t="s">
         <v>248</v>
       </c>
@@ -3457,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" ht="25.5">
       <c r="A78" s="1" t="s">
         <v>249</v>
       </c>
@@ -3474,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
         <v>250</v>
       </c>
@@ -3491,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:5" ht="25.5">
       <c r="A80" s="1" t="s">
         <v>251</v>
       </c>
@@ -3508,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" ht="25.5">
       <c r="A81" s="1" t="s">
         <v>252</v>
       </c>
@@ -3525,7 +3551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:5" s="3" customFormat="1">
       <c r="A82" s="3" t="s">
         <v>259</v>
       </c>
@@ -3542,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:5" ht="25.5">
       <c r="A83" s="1" t="s">
         <v>260</v>
       </c>
@@ -3559,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
         <v>261</v>
       </c>
@@ -3576,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
         <v>262</v>
       </c>
@@ -3593,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:5" ht="25.5">
       <c r="A86" s="1" t="s">
         <v>263</v>
       </c>
@@ -3624,7 +3650,7 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
@@ -3634,7 +3660,7 @@
     <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3651,7 +3677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -3668,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -3685,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -3702,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -3719,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -3736,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -3753,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
@@ -3770,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
@@ -3787,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -3804,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -3821,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="25.5">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -3838,7 +3864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -3855,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>87</v>
       </c>
@@ -3872,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="25.5">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -3889,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -3906,7 +3932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="25.5">
       <c r="A17" s="1" t="s">
         <v>90</v>
       </c>
@@ -3923,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" ht="25.5">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
@@ -3940,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>92</v>
       </c>
@@ -3957,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>93</v>
       </c>
@@ -3974,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>94</v>
       </c>
@@ -3991,7 +4017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>122</v>
       </c>
@@ -4008,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="1" t="s">
         <v>124</v>
       </c>
@@ -4025,7 +4051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" ht="28.8">
       <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
@@ -4042,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" ht="28.8">
       <c r="A25" s="1" t="s">
         <v>128</v>
       </c>
@@ -4059,7 +4085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" ht="28.8">
       <c r="A26" s="1" t="s">
         <v>129</v>
       </c>
@@ -4076,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>135</v>
       </c>
@@ -4093,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" ht="28.8">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -4110,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="28.8">
       <c r="A29" s="1" t="s">
         <v>133</v>
       </c>
@@ -4140,7 +4166,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
@@ -4150,7 +4176,7 @@
     <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4167,7 +4193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
@@ -4184,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -4201,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -4218,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -4235,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="26.1">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -4252,7 +4278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -4269,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="1" t="s">
         <v>274</v>
       </c>
@@ -4286,7 +4312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>275</v>
       </c>
@@ -4303,7 +4329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="37.799999999999997">
       <c r="A10" s="1" t="s">
         <v>276</v>
       </c>
@@ -4320,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="37.799999999999997">
       <c r="A11" s="1" t="s">
         <v>282</v>
       </c>
@@ -4337,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>277</v>
       </c>
@@ -4354,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="25.5">
       <c r="A13" s="1" t="s">
         <v>283</v>
       </c>
@@ -4371,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="25.5">
       <c r="A14" s="1" t="s">
         <v>284</v>
       </c>
@@ -4388,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A15" s="3" t="s">
         <v>81</v>
       </c>
@@ -4405,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -4422,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>83</v>
       </c>
@@ -4439,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" ht="37.799999999999997">
       <c r="A18" s="1" t="s">
         <v>84</v>
       </c>
@@ -4456,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" ht="25.5">
       <c r="A19" s="1" t="s">
         <v>85</v>
       </c>
@@ -4473,7 +4499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A20" s="3" t="s">
         <v>144</v>
       </c>
@@ -4490,7 +4516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" ht="62.4">
       <c r="A21" s="1" t="s">
         <v>145</v>
       </c>
@@ -4507,7 +4533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" ht="25.5">
       <c r="A22" s="1" t="s">
         <v>146</v>
       </c>
@@ -4524,7 +4550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="25.5">
       <c r="A23" s="1" t="s">
         <v>147</v>
       </c>
@@ -4541,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" ht="37.799999999999997">
       <c r="A24" s="1" t="s">
         <v>148</v>
       </c>
@@ -4558,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" ht="25.5">
       <c r="A25" s="1" t="s">
         <v>149</v>
       </c>
@@ -4575,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>293</v>
       </c>
@@ -4592,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" ht="25.5">
       <c r="A27" s="1" t="s">
         <v>294</v>
       </c>
@@ -4616,13 +4642,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49.15625" customWidth="1"/>
     <col min="2" max="2" width="62.9453125" customWidth="1"/>
@@ -4631,7 +4657,7 @@
     <col min="5" max="5" width="48.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4648,7 +4674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="57.6">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -4665,7 +4691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4682,7 +4708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -4699,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -4716,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -4733,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>485</v>
       </c>
@@ -4750,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="14.7" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -4767,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -4784,7 +4810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -4801,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -4818,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -4835,7 +4861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -4852,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -4869,7 +4895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" s="1" customFormat="1">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -4886,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" s="1" customFormat="1">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -4903,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" s="1" customFormat="1">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -4920,7 +4946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" s="1" customFormat="1">
       <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
@@ -4937,7 +4963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" s="1" customFormat="1">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -4954,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" s="1" customFormat="1">
       <c r="A20" s="1" t="s">
         <v>419</v>
       </c>
@@ -4971,7 +4997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" s="1" customFormat="1">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -4988,7 +5014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -5005,7 +5031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" s="1" customFormat="1">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -5022,7 +5048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" s="1" customFormat="1">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -5039,7 +5065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -5056,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -5073,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -5090,7 +5116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -5107,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" s="1" customFormat="1">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -5124,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" s="1" customFormat="1">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
@@ -5141,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -5158,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" s="1" customFormat="1">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -5175,7 +5201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" s="1" customFormat="1">
       <c r="A33" s="1" t="s">
         <v>47</v>
       </c>
@@ -5192,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -5209,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -5226,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" s="1" customFormat="1">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
@@ -5243,7 +5269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
@@ -5260,7 +5286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" s="1" customFormat="1">
       <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
@@ -5277,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" s="1" customFormat="1">
       <c r="A39" s="1" t="s">
         <v>68</v>
       </c>
@@ -5294,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" s="1" customFormat="1">
       <c r="A40" s="1" t="s">
         <v>113</v>
       </c>
@@ -5311,7 +5337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" s="1" customFormat="1">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
@@ -5328,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" s="1" customFormat="1">
       <c r="A42" s="1" t="s">
         <v>109</v>
       </c>
@@ -5345,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" s="1" customFormat="1">
       <c r="A43" s="1" t="s">
         <v>405</v>
       </c>
@@ -5362,7 +5388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" s="1" customFormat="1">
       <c r="A44" s="1" t="s">
         <v>112</v>
       </c>
@@ -5379,7 +5405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A45" s="1" t="s">
         <v>138</v>
       </c>
@@ -5396,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" s="1" customFormat="1">
       <c r="A46" s="1" t="s">
         <v>409</v>
       </c>
@@ -5413,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" s="1" customFormat="1">
       <c r="A47" s="1" t="s">
         <v>411</v>
       </c>
@@ -5430,7 +5456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" s="1" customFormat="1">
       <c r="A48" s="1" t="s">
         <v>412</v>
       </c>
@@ -5447,7 +5473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" s="1" customFormat="1">
       <c r="A49" s="1" t="s">
         <v>413</v>
       </c>
@@ -5464,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" s="1" customFormat="1">
       <c r="A50" s="1" t="s">
         <v>421</v>
       </c>
@@ -5481,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" s="1" customFormat="1">
       <c r="A51" s="1" t="s">
         <v>423</v>
       </c>
@@ -5498,7 +5524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" s="1" customFormat="1">
       <c r="A52" s="1" t="s">
         <v>425</v>
       </c>
@@ -5515,7 +5541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" s="1" customFormat="1">
       <c r="A53" s="1" t="s">
         <v>142</v>
       </c>
@@ -5532,7 +5558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" s="1" customFormat="1">
       <c r="A54" s="1" t="s">
         <v>417</v>
       </c>
@@ -5549,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" s="1" customFormat="1">
       <c r="A55" s="1" t="s">
         <v>427</v>
       </c>
@@ -5566,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" s="1" customFormat="1">
       <c r="A56" s="1" t="s">
         <v>122</v>
       </c>
@@ -5583,7 +5609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A57" s="1" t="s">
         <v>124</v>
       </c>
@@ -5600,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A58" s="1" t="s">
         <v>126</v>
       </c>
@@ -5617,7 +5643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A59" s="1" t="s">
         <v>128</v>
       </c>
@@ -5634,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A60" s="1" t="s">
         <v>129</v>
       </c>
@@ -5651,7 +5677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" s="1" customFormat="1">
       <c r="A61" s="1" t="s">
         <v>135</v>
       </c>
@@ -5668,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A62" s="1" t="s">
         <v>131</v>
       </c>
@@ -5685,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A63" s="1" t="s">
         <v>133</v>
       </c>
@@ -5702,7 +5728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
         <v>429</v>
       </c>
@@ -5719,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>430</v>
       </c>
@@ -5736,7 +5762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>433</v>
       </c>
@@ -5753,7 +5779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
         <v>434</v>
       </c>
@@ -5770,7 +5796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>436</v>
       </c>
@@ -5787,7 +5813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>437</v>
       </c>
@@ -5804,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
         <v>443</v>
       </c>
@@ -5821,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
         <v>444</v>
       </c>
@@ -5838,7 +5864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:5" ht="28.8">
       <c r="A72" s="1" t="s">
         <v>445</v>
       </c>
@@ -5855,7 +5881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" ht="28.8">
       <c r="A73" s="1" t="s">
         <v>446</v>
       </c>
@@ -5872,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" ht="28.8">
       <c r="A74" s="1" t="s">
         <v>447</v>
       </c>
@@ -5889,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" ht="28.8">
       <c r="A75" s="1" t="s">
         <v>448</v>
       </c>
@@ -5906,7 +5932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
         <v>450</v>
       </c>
@@ -5923,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A77" s="12" t="s">
         <v>452</v>
       </c>
@@ -5940,7 +5966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A78" s="12" t="s">
         <v>453</v>
       </c>
@@ -5957,7 +5983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:5" s="12" customFormat="1">
       <c r="A79" s="12" t="s">
         <v>454</v>
       </c>
@@ -5974,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:5" s="1" customFormat="1" ht="28.8">
       <c r="A80" s="1" t="s">
         <v>455</v>
       </c>
@@ -5991,7 +6017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:6" s="1" customFormat="1" ht="28.8">
       <c r="A81" s="1" t="s">
         <v>456</v>
       </c>
@@ -6008,7 +6034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:6" s="1" customFormat="1" ht="28.8">
       <c r="A82" s="1" t="s">
         <v>469</v>
       </c>
@@ -6025,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:6" s="1" customFormat="1" ht="28.8">
       <c r="A83" s="1" t="s">
         <v>476</v>
       </c>
@@ -6042,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:6" s="1" customFormat="1">
       <c r="A84" s="1" t="s">
         <v>470</v>
       </c>
@@ -6059,7 +6085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:6" s="1" customFormat="1" ht="28.8">
       <c r="A85" s="1" t="s">
         <v>473</v>
       </c>
@@ -6076,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
         <v>479</v>
       </c>
@@ -6094,7 +6120,7 @@
       </c>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>480</v>
       </c>
@@ -6112,7 +6138,7 @@
       </c>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
         <v>481</v>
       </c>
@@ -6130,7 +6156,7 @@
       </c>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
         <v>482</v>
       </c>
@@ -6148,7 +6174,7 @@
       </c>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
         <v>483</v>
       </c>
@@ -6166,8 +6192,60 @@
       </c>
       <c r="F90" s="1"/>
     </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>489</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6179,7 +6257,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
@@ -6189,7 +6267,7 @@
     <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6206,7 +6284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -6223,7 +6301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -6240,7 +6318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -6257,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -6274,7 +6352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -6291,7 +6369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -6308,7 +6386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
@@ -6325,7 +6403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
@@ -6342,7 +6420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -6359,7 +6437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -6376,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="25.5">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -6393,7 +6471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -6410,7 +6488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>87</v>
       </c>
@@ -6427,7 +6505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="25.5">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -6444,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -6461,7 +6539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="25.5">
       <c r="A17" s="1" t="s">
         <v>90</v>
       </c>
@@ -6478,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" ht="25.5">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
@@ -6495,7 +6573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>92</v>
       </c>
@@ -6512,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>93</v>
       </c>
@@ -6529,7 +6607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>94</v>
       </c>
@@ -6546,7 +6624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>122</v>
       </c>
@@ -6563,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="1" t="s">
         <v>124</v>
       </c>
@@ -6580,7 +6658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" ht="28.8">
       <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
@@ -6597,7 +6675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" ht="28.8">
       <c r="A25" s="1" t="s">
         <v>128</v>
       </c>
@@ -6614,7 +6692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" ht="28.8">
       <c r="A26" s="1" t="s">
         <v>129</v>
       </c>
@@ -6631,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>135</v>
       </c>
@@ -6648,7 +6726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" ht="28.8">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -6665,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="28.8">
       <c r="A29" s="1" t="s">
         <v>133</v>
       </c>
@@ -6695,7 +6773,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49.15625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62.9453125" style="1" customWidth="1"/>
@@ -6705,7 +6783,7 @@
     <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6722,7 +6800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
@@ -6739,7 +6817,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -6756,7 +6834,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" ht="27">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -6773,7 +6851,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -6790,7 +6868,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -6807,7 +6885,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" ht="24.6">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -6825,7 +6903,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" ht="25.5">
       <c r="A8" s="1" t="s">
         <v>274</v>
       </c>
@@ -6842,7 +6920,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>81</v>
       </c>
@@ -6859,7 +6937,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" ht="24.6">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -6876,7 +6954,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" ht="25.5">
       <c r="A11" s="1" t="s">
         <v>83</v>
       </c>
@@ -6893,7 +6971,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" ht="24.6">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -6910,7 +6988,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" ht="25.5">
       <c r="A13" s="1" t="s">
         <v>85</v>
       </c>
@@ -6927,7 +7005,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" ht="25.5">
       <c r="A14" s="1" t="s">
         <v>86</v>
       </c>
@@ -6944,7 +7022,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" ht="25.5">
       <c r="A15" s="1" t="s">
         <v>87</v>
       </c>
@@ -6961,7 +7039,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" s="3" customFormat="1" ht="25.5">
       <c r="A16" s="3" t="s">
         <v>144</v>
       </c>
@@ -6978,7 +7056,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="25.5">
       <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
@@ -6995,7 +7073,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>146</v>
       </c>
@@ -7012,7 +7090,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="39.299999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" ht="39.299999999999997">
       <c r="A19" s="1" t="s">
         <v>147</v>
       </c>
@@ -7029,7 +7107,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" ht="25.5">
       <c r="A20" s="1" t="s">
         <v>148</v>
       </c>
@@ -7046,7 +7124,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" ht="25.5">
       <c r="A21" s="1" t="s">
         <v>149</v>
       </c>
@@ -7063,7 +7141,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" ht="37.799999999999997">
       <c r="A22" s="1" t="s">
         <v>293</v>
       </c>
@@ -7080,7 +7158,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="37.799999999999997">
       <c r="A23" s="1" t="s">
         <v>294</v>
       </c>
@@ -7097,7 +7175,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="25.5">
       <c r="A24" s="3" t="s">
         <v>156</v>
       </c>
@@ -7114,7 +7192,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" ht="25.5">
       <c r="A25" s="1" t="s">
         <v>157</v>
       </c>
@@ -7131,7 +7209,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" ht="25.5">
       <c r="A26" s="1" t="s">
         <v>158</v>
       </c>
@@ -7148,7 +7226,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" ht="25.5">
       <c r="A27" s="1" t="s">
         <v>159</v>
       </c>
@@ -7165,7 +7243,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" ht="36.9">
       <c r="A28" s="1" t="s">
         <v>160</v>
       </c>
@@ -7182,7 +7260,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>346</v>
       </c>
@@ -7199,7 +7277,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" ht="36.9">
       <c r="A30" s="1" t="s">
         <v>347</v>
       </c>
@@ -7216,7 +7294,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" s="3" customFormat="1">
       <c r="A31" s="3" t="s">
         <v>165</v>
       </c>
@@ -7233,7 +7311,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>166</v>
       </c>
@@ -7250,7 +7328,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>167</v>
       </c>
@@ -7267,7 +7345,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" ht="27">
       <c r="A34" s="1" t="s">
         <v>168</v>
       </c>
@@ -7284,7 +7362,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" ht="25.5">
       <c r="A35" s="1" t="s">
         <v>169</v>
       </c>
@@ -7301,7 +7379,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" ht="37.799999999999997">
       <c r="A36" s="1" t="s">
         <v>170</v>
       </c>
@@ -7318,7 +7396,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" ht="25.5">
       <c r="A37" s="1" t="s">
         <v>171</v>
       </c>
@@ -7335,7 +7413,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="1" t="s">
         <v>355</v>
       </c>
@@ -7352,7 +7430,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" s="3" customFormat="1" ht="37.799999999999997">
       <c r="A39" s="3" t="s">
         <v>178</v>
       </c>
@@ -7369,7 +7447,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" ht="25.5">
       <c r="A40" s="1" t="s">
         <v>180</v>
       </c>
@@ -7386,7 +7464,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="27">
       <c r="A41" s="1" t="s">
         <v>181</v>
       </c>
@@ -7403,7 +7481,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" ht="25.5">
       <c r="A42" s="1" t="s">
         <v>179</v>
       </c>
@@ -7420,7 +7498,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" ht="25.5">
       <c r="A43" s="1" t="s">
         <v>182</v>
       </c>
@@ -7437,7 +7515,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="49.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" ht="49.2">
       <c r="A44" s="1" t="s">
         <v>183</v>
       </c>
@@ -7454,7 +7532,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" s="3" customFormat="1" ht="37.799999999999997">
       <c r="A45" s="3" t="s">
         <v>194</v>
       </c>
@@ -7471,7 +7549,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" ht="25.5">
       <c r="A46" s="1" t="s">
         <v>195</v>
       </c>
@@ -7488,7 +7566,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" ht="36.9">
       <c r="A47" s="1" t="s">
         <v>196</v>
       </c>
@@ -7505,7 +7583,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="27" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" ht="27">
       <c r="A48" s="1" t="s">
         <v>197</v>
       </c>
@@ -7522,7 +7600,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="50.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" ht="50.7">
       <c r="A49" s="1" t="s">
         <v>198</v>
       </c>
@@ -7539,7 +7617,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" ht="25.5">
       <c r="A50" s="1" t="s">
         <v>199</v>
       </c>
@@ -7556,7 +7634,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" ht="25.5">
       <c r="A51" s="1" t="s">
         <v>200</v>
       </c>
@@ -7573,7 +7651,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
update warning anim to control visible time add icons to incident history remove unused code from alterations
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="597">
   <si>
     <t>XXXX</t>
   </si>
@@ -2026,6 +2026,30 @@
   </si>
   <si>
     <t>Selecciona un idioma</t>
+  </si>
+  <si>
+    <t>Requrires {0} officers for {1} turns</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_REQUIREMENT_PLURAL</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_REQUIREMENT_SINGULAR</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_REQUIREMENT_OFFICER_PLURAL</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_REQUIREMENT_TURN_PLURAL</t>
+  </si>
+  <si>
+    <t>Requires {0} officers for 1 turn</t>
+  </si>
+  <si>
+    <t>Requrires 1 officer for 1 turn</t>
+  </si>
+  <si>
+    <t>Requires 1 officer for {0} turns</t>
   </si>
 </sst>
 </file>
@@ -4950,10 +4974,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6584,6 +6608,74 @@
       </c>
       <c r="E95" s="16" t="s">
         <v>584</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="14" t="s">
+        <v>591</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaks to UI: change severity colors change layering of objects change text to be more descriptive change font size add multipliers to increments and decrements to satisfaction
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="573">
   <si>
     <t>XXXX</t>
   </si>
@@ -1389,9 +1389,6 @@
     <t>BASIC_TEXT_NO_OFFICERS</t>
   </si>
   <si>
-    <t>No officers available!</t>
-  </si>
-  <si>
     <t>BASIC_TEXT_RESUME</t>
   </si>
   <si>
@@ -1972,6 +1969,15 @@
   </si>
   <si>
     <t>The ignore button will not send any officers to investigate an incident. *2n*Use this when you do not have enough officers available or the incident is too resource intensive. But, use the option with care, ignored incidents may develop to be much worse</t>
+  </si>
+  <si>
+    <t>Not Enough Officers!</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CLOSE_CASE</t>
+  </si>
+  <si>
+    <t>Close Case</t>
   </si>
 </sst>
 </file>
@@ -2881,7 +2887,7 @@
         <v>154</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>0</v>
@@ -3051,7 +3057,7 @@
         <v>168</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
@@ -3357,7 +3363,7 @@
         <v>200</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
@@ -3663,7 +3669,7 @@
         <v>241</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>0</v>
@@ -3867,7 +3873,7 @@
         <v>261</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>0</v>
@@ -4797,7 +4803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -5704,10 +5710,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5751,7 +5757,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="11" customFormat="1">
@@ -5759,16 +5765,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="11" customFormat="1">
@@ -5785,7 +5791,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="11" customFormat="1">
@@ -5802,7 +5808,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="11" customFormat="1">
@@ -5819,16 +5825,16 @@
         <v>0</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="11" customFormat="1">
       <c r="A7" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>452</v>
-      </c>
       <c r="C7" s="11" t="s">
         <v>0</v>
       </c>
@@ -5836,7 +5842,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="11" customFormat="1" ht="14.7" customHeight="1">
@@ -5853,7 +5859,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="11" customFormat="1">
@@ -5870,7 +5876,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="11" customFormat="1">
@@ -5887,7 +5893,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="11" customFormat="1">
@@ -5904,7 +5910,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="11" customFormat="1">
@@ -5921,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -5938,7 +5944,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="11" customFormat="1">
@@ -5955,7 +5961,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -5972,7 +5978,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -5989,7 +5995,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="11" customFormat="1">
@@ -6006,7 +6012,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="11" customFormat="1">
@@ -6023,7 +6029,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="11" customFormat="1">
@@ -6040,16 +6046,16 @@
         <v>0</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="11" customFormat="1">
       <c r="A20" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>386</v>
-      </c>
       <c r="C20" s="11" t="s">
         <v>0</v>
       </c>
@@ -6057,7 +6063,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1">
@@ -6074,7 +6080,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="11" customFormat="1">
@@ -6091,7 +6097,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="11" customFormat="1">
@@ -6108,7 +6114,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="11" customFormat="1">
@@ -6125,7 +6131,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="11" customFormat="1">
@@ -6142,7 +6148,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="11" customFormat="1">
@@ -6159,7 +6165,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="11" customFormat="1">
@@ -6176,7 +6182,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="11" customFormat="1">
@@ -6193,7 +6199,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="11" customFormat="1">
@@ -6210,7 +6216,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="11" customFormat="1">
@@ -6227,7 +6233,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="11" customFormat="1" ht="43.2">
@@ -6244,7 +6250,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="11" customFormat="1">
@@ -6261,7 +6267,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="11" customFormat="1">
@@ -6269,16 +6275,16 @@
         <v>46</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>490</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="11" customFormat="1">
@@ -6295,7 +6301,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="11" customFormat="1">
@@ -6312,7 +6318,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="11" customFormat="1">
@@ -6329,7 +6335,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="11" customFormat="1">
@@ -6346,7 +6352,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="11" customFormat="1">
@@ -6363,7 +6369,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="11" customFormat="1">
@@ -6380,7 +6386,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="11" customFormat="1">
@@ -6397,7 +6403,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="11" customFormat="1">
@@ -6414,7 +6420,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="11" customFormat="1">
@@ -6431,7 +6437,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="11" customFormat="1">
@@ -6448,7 +6454,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="11" customFormat="1">
@@ -6465,7 +6471,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6482,7 +6488,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="11" customFormat="1">
@@ -6490,7 +6496,7 @@
         <v>375</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>376</v>
+        <v>570</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>0</v>
@@ -6499,15 +6505,15 @@
         <v>0</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="11" customFormat="1">
       <c r="A47" s="11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>0</v>
@@ -6516,15 +6522,15 @@
         <v>0</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="11" customFormat="1">
       <c r="A48" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>0</v>
@@ -6533,16 +6539,16 @@
         <v>0</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="11" customFormat="1">
       <c r="A49" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="B49" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>380</v>
-      </c>
       <c r="C49" s="11" t="s">
         <v>0</v>
       </c>
@@ -6550,16 +6556,16 @@
         <v>0</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="11" customFormat="1">
       <c r="A50" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>388</v>
-      </c>
       <c r="C50" s="11" t="s">
         <v>0</v>
       </c>
@@ -6567,16 +6573,16 @@
         <v>0</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="11" customFormat="1">
       <c r="A51" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="B51" s="11" t="s">
-        <v>390</v>
-      </c>
       <c r="C51" s="11" t="s">
         <v>0</v>
       </c>
@@ -6584,16 +6590,16 @@
         <v>0</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="11" customFormat="1">
       <c r="A52" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>392</v>
-      </c>
       <c r="C52" s="11" t="s">
         <v>0</v>
       </c>
@@ -6601,15 +6607,15 @@
         <v>0</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="11" customFormat="1" ht="28.8">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="11" customFormat="1">
       <c r="A53" s="11" t="s">
-        <v>140</v>
+        <v>571</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>141</v>
+        <v>572</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>0</v>
@@ -6618,33 +6624,33 @@
         <v>0</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>547</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="11" customFormat="1" ht="28.8">
       <c r="A54" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="11" customFormat="1" ht="28.8">
+      <c r="A55" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="11" customFormat="1">
-      <c r="A55" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>394</v>
-      </c>
       <c r="C55" s="11" t="s">
         <v>0</v>
       </c>
@@ -6652,84 +6658,84 @@
         <v>0</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="11" customFormat="1">
       <c r="A56" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="11" customFormat="1">
+      <c r="A57" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B57" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="12" t="s">
+      <c r="C57" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="11" customFormat="1" ht="57.6">
+      <c r="A58" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>513</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="11" customFormat="1" ht="57.6">
-      <c r="A57" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="11" customFormat="1" ht="43.2">
-      <c r="A58" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="11" customFormat="1" ht="43.2">
       <c r="A59" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="11" customFormat="1" ht="43.2">
+      <c r="A60" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B60" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="11" customFormat="1" ht="28.8">
-      <c r="A60" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>128</v>
-      </c>
       <c r="C60" s="11" t="s">
         <v>0</v>
       </c>
@@ -6737,15 +6743,15 @@
         <v>0</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="11" customFormat="1" ht="28.8">
       <c r="A61" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>0</v>
@@ -6754,33 +6760,33 @@
         <v>0</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="11" customFormat="1" ht="28.8">
       <c r="A62" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="11" customFormat="1" ht="28.8">
+      <c r="A63" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B63" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C62" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="11" customFormat="1" ht="57.6">
-      <c r="A63" s="11" t="s">
-        <v>565</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>570</v>
-      </c>
       <c r="C63" s="11" t="s">
         <v>0</v>
       </c>
@@ -6788,12 +6794,12 @@
         <v>0</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>0</v>
+        <v>518</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="11" customFormat="1" ht="57.6">
       <c r="A64" s="11" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>569</v>
@@ -6808,9 +6814,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="11" customFormat="1" ht="43.2">
+    <row r="65" spans="1:5" s="11" customFormat="1" ht="57.6">
       <c r="A65" s="11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B65" s="11" t="s">
         <v>568</v>
@@ -6827,28 +6833,28 @@
     </row>
     <row r="66" spans="1:5" s="11" customFormat="1" ht="43.2">
       <c r="A66" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="11" customFormat="1" ht="43.2">
+      <c r="A67" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B67" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C66" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="28.8">
-      <c r="A67" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>398</v>
-      </c>
       <c r="C67" s="11" t="s">
         <v>0</v>
       </c>
@@ -6856,12 +6862,12 @@
         <v>0</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="28.8">
       <c r="A68" s="11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>397</v>
@@ -6873,33 +6879,33 @@
         <v>0</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="13" t="s">
-        <v>399</v>
+      <c r="A69" s="11" t="s">
+        <v>395</v>
       </c>
       <c r="B69" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="B70" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C69" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>401</v>
-      </c>
       <c r="C70" s="11" t="s">
         <v>0</v>
       </c>
@@ -6907,15 +6913,15 @@
         <v>0</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>523</v>
+        <v>488</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="11" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>454</v>
+        <v>400</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>0</v>
@@ -6924,12 +6930,12 @@
         <v>0</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>453</v>
@@ -6941,15 +6947,15 @@
         <v>0</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="28.8">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="11" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>432</v>
+        <v>452</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>0</v>
@@ -6958,12 +6964,12 @@
         <v>0</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="28.8">
       <c r="A74" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>431</v>
@@ -6975,12 +6981,12 @@
         <v>0</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="28.8">
       <c r="A75" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>430</v>
@@ -6992,12 +6998,12 @@
         <v>0</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8">
       <c r="A76" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>429</v>
@@ -7009,12 +7015,12 @@
         <v>0</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8">
       <c r="A77" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>428</v>
@@ -7026,66 +7032,66 @@
         <v>0</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8">
       <c r="A78" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="28.8">
+      <c r="A79" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="B79" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="C79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="C78" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="12" t="s">
+      <c r="B80" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="12" t="s">
         <v>531</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="28.8">
-      <c r="A80" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="28.8">
       <c r="A81" s="13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>0</v>
@@ -7094,15 +7100,15 @@
         <v>0</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8">
       <c r="A82" s="13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>0</v>
@@ -7111,15 +7117,15 @@
         <v>0</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="11" customFormat="1" ht="28.8">
-      <c r="A83" s="11" t="s">
-        <v>421</v>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="28.8">
+      <c r="A83" s="13" t="s">
+        <v>419</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>0</v>
@@ -7128,16 +7134,16 @@
         <v>0</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A84" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B84" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="B84" s="11" t="s">
-        <v>426</v>
-      </c>
       <c r="C84" s="11" t="s">
         <v>0</v>
       </c>
@@ -7145,15 +7151,15 @@
         <v>0</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A85" s="11" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>0</v>
@@ -7162,15 +7168,15 @@
         <v>0</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A86" s="11" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>0</v>
@@ -7179,15 +7185,15 @@
         <v>0</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A87" s="11" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="C87" s="11" t="s">
         <v>0</v>
@@ -7196,33 +7202,33 @@
         <v>0</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A88" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="11" customFormat="1" ht="28.8">
+      <c r="A89" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B89" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="B88" s="11" t="s">
-        <v>440</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>437</v>
-      </c>
       <c r="C89" s="11" t="s">
         <v>0</v>
       </c>
@@ -7230,16 +7236,15 @@
         <v>0</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>546</v>
-      </c>
-      <c r="F89" s="11"/>
+        <v>540</v>
+      </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="C90" s="11" t="s">
         <v>0</v>
@@ -7254,10 +7259,10 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="C91" s="11" t="s">
         <v>0</v>
@@ -7272,10 +7277,10 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>0</v>
@@ -7290,10 +7295,10 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>0</v>
@@ -7307,96 +7312,97 @@
       <c r="F93" s="11"/>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="13" t="s">
-        <v>455</v>
+      <c r="A94" s="11" t="s">
+        <v>448</v>
       </c>
       <c r="B94" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="F94" s="11"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="12" t="s">
         <v>555</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="12" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="B95" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="E95" s="11" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="B97" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="B96" s="14" t="s">
-        <v>459</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>459</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>459</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="13" t="s">
-        <v>549</v>
-      </c>
-      <c r="B97" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D97" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="15" t="s">
-        <v>551</v>
+      <c r="C97" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="13" t="s">
+        <v>548</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>552</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="15" t="s">
         <v>550</v>
-      </c>
-      <c r="B98" s="13" t="s">
-        <v>554</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D98" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E98" s="15" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="13" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="C99" s="13" t="s">
         <v>0</v>
@@ -7404,8 +7410,8 @@
       <c r="D99" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E99" s="13" t="s">
-        <v>0</v>
+      <c r="E99" s="15" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -7413,7 +7419,7 @@
         <v>558</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="C100" s="13" t="s">
         <v>0</v>
@@ -7427,10 +7433,10 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="13" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="C101" s="13" t="s">
         <v>0</v>
@@ -7444,11 +7450,11 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="13" t="s">
+        <v>559</v>
+      </c>
+      <c r="B102" s="13" t="s">
         <v>561</v>
       </c>
-      <c r="B102" s="13" t="s">
-        <v>564</v>
-      </c>
       <c r="C102" s="13" t="s">
         <v>0</v>
       </c>
@@ -7456,6 +7462,23 @@
         <v>0</v>
       </c>
       <c r="E102" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="13" t="s">
+        <v>560</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>563</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="13" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial changes to game over screen with new information
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="576">
   <si>
     <t>XXXX</t>
   </si>
@@ -1743,9 +1743,6 @@
     <t>Oficiales requeridos</t>
   </si>
   <si>
-    <t>Sobrevivieron gira</t>
-  </si>
-  <si>
     <t>Puntuación más alta</t>
   </si>
   <si>
@@ -1978,6 +1975,18 @@
   </si>
   <si>
     <t>Close Case</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CASES_RESOLVED</t>
+  </si>
+  <si>
+    <t>Cases Resolved</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_TURNS_SURVIVED</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
@@ -5710,10 +5719,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5757,7 +5766,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="11" customFormat="1">
@@ -6343,7 +6352,7 @@
         <v>56</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>373</v>
+        <v>575</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>0</v>
@@ -6352,7 +6361,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="11" customFormat="1">
@@ -6369,15 +6378,15 @@
         <v>0</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="11" customFormat="1">
       <c r="A39" s="11" t="s">
-        <v>66</v>
+        <v>572</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>115</v>
+        <v>573</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>0</v>
@@ -6386,15 +6395,15 @@
         <v>0</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="11" customFormat="1">
       <c r="A40" s="11" t="s">
-        <v>111</v>
+        <v>574</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>112</v>
+        <v>373</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>0</v>
@@ -6403,15 +6412,15 @@
         <v>0</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>497</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="11" customFormat="1">
       <c r="A41" s="11" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>0</v>
@@ -6420,15 +6429,15 @@
         <v>0</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="11" customFormat="1">
       <c r="A42" s="11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>0</v>
@@ -6437,15 +6446,15 @@
         <v>0</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="11" customFormat="1">
       <c r="A43" s="11" t="s">
-        <v>371</v>
+        <v>113</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>372</v>
+        <v>114</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>0</v>
@@ -6454,15 +6463,15 @@
         <v>0</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="11" customFormat="1">
       <c r="A44" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>0</v>
@@ -6471,15 +6480,15 @@
         <v>0</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="11" customFormat="1" ht="28.8">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="11" customFormat="1">
       <c r="A45" s="11" t="s">
-        <v>136</v>
+        <v>371</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>137</v>
+        <v>372</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>0</v>
@@ -6488,15 +6497,15 @@
         <v>0</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="11" customFormat="1">
       <c r="A46" s="11" t="s">
-        <v>375</v>
+        <v>110</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>570</v>
+        <v>109</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>0</v>
@@ -6505,15 +6514,15 @@
         <v>0</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="11" customFormat="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="11" customFormat="1" ht="28.8">
       <c r="A47" s="11" t="s">
-        <v>376</v>
+        <v>136</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>380</v>
+        <v>137</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>0</v>
@@ -6522,15 +6531,15 @@
         <v>0</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="11" customFormat="1">
       <c r="A48" s="11" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>381</v>
+        <v>569</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>0</v>
@@ -6539,15 +6548,15 @@
         <v>0</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="11" customFormat="1">
       <c r="A49" s="11" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>0</v>
@@ -6556,15 +6565,15 @@
         <v>0</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="11" customFormat="1">
       <c r="A50" s="11" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>0</v>
@@ -6573,15 +6582,15 @@
         <v>0</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="11" customFormat="1">
       <c r="A51" s="11" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>0</v>
@@ -6590,15 +6599,15 @@
         <v>0</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="11" customFormat="1">
       <c r="A52" s="11" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>0</v>
@@ -6607,321 +6616,321 @@
         <v>0</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="11" customFormat="1">
       <c r="A53" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="11" customFormat="1">
+      <c r="A54" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="11" customFormat="1">
+      <c r="A55" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>571</v>
       </c>
-      <c r="B53" s="11" t="s">
-        <v>572</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="11" customFormat="1" ht="28.8">
-      <c r="A54" s="11" t="s">
+      <c r="C55" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="11" customFormat="1" ht="28.8">
+      <c r="A56" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B56" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="11" customFormat="1" ht="28.8">
-      <c r="A55" s="11" t="s">
+      <c r="C56" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="11" customFormat="1" ht="28.8">
+      <c r="A57" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B57" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="12" t="s">
+      <c r="C57" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="11" customFormat="1">
+      <c r="A58" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="11" customFormat="1">
-      <c r="A56" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="12" t="s">
+    <row r="59" spans="1:5" s="11" customFormat="1">
+      <c r="A59" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="11" customFormat="1">
-      <c r="A57" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="12" t="s">
+    <row r="60" spans="1:5" s="11" customFormat="1" ht="57.6">
+      <c r="A60" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="11" customFormat="1" ht="57.6">
-      <c r="A58" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="12" t="s">
+    <row r="61" spans="1:5" s="11" customFormat="1" ht="43.2">
+      <c r="A61" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="12" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="11" customFormat="1" ht="43.2">
-      <c r="A59" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="12" t="s">
+    <row r="62" spans="1:5" s="11" customFormat="1" ht="43.2">
+      <c r="A62" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12" t="s">
         <v>514</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="11" customFormat="1" ht="43.2">
-      <c r="A60" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="11" customFormat="1" ht="28.8">
-      <c r="A61" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="11" customFormat="1" ht="28.8">
-      <c r="A62" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="11" customFormat="1" ht="28.8">
       <c r="A63" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="11" customFormat="1" ht="28.8">
+      <c r="A64" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="11" customFormat="1" ht="28.8">
+      <c r="A65" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B65" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C63" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="12" t="s">
+      <c r="C65" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="11" customFormat="1" ht="57.6">
+      <c r="A66" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="11" customFormat="1" ht="57.6">
+      <c r="A67" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="11" customFormat="1" ht="43.2">
+      <c r="A68" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="11" customFormat="1" ht="43.2">
+      <c r="A69" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="12" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="11" customFormat="1" ht="57.6">
-      <c r="A64" s="11" t="s">
-        <v>564</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>569</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="11" customFormat="1" ht="57.6">
-      <c r="A65" s="11" t="s">
-        <v>565</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="11" customFormat="1" ht="43.2">
-      <c r="A66" s="11" t="s">
-        <v>566</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>567</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="11" customFormat="1" ht="43.2">
-      <c r="A67" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" s="12" t="s">
+    <row r="70" spans="1:5" ht="28.8">
+      <c r="A70" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>519</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="28.8">
-      <c r="A68" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="13" t="s">
-        <v>398</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="11" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>0</v>
@@ -6930,15 +6939,15 @@
         <v>0</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="11" t="s">
-        <v>401</v>
+      <c r="A72" s="13" t="s">
+        <v>398</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>453</v>
+        <v>47</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>0</v>
@@ -6947,50 +6956,50 @@
         <v>0</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>523</v>
+        <v>488</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B75" s="11" t="s">
         <v>452</v>
       </c>
-      <c r="C73" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="28.8">
-      <c r="A74" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="28.8">
-      <c r="A75" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>430</v>
-      </c>
       <c r="C75" s="11" t="s">
         <v>0</v>
       </c>
@@ -6998,15 +7007,15 @@
         <v>0</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8">
       <c r="A76" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>0</v>
@@ -7015,15 +7024,15 @@
         <v>0</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8">
       <c r="A77" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>0</v>
@@ -7032,15 +7041,15 @@
         <v>0</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8">
       <c r="A78" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>0</v>
@@ -7049,118 +7058,118 @@
         <v>0</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="28.8">
       <c r="A79" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="28.8">
+      <c r="A80" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="28.8">
+      <c r="A81" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="B79" s="11" t="s">
+      <c r="B81" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="C79" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="12" t="s">
+      <c r="C81" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="12" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="12" t="s">
         <v>530</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="28.8">
-      <c r="A81" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.8">
-      <c r="A82" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8">
       <c r="A83" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="28.8">
+      <c r="A84" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="28.8">
+      <c r="A85" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B85" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="C83" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="12" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="11" customFormat="1" ht="28.8">
-      <c r="A84" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="11" customFormat="1" ht="28.8">
-      <c r="A85" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>425</v>
-      </c>
       <c r="C85" s="11" t="s">
         <v>0</v>
       </c>
@@ -7168,15 +7177,15 @@
         <v>0</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A86" s="11" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>0</v>
@@ -7185,15 +7194,15 @@
         <v>0</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A87" s="11" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="C87" s="11" t="s">
         <v>0</v>
@@ -7202,15 +7211,15 @@
         <v>0</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A88" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C88" s="11" t="s">
         <v>0</v>
@@ -7219,51 +7228,50 @@
         <v>0</v>
       </c>
       <c r="E88" s="12" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A89" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="12" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="11" customFormat="1" ht="28.8">
+      <c r="A90" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="12" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="11" customFormat="1" ht="28.8">
+      <c r="A91" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="B91" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="C89" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="12" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="F90" s="11"/>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="B91" s="11" t="s">
-        <v>442</v>
-      </c>
       <c r="C91" s="11" t="s">
         <v>0</v>
       </c>
@@ -7271,16 +7279,15 @@
         <v>0</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>544</v>
-      </c>
-      <c r="F91" s="11"/>
+        <v>539</v>
+      </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>0</v>
@@ -7289,16 +7296,16 @@
         <v>0</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="F92" s="11"/>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>0</v>
@@ -7307,16 +7314,16 @@
         <v>0</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F93" s="11"/>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
       <c r="C94" s="11" t="s">
         <v>0</v>
@@ -7325,101 +7332,103 @@
         <v>0</v>
       </c>
       <c r="E94" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="F94" s="11"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="F94" s="11"/>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="B95" s="11" t="s">
-        <v>554</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>555</v>
-      </c>
+      <c r="F95" s="11"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="F96" s="11"/>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="B96" s="11" t="s">
+      <c r="B98" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C98" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D98" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="E96" s="11" t="s">
+      <c r="E98" s="11" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="11" t="s">
+    <row r="99" spans="1:5">
+      <c r="A99" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B99" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C99" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D99" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="E97" s="14" t="s">
+      <c r="E99" s="14" t="s">
         <v>458</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="13" t="s">
-        <v>548</v>
-      </c>
-      <c r="B98" s="13" t="s">
-        <v>552</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D98" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E98" s="15" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="13" t="s">
-        <v>549</v>
-      </c>
-      <c r="B99" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="C99" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D99" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E99" s="15" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="13" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="C100" s="13" t="s">
         <v>0</v>
@@ -7427,16 +7436,16 @@
       <c r="D100" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E100" s="13" t="s">
-        <v>0</v>
+      <c r="E100" s="15" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="13" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C101" s="13" t="s">
         <v>0</v>
@@ -7444,13 +7453,13 @@
       <c r="D101" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E101" s="13" t="s">
-        <v>0</v>
+      <c r="E101" s="15" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="13" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B102" s="13" t="s">
         <v>561</v>
@@ -7467,18 +7476,52 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>555</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="13" t="s">
+        <v>558</v>
+      </c>
+      <c r="B104" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="B103" s="13" t="s">
-        <v>563</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D103" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E103" s="13" t="s">
+      <c r="C104" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="13" t="s">
+        <v>559</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>562</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="13" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add information panel to give quick tips about incidents, officers and the satisfaction bar on screen
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="586">
   <si>
     <t>XXXX</t>
   </si>
@@ -1987,6 +1987,36 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>TIPS_SATISFACTION</t>
+  </si>
+  <si>
+    <t>{0}% Citizen Satisfaction*n*Keep the badge out of the red area by making good choices</t>
+  </si>
+  <si>
+    <t>{0} Active Cases*n*Close cases by making good choices to make a big difference to citizen satisfaction</t>
+  </si>
+  <si>
+    <t>TIPS_INCIDENT</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICER</t>
+  </si>
+  <si>
+    <t>TIPS_OFFICERS</t>
+  </si>
+  <si>
+    <t>TIPS_INCIDENTS</t>
+  </si>
+  <si>
+    <t>{0} Active Case*n*Close cases by making good choices to make a big difference to citizen satisfaction</t>
+  </si>
+  <si>
+    <t>{0} Available Officer*n*A limited number available so be careful, you never know when a severe incident may occur</t>
+  </si>
+  <si>
+    <t>{0} Available Officers*n*A limited number available so be careful, you never know when a severe incident may occur</t>
   </si>
 </sst>
 </file>
@@ -5719,10 +5749,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7522,6 +7552,91 @@
         <v>0</v>
       </c>
       <c r="E105" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="28.8">
+      <c r="A106" s="13" t="s">
+        <v>576</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>577</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="28.8">
+      <c r="A107" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="28.8">
+      <c r="A108" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="28.8">
+      <c r="A109" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="28.8">
+      <c r="A110" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="13" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add turn info to the infomration screen
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="590">
   <si>
     <t>XXXX</t>
   </si>
@@ -2017,6 +2017,18 @@
   </si>
   <si>
     <t>{0} Available Officers*n*A limited number available so be careful, you never know when a severe incident may occur</t>
+  </si>
+  <si>
+    <t>TIPS_TURN</t>
+  </si>
+  <si>
+    <t>TIPS_TURNS</t>
+  </si>
+  <si>
+    <t>{0} Turns Survived*n*Each turn will consist of a number of cases with choices to make</t>
+  </si>
+  <si>
+    <t>{0} Turn Survived*n*Each turn will consist of a number of cases with choices to make</t>
   </si>
 </sst>
 </file>
@@ -5749,10 +5761,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7637,6 +7649,40 @@
         <v>0</v>
       </c>
       <c r="E110" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="28.8">
+      <c r="A111" s="13" t="s">
+        <v>586</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>589</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.8">
+      <c r="A112" s="13" t="s">
+        <v>587</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>588</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="13" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add remaining scenarios for Valencia
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="608">
   <si>
     <t>XXXX</t>
   </si>
@@ -1560,9 +1560,6 @@
     <t>Great Job!</t>
   </si>
   <si>
-    <t>Remember thet officers sent to incidents requiring just 1 turn will return at the start of the next turn</t>
-  </si>
-  <si>
     <t>TIPS_OFFICER_ONE_TURN_NEGATIVE_1</t>
   </si>
   <si>
@@ -1671,18 +1668,6 @@
     <t>Los oficiales no pueden hacer ninguna detención en relación con el caso</t>
   </si>
   <si>
-    <t>¡Pedir a los ciudadanos en busca de ayuda!</t>
-  </si>
-  <si>
-    <t>Ciudadanos proporcionan evidencia a través de la aplicación INSPEC2T, 2 han sido acusados</t>
-  </si>
-  <si>
-    <t>Ciudadano no proporciona ninguna evidencia sólida para el caso</t>
-  </si>
-  <si>
-    <t>Sin más incidentes para comprobar esta vuelta</t>
-  </si>
-  <si>
     <t>Ir</t>
   </si>
   <si>
@@ -1710,9 +1695,6 @@
     <t>Oficiales</t>
   </si>
   <si>
-    <t>Detenciones</t>
-  </si>
-  <si>
     <t>Casos activos</t>
   </si>
   <si>
@@ -1722,9 +1704,6 @@
     <t>Juego terminado</t>
   </si>
   <si>
-    <t>Usted sobrevivió {0} Activa*2n*La felicidad ciudadana caído por debajo del 10%, los ciudadanos ya no se sienten seguros bajo su control</t>
-  </si>
-  <si>
     <t>Disponible</t>
   </si>
   <si>
@@ -1758,15 +1737,9 @@
     <t>Ubicación</t>
   </si>
   <si>
-    <t>Descargar la aplicación INSPEC2T Ahora!</t>
-  </si>
-  <si>
     <t>Descripción</t>
   </si>
   <si>
-    <t>¡ADVERTENCIA! Selección de espera hará que el caso de expirar, la reducción de satisfacción de los ciudadanos</t>
-  </si>
-  <si>
     <t>No hay directores disponibles!</t>
   </si>
   <si>
@@ -1788,45 +1761,18 @@
     <t>Cambiar locación</t>
   </si>
   <si>
-    <t>Ayudar a su fuerza de policía local para resolver crímenes reales con la aplicación Inspeccionar</t>
-  </si>
-  <si>
     <t>Cómo jugar</t>
   </si>
   <si>
     <t>Pulse para continuar…</t>
   </si>
   <si>
-    <t>La parte superior de la pantalla muestra el estado actual de la satisfacción, más allá en rojo que vaya, cuanto más cerca esté a punto de perder. Resolver los casos de mantenerse fuera de la zona roja</t>
-  </si>
-  <si>
-    <t>La barra de estado muestra la satisfacción real, tratar de mantener esta por encima del 10% para el mayor número de vueltas como puedas</t>
-  </si>
-  <si>
-    <t>El indicador oficial le informa cuántos agentes están disponibles y el número de vueltas hasta que los oficiales en el campo, no vuelva y vuelven a estar disponibles</t>
-  </si>
-  <si>
-    <t>Este cuadro le dará información sobre el caso actual y mantendrá informados de su condición</t>
-  </si>
-  <si>
-    <t>Cada caso se necesita un número de oficiales para asistir a un número determinado de vueltas</t>
-  </si>
-  <si>
-    <t>Aquí podrás ver todos sus incidentes activos, que son de color coordinado por la gravedad. El rojo es más grave</t>
-  </si>
-  <si>
     <t>Cada caso puede tener hasta 3 opciones, esperar a más oficiales, mandan a los funcionarios requeridos o pedir a los ciudadanos en busca de ayuda cuando esté disponible</t>
   </si>
   <si>
-    <t>Ayúdanos para que la aplicación mejor, mediante el envío de su respuesta!</t>
-  </si>
-  <si>
     <t>Enviar comentarios!</t>
   </si>
   <si>
-    <t>{0}% de satisfacción</t>
-  </si>
-  <si>
     <t>{0} No haga caso de la caja {1}*2n*-{2}% Satisfacción</t>
   </si>
   <si>
@@ -1842,75 +1788,12 @@
     <t>Los ciudadanos pueden ser capaces de ayudar con los casos con información o pruebas, aprovechar al máximo la opción</t>
   </si>
   <si>
-    <t>Forse la prossima volta chiedere ai cittadini di informazioni, potrebbe ridurre gli ufficiali richiesti</t>
-  </si>
-  <si>
-    <t>Forse la prossima volta chiedere aiuto dei cittadini dalla INSPEC2T app, si potrebbe ridurre il numero di giri richiesto</t>
-  </si>
-  <si>
-    <t>Ignorando un caso abbasserà la soddisfazione alla fine del turno, cerca di chiudere il maggior numero di casi possibili</t>
-  </si>
-  <si>
-    <t>A volte è meglio risparmiare ufficiali per un caso più grave</t>
-  </si>
-  <si>
-    <t>Ignorando incidenti è più probabile che dare risoluzioni negativi per gli incidenti, cerca di non ignorare i casi</t>
-  </si>
-  <si>
-    <t>Alcuni incidenti si svilupperà meno di altri, ricordati di valutare le informazioni fornite con attenzione</t>
-  </si>
-  <si>
-    <t>Fare attenzione, a volte incidenti ignorando causerà loro di svilupparsi.</t>
-  </si>
-  <si>
-    <t>Ricordatevi di tenere d'occhio le prossime incidenti per mantenere ufficiali per gli incidenti potenzialmente più gravi</t>
-  </si>
-  <si>
-    <t>Agenti di invio condurranno sempre ad una risoluzione positiva, ma a costo di risorse, fare attenzione decisioni</t>
-  </si>
-  <si>
-    <t>Ricordate gli ufficiali inviati agli incidenti che richiedono solo 1 giro tornerà all'inizio del turno successivo</t>
-  </si>
-  <si>
-    <t>L'invio di agenti di incidenti che richiedono solo 1 giro è un ottimo modo per cancellare i casi attivi</t>
-  </si>
-  <si>
-    <t>Ignorando alti casi di gravità avrà un grande impatto sulla soddisfazione.</t>
-  </si>
-  <si>
-    <t>Assicurati di dare alta priorità gravità dei casi, non riuscendo a risolvere le darà un grande rigore soddisfazione!</t>
-  </si>
-  <si>
-    <t>¡Bello!</t>
-  </si>
-  <si>
-    <t>¡Eccezionale!</t>
-  </si>
-  <si>
-    <t>¡Ottimo lavoro!</t>
-  </si>
-  <si>
-    <t>¡Bella scelta!</t>
-  </si>
-  <si>
-    <t>¡Ben fatto!</t>
-  </si>
-  <si>
-    <t>Si prega di impostare la posizione qui sotto per ottenere la migliore esperienza!</t>
-  </si>
-  <si>
-    <t>Benvenuti a risorsa forza, assumere il ruolo di un operatore di polizia e contribuire a risolvere i crimini in tutta la città. È necessario utilizzare con attenzione le risorse per risolvere i casi e mantenere i civili felici e sentirsi al sicuro. *2n*Ma attenzione, gli ufficiali sono limitati in modo da utilizzare con saggezza</t>
-  </si>
-  <si>
     <t>WARNING_TEXT_LOCATION</t>
   </si>
   <si>
     <t>WARNING_TEXT_LANGUAGE</t>
   </si>
   <si>
-    <t>establecer una posición</t>
-  </si>
-  <si>
     <t>establecer un idioma</t>
   </si>
   <si>
@@ -1926,9 +1809,6 @@
     <t>Selecciona un idioma</t>
   </si>
   <si>
-    <t>Requrires {0} officers for {1} turns</t>
-  </si>
-  <si>
     <t>BASIC_TEXT_REQUIREMENT_PLURAL</t>
   </si>
   <si>
@@ -1944,9 +1824,6 @@
     <t>Requires {0} officers for 1 turn</t>
   </si>
   <si>
-    <t>Requrires 1 officer for 1 turn</t>
-  </si>
-  <si>
     <t>Requires 1 officer for {0} turns</t>
   </si>
   <si>
@@ -2029,6 +1906,183 @@
   </si>
   <si>
     <t>{0} Turn Survived*n*Each turn will consist of a number of cases with choices to make</t>
+  </si>
+  <si>
+    <t>Asegúrese de dar alta prioridad a los casos de gravedad, no resolverlo dará una gran pena de satisfacción!</t>
+  </si>
+  <si>
+    <t>Ignorar los casos de alta severidad tendrá un gran impacto en la satisfacción.</t>
+  </si>
+  <si>
+    <t>Envío de oficiales a incidentes que sólo requieren 1 turno es una gran manera de borrar los casos activos</t>
+  </si>
+  <si>
+    <t>Remember that officers sent to incidents requiring just 1 turn will return at the start of the next turn</t>
+  </si>
+  <si>
+    <t>Requires {0} officers for {1} turns</t>
+  </si>
+  <si>
+    <t>Requires 1 officer for 1 turn</t>
+  </si>
+  <si>
+    <t>Recuerde que los oficiales enviados a incidentes que requieren sólo 1 vuelta regresarán al inicio del siguiente turno</t>
+  </si>
+  <si>
+    <t>Los oficiales de envío siempre darán lugar a una resolución positiva, pero a costa de los recursos, tomarán decisiones con cuidado</t>
+  </si>
+  <si>
+    <t>Recuerde mantener un ojo en los próximos incidentes para mantener a los oficiales de los incidentes potencialmente más graves</t>
+  </si>
+  <si>
+    <t>Tenga cuidado, a veces ignorar incidentes hará que se desarrollen.</t>
+  </si>
+  <si>
+    <t>¡Bien hecho!</t>
+  </si>
+  <si>
+    <t>¡Buena elección!</t>
+  </si>
+  <si>
+    <t>¡Gran trabajo!</t>
+  </si>
+  <si>
+    <t>¡Increíble!</t>
+  </si>
+  <si>
+    <t>¡Bonito!</t>
+  </si>
+  <si>
+    <t>Establecer una ubicación</t>
+  </si>
+  <si>
+    <t>Algunos incidentes se desarrollarán menos que otros, recuerde evaluar la información proporcionada cuidadosamente</t>
+  </si>
+  <si>
+    <t>Ignorar los incidentes es más probable que dé resoluciones negativas para los incidentes, tratar de no ignorar los casos</t>
+  </si>
+  <si>
+    <t>A veces es mejor salvar a los oficiales para un caso más severo</t>
+  </si>
+  <si>
+    <t>Ignorar un caso reducirá la satisfacción al final del turno, tratar de cerrar el mayor número posible de casos</t>
+  </si>
+  <si>
+    <t>Tal vez la próxima vez que pida ayuda a los ciudadanos de la aplicación INSPEC2T, podría reducir el número de turnos requeridos</t>
+  </si>
+  <si>
+    <t>Tal vez la próxima vez que pidan información a los ciudadanos, podría reducir los oficiales requeridos</t>
+  </si>
+  <si>
+    <t>{0}% Satisfacción</t>
+  </si>
+  <si>
+    <t>¡Ayúdanos a mejorar la aplicación, enviándonos tus comentarios!</t>
+  </si>
+  <si>
+    <t>Enviando el número requerido de oficiales a un incidente descubrirá más información o llevará a resolver un caso. *2n* Los oficiales enviados a un incidente no estarán disponibles hasta que regresen</t>
+  </si>
+  <si>
+    <t>A veces, el botón de ciudadanía estará disponible donde se puede pedir a los miembros del público que ayuden a brindar asistencia con un incidente. *2n* Un recurso efectivo, pero pedir ayuda en todos los incidentes no será beneficioso y puede poner en peligro a los ciudadanos</t>
+  </si>
+  <si>
+    <t>El botón de ignorar no enviará a ningún oficial a investigar un incidente. *2n* Use esto cuando no tenga suficientes oficiales disponibles o el incidente sea demasiado intensivo en recursos. Pero, use la opción con cuidado, los incidentes ignorados pueden desarrollarse para ser mucho peor</t>
+  </si>
+  <si>
+    <t>Aquí verá todos sus incidentes activos, que son el color coordinado por la gravedad. El rojo es más severo</t>
+  </si>
+  <si>
+    <t>Cada caso necesitará un número de oficiales para asistir por un número determinado de vueltas</t>
+  </si>
+  <si>
+    <t>Esta casilla te dará información sobre el caso actual y te mantendrá informado sobre su estado</t>
+  </si>
+  <si>
+    <t>El indicador de oficial le informa cuántos oficiales están disponibles y cuántos turnos hasta que los oficiales en el campo regresan y vuelven a estar disponibles</t>
+  </si>
+  <si>
+    <t>La barra de estado muestra la satisfacción real, intenta mantener esto por encima del 10% para tantas vueltas como puedas</t>
+  </si>
+  <si>
+    <t>La parte superior de la pantalla muestra el estado de satisfacción actual, cuanto más en rojo que ir, más cerca está de perder. Resolver los casos para mantenerse fuera del rojo</t>
+  </si>
+  <si>
+    <t>Ayude a su policía local a resolver crímenes reales con la aplicación Inspec2t</t>
+  </si>
+  <si>
+    <t>Por favor, establezca su ubicación a continuación para obtener la mejor experiencia!</t>
+  </si>
+  <si>
+    <t>Caso cerrado</t>
+  </si>
+  <si>
+    <t>¡ADVERTENCIA! Seleccionar la espera hará que el caso expire, reduciendo la satisfacción ciudadana</t>
+  </si>
+  <si>
+    <t>Descargue la aplicación INSPEC2T ahora!</t>
+  </si>
+  <si>
+    <t>vueltas sobrevivientes</t>
+  </si>
+  <si>
+    <t>Casos Resueltos</t>
+  </si>
+  <si>
+    <t>Puntuación</t>
+  </si>
+  <si>
+    <t>Sobreviviste {0} Vueltas *2n* La felicidad ciudadana cae por debajo del 10%, los ciudadanos ya no se sienten seguros bajo tu control</t>
+  </si>
+  <si>
+    <t>arrestos</t>
+  </si>
+  <si>
+    <t>El ciudadano no proporciona ninguna evidencia sólida para el caso</t>
+  </si>
+  <si>
+    <t>No más incidentes para comprobar este turno</t>
+  </si>
+  <si>
+    <t>Los ciudadanos aportan pruebas a través de la aplicación INSPEC2T, 2 han sido acusados</t>
+  </si>
+  <si>
+    <t>¡Pida ayuda a los ciudadanos!</t>
+  </si>
+  <si>
+    <t>Bienvenido a la fuerza de recursos, asumir el papel de un operador de policía y ayudar a resolver los crímenes en toda la ciudad. Debes usar tus recursos cuidadosamente para resolver casos y mantener a los civiles contentos y seguros. *2n* Pero ten cuidado, los oficiales son limitados, así que úsalos sabiamente</t>
+  </si>
+  <si>
+    <t>Requiere 1 oficial durante 1 turno</t>
+  </si>
+  <si>
+    <t>Requiere {0} oficiales para {1} vueltas</t>
+  </si>
+  <si>
+    <t>Requiere {0} oficiales para 1 turno</t>
+  </si>
+  <si>
+    <t>Requiere 1 oficial para {0} turnos</t>
+  </si>
+  <si>
+    <t>{0}% Satisfacción ciudadana *n* Mantenga la insignia fuera del área roja haciendo buenas elecciones</t>
+  </si>
+  <si>
+    <t>{0} Caso Activo *n* Cierre los casos tomando buenas decisiones para hacer una gran diferencia en la satisfacción de los ciudadanos</t>
+  </si>
+  <si>
+    <t>{0} Casos activos *n* Cierre los casos haciendo buenas elecciones para hacer una gran diferencia en la satisfacción de los ciudadanos</t>
+  </si>
+  <si>
+    <t>{0} Oficial disponible *n* Un número limitado disponible, así que tenga cuidado, nunca se sabe cuándo puede ocurrir un incidente grave</t>
+  </si>
+  <si>
+    <t>{0} Oficiales Disponibles *n* Un número limitado disponible, así que ten cuidado, nunca se sabe cuándo puede ocurrir un incidente grave</t>
+  </si>
+  <si>
+    <t>{0} Turn Survived *n* Cada turno consistirá en un número de casos con opciones para hacer</t>
+  </si>
+  <si>
+    <t>{0} Turnos Sobrevividos *n* Cada turno consistirá en un número de casos con opciones para hacer</t>
   </si>
 </sst>
 </file>
@@ -2130,7 +2184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2165,17 +2219,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5763,18 +5823,18 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="49.15625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="62.9453125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.83984375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="16.89453125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="48.47265625" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="8.83984375" style="13"/>
+    <col min="1" max="1" width="49.15625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="62.9453125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14.83984375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.89453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="48.47265625" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="11" customFormat="1">
@@ -5790,7 +5850,7 @@
       <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5807,8 +5867,8 @@
       <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>546</v>
+      <c r="E2" s="16" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="11" customFormat="1">
@@ -5816,16 +5876,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="11" customFormat="1">
@@ -5841,8 +5901,8 @@
       <c r="D4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>460</v>
+      <c r="E4" s="15" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="11" customFormat="1">
@@ -5858,8 +5918,8 @@
       <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>461</v>
+      <c r="E5" s="14" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="11" customFormat="1">
@@ -5875,25 +5935,25 @@
       <c r="D6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>462</v>
+      <c r="E6" s="15" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="11" customFormat="1">
       <c r="A7" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>451</v>
-      </c>
       <c r="C7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>463</v>
+      <c r="E7" s="15" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="11" customFormat="1" ht="14.7" customHeight="1">
@@ -5909,8 +5969,8 @@
       <c r="D8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>464</v>
+      <c r="E8" s="15" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="11" customFormat="1">
@@ -5926,8 +5986,8 @@
       <c r="D9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>465</v>
+      <c r="E9" s="15" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="11" customFormat="1">
@@ -5943,8 +6003,8 @@
       <c r="D10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>466</v>
+      <c r="E10" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="11" customFormat="1">
@@ -5960,8 +6020,8 @@
       <c r="D11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>467</v>
+      <c r="E11" s="15" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="11" customFormat="1">
@@ -5977,8 +6037,8 @@
       <c r="D12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>468</v>
+      <c r="E12" s="15" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -5994,8 +6054,8 @@
       <c r="D13" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>469</v>
+      <c r="E13" s="15" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="11" customFormat="1">
@@ -6011,8 +6071,8 @@
       <c r="D14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>470</v>
+      <c r="E14" s="17" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6028,8 +6088,8 @@
       <c r="D15" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>471</v>
+      <c r="E15" s="17" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6045,8 +6105,8 @@
       <c r="D16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>472</v>
+      <c r="E16" s="17" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="11" customFormat="1">
@@ -6062,8 +6122,8 @@
       <c r="D17" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>473</v>
+      <c r="E17" s="17" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="11" customFormat="1">
@@ -6079,8 +6139,8 @@
       <c r="D18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>474</v>
+      <c r="E18" s="15" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="11" customFormat="1">
@@ -6096,8 +6156,8 @@
       <c r="D19" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>475</v>
+      <c r="E19" s="15" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="11" customFormat="1">
@@ -6113,8 +6173,8 @@
       <c r="D20" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>476</v>
+      <c r="E20" s="15" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1">
@@ -6130,8 +6190,8 @@
       <c r="D21" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>477</v>
+      <c r="E21" s="15" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="11" customFormat="1">
@@ -6147,8 +6207,8 @@
       <c r="D22" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>478</v>
+      <c r="E22" s="15" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="11" customFormat="1">
@@ -6164,8 +6224,8 @@
       <c r="D23" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>479</v>
+      <c r="E23" s="15" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="11" customFormat="1">
@@ -6181,8 +6241,8 @@
       <c r="D24" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>480</v>
+      <c r="E24" s="15" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="11" customFormat="1">
@@ -6198,8 +6258,8 @@
       <c r="D25" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>481</v>
+      <c r="E25" s="15" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="11" customFormat="1">
@@ -6215,8 +6275,8 @@
       <c r="D26" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>482</v>
+      <c r="E26" s="15" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="11" customFormat="1">
@@ -6232,8 +6292,8 @@
       <c r="D27" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>483</v>
+      <c r="E27" s="17" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="11" customFormat="1">
@@ -6249,8 +6309,8 @@
       <c r="D28" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>484</v>
+      <c r="E28" s="15" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="11" customFormat="1">
@@ -6266,8 +6326,8 @@
       <c r="D29" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>485</v>
+      <c r="E29" s="15" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="11" customFormat="1">
@@ -6283,8 +6343,8 @@
       <c r="D30" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>486</v>
+      <c r="E30" s="15" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="11" customFormat="1" ht="43.2">
@@ -6300,8 +6360,8 @@
       <c r="D31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>487</v>
+      <c r="E31" s="16" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="11" customFormat="1">
@@ -6317,8 +6377,8 @@
       <c r="D32" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>488</v>
+      <c r="E32" s="15" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="11" customFormat="1">
@@ -6326,7 +6386,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>0</v>
@@ -6334,8 +6394,8 @@
       <c r="D33" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E33" s="12" t="s">
-        <v>490</v>
+      <c r="E33" s="15" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="11" customFormat="1">
@@ -6351,8 +6411,8 @@
       <c r="D34" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="s">
-        <v>493</v>
+      <c r="E34" s="15" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="11" customFormat="1">
@@ -6368,8 +6428,8 @@
       <c r="D35" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="12" t="s">
-        <v>492</v>
+      <c r="E35" s="15" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="11" customFormat="1">
@@ -6385,8 +6445,8 @@
       <c r="D36" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E36" s="12" t="s">
-        <v>491</v>
+      <c r="E36" s="15" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="11" customFormat="1">
@@ -6394,7 +6454,7 @@
         <v>56</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>575</v>
+        <v>534</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>0</v>
@@ -6402,8 +6462,8 @@
       <c r="D37" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E37" s="12" t="s">
-        <v>0</v>
+      <c r="E37" s="16" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="11" customFormat="1">
@@ -6419,16 +6479,16 @@
       <c r="D38" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E38" s="12" t="s">
-        <v>494</v>
+      <c r="E38" s="15" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="11" customFormat="1">
       <c r="A39" s="11" t="s">
-        <v>572</v>
+        <v>531</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>573</v>
+        <v>532</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>0</v>
@@ -6436,13 +6496,13 @@
       <c r="D39" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="12" t="s">
-        <v>0</v>
+      <c r="E39" s="16" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="11" customFormat="1">
       <c r="A40" s="11" t="s">
-        <v>574</v>
+        <v>533</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>373</v>
@@ -6453,8 +6513,8 @@
       <c r="D40" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="12" t="s">
-        <v>0</v>
+      <c r="E40" s="17" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="11" customFormat="1">
@@ -6470,8 +6530,8 @@
       <c r="D41" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="12" t="s">
-        <v>495</v>
+      <c r="E41" s="15" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="11" customFormat="1">
@@ -6487,8 +6547,8 @@
       <c r="D42" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E42" s="12" t="s">
-        <v>496</v>
+      <c r="E42" s="15" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="11" customFormat="1">
@@ -6504,8 +6564,8 @@
       <c r="D43" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E43" s="12" t="s">
-        <v>497</v>
+      <c r="E43" s="15" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="11" customFormat="1">
@@ -6521,8 +6581,8 @@
       <c r="D44" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E44" s="12" t="s">
-        <v>498</v>
+      <c r="E44" s="15" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="11" customFormat="1">
@@ -6538,8 +6598,8 @@
       <c r="D45" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="12" t="s">
-        <v>499</v>
+      <c r="E45" s="16" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="11" customFormat="1">
@@ -6555,8 +6615,8 @@
       <c r="D46" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E46" s="12" t="s">
-        <v>500</v>
+      <c r="E46" s="15" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6572,8 +6632,8 @@
       <c r="D47" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E47" s="12" t="s">
-        <v>501</v>
+      <c r="E47" s="16" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="11" customFormat="1">
@@ -6581,7 +6641,7 @@
         <v>375</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>569</v>
+        <v>528</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>0</v>
@@ -6589,8 +6649,8 @@
       <c r="D48" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="12" t="s">
-        <v>502</v>
+      <c r="E48" s="15" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="11" customFormat="1">
@@ -6606,8 +6666,8 @@
       <c r="D49" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E49" s="12" t="s">
-        <v>503</v>
+      <c r="E49" s="15" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="11" customFormat="1">
@@ -6623,8 +6683,8 @@
       <c r="D50" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E50" s="12" t="s">
-        <v>504</v>
+      <c r="E50" s="15" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="11" customFormat="1">
@@ -6640,8 +6700,8 @@
       <c r="D51" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E51" s="12" t="s">
-        <v>505</v>
+      <c r="E51" s="15" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="11" customFormat="1">
@@ -6657,8 +6717,8 @@
       <c r="D52" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E52" s="12" t="s">
-        <v>506</v>
+      <c r="E52" s="15" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="11" customFormat="1">
@@ -6674,8 +6734,8 @@
       <c r="D53" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E53" s="12" t="s">
-        <v>507</v>
+      <c r="E53" s="15" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="11" customFormat="1">
@@ -6691,16 +6751,16 @@
       <c r="D54" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E54" s="12" t="s">
-        <v>508</v>
+      <c r="E54" s="17" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="11" customFormat="1">
       <c r="A55" s="11" t="s">
-        <v>570</v>
+        <v>529</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>571</v>
+        <v>530</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>0</v>
@@ -6708,8 +6768,8 @@
       <c r="D55" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="12" t="s">
-        <v>0</v>
+      <c r="E55" s="17" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6725,8 +6785,8 @@
       <c r="D56" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E56" s="12" t="s">
-        <v>545</v>
+      <c r="E56" s="17" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6742,8 +6802,8 @@
       <c r="D57" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E57" s="12" t="s">
-        <v>509</v>
+      <c r="E57" s="17" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="11" customFormat="1">
@@ -6759,8 +6819,8 @@
       <c r="D58" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E58" s="12" t="s">
-        <v>510</v>
+      <c r="E58" s="15" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="11" customFormat="1">
@@ -6776,8 +6836,8 @@
       <c r="D59" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="12" t="s">
-        <v>511</v>
+      <c r="E59" s="15" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="11" customFormat="1" ht="57.6">
@@ -6793,8 +6853,8 @@
       <c r="D60" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E60" s="12" t="s">
-        <v>512</v>
+      <c r="E60" s="17" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="11" customFormat="1" ht="43.2">
@@ -6810,8 +6870,8 @@
       <c r="D61" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E61" s="12" t="s">
-        <v>513</v>
+      <c r="E61" s="17" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="11" customFormat="1" ht="43.2">
@@ -6827,8 +6887,8 @@
       <c r="D62" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E62" s="12" t="s">
-        <v>514</v>
+      <c r="E62" s="16" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6844,8 +6904,8 @@
       <c r="D63" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E63" s="12" t="s">
-        <v>515</v>
+      <c r="E63" s="17" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6861,8 +6921,8 @@
       <c r="D64" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E64" s="12" t="s">
-        <v>516</v>
+      <c r="E64" s="16" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="11" customFormat="1" ht="28.8">
@@ -6878,16 +6938,16 @@
       <c r="D65" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E65" s="12" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="11" customFormat="1" ht="57.6">
+      <c r="E65" s="17" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="11" customFormat="1" ht="72">
       <c r="A66" s="11" t="s">
-        <v>563</v>
+        <v>522</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>568</v>
+        <v>527</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>0</v>
@@ -6895,16 +6955,16 @@
       <c r="D66" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E66" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="11" customFormat="1" ht="57.6">
+      <c r="E66" s="16" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="11" customFormat="1" ht="72">
       <c r="A67" s="11" t="s">
-        <v>564</v>
+        <v>523</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>567</v>
+        <v>526</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>0</v>
@@ -6912,16 +6972,16 @@
       <c r="D67" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E67" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="11" customFormat="1" ht="43.2">
+      <c r="E67" s="16" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="11" customFormat="1" ht="57.6">
       <c r="A68" s="11" t="s">
-        <v>565</v>
+        <v>524</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>566</v>
+        <v>525</v>
       </c>
       <c r="C68" s="11" t="s">
         <v>0</v>
@@ -6929,8 +6989,8 @@
       <c r="D68" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E68" s="12" t="s">
-        <v>0</v>
+      <c r="E68" s="17" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="11" customFormat="1" ht="43.2">
@@ -6946,8 +7006,8 @@
       <c r="D69" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="12" t="s">
-        <v>518</v>
+      <c r="E69" s="15" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="28.8">
@@ -6963,8 +7023,8 @@
       <c r="D70" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E70" s="12" t="s">
-        <v>519</v>
+      <c r="E70" s="17" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -6980,12 +7040,12 @@
       <c r="D71" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E71" s="12" t="s">
-        <v>520</v>
+      <c r="E71" s="15" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="12" t="s">
         <v>398</v>
       </c>
       <c r="B72" s="11" t="s">
@@ -6997,8 +7057,8 @@
       <c r="D72" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E72" s="12" t="s">
-        <v>488</v>
+      <c r="E72" s="15" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -7014,8 +7074,8 @@
       <c r="D73" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E73" s="12" t="s">
-        <v>521</v>
+      <c r="E73" s="17" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -7023,7 +7083,7 @@
         <v>401</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>0</v>
@@ -7031,8 +7091,8 @@
       <c r="D74" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E74" s="12" t="s">
-        <v>522</v>
+      <c r="E74" s="15" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -7040,7 +7100,7 @@
         <v>402</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>0</v>
@@ -7048,8 +7108,8 @@
       <c r="D75" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E75" s="12" t="s">
-        <v>523</v>
+      <c r="E75" s="15" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8">
@@ -7065,8 +7125,8 @@
       <c r="D76" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E76" s="12" t="s">
-        <v>524</v>
+      <c r="E76" s="15" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8">
@@ -7082,8 +7142,8 @@
       <c r="D77" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E77" s="12" t="s">
-        <v>525</v>
+      <c r="E77" s="15" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8">
@@ -7099,8 +7159,8 @@
       <c r="D78" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E78" s="12" t="s">
-        <v>526</v>
+      <c r="E78" s="15" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="28.8">
@@ -7116,11 +7176,11 @@
       <c r="D79" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E79" s="12" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="28.8">
+      <c r="E79" s="17" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="43.2">
       <c r="A80" s="11" t="s">
         <v>412</v>
       </c>
@@ -7133,8 +7193,8 @@
       <c r="D80" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E80" s="12" t="s">
-        <v>528</v>
+      <c r="E80" s="17" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="28.8">
@@ -7150,11 +7210,11 @@
       <c r="D81" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E81" s="12" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="E81" s="17" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="28.8">
       <c r="A82" s="11" t="s">
         <v>415</v>
       </c>
@@ -7167,12 +7227,12 @@
       <c r="D82" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E82" s="12" t="s">
-        <v>530</v>
+      <c r="E82" s="17" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="12" t="s">
         <v>417</v>
       </c>
       <c r="B83" s="11" t="s">
@@ -7184,12 +7244,12 @@
       <c r="D83" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="12" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="28.8">
-      <c r="A84" s="13" t="s">
+      <c r="E83" s="17" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="43.2">
+      <c r="A84" s="12" t="s">
         <v>418</v>
       </c>
       <c r="B84" s="11" t="s">
@@ -7201,12 +7261,12 @@
       <c r="D84" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E84" s="12" t="s">
-        <v>532</v>
+      <c r="E84" s="17" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="28.8">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="12" t="s">
         <v>419</v>
       </c>
       <c r="B85" s="11" t="s">
@@ -7218,11 +7278,11 @@
       <c r="D85" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E85" s="12" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" s="11" customFormat="1" ht="28.8">
+      <c r="E85" s="17" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="11" customFormat="1" ht="43.2">
       <c r="A86" s="11" t="s">
         <v>420</v>
       </c>
@@ -7235,11 +7295,11 @@
       <c r="D86" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E86" s="12" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="11" customFormat="1" ht="28.8">
+      <c r="E86" s="17" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="11" customFormat="1" ht="43.2">
       <c r="A87" s="11" t="s">
         <v>421</v>
       </c>
@@ -7252,16 +7312,16 @@
       <c r="D87" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E87" s="12" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" s="11" customFormat="1" ht="28.8">
+      <c r="E87" s="17" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="11" customFormat="1" ht="43.2">
       <c r="A88" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>433</v>
+        <v>552</v>
       </c>
       <c r="C88" s="11" t="s">
         <v>0</v>
@@ -7269,16 +7329,16 @@
       <c r="D88" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E88" s="12" t="s">
-        <v>536</v>
+      <c r="E88" s="16" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A89" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C89" s="11" t="s">
         <v>0</v>
@@ -7286,16 +7346,16 @@
       <c r="D89" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E89" s="12" t="s">
-        <v>537</v>
+      <c r="E89" s="17" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A90" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C90" s="11" t="s">
         <v>0</v>
@@ -7303,33 +7363,33 @@
       <c r="D90" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E90" s="12" t="s">
-        <v>538</v>
+      <c r="E90" s="17" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="11" customFormat="1" ht="28.8">
       <c r="A91" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="B91" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="B91" s="11" t="s">
-        <v>439</v>
-      </c>
       <c r="C91" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D91" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E91" s="12" t="s">
-        <v>539</v>
+      <c r="E91" s="17" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>0</v>
@@ -7337,17 +7397,17 @@
       <c r="D92" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E92" s="12" t="s">
-        <v>544</v>
+      <c r="E92" s="16" t="s">
+        <v>559</v>
       </c>
       <c r="F92" s="11"/>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>0</v>
@@ -7355,14 +7415,14 @@
       <c r="D93" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E93" s="12" t="s">
-        <v>543</v>
+      <c r="E93" s="17" t="s">
+        <v>560</v>
       </c>
       <c r="F93" s="11"/>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>432</v>
@@ -7373,17 +7433,17 @@
       <c r="D94" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E94" s="12" t="s">
-        <v>542</v>
+      <c r="E94" s="16" t="s">
+        <v>561</v>
       </c>
       <c r="F94" s="11"/>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>0</v>
@@ -7391,35 +7451,35 @@
       <c r="D95" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E95" s="12" t="s">
-        <v>541</v>
+      <c r="E95" s="17" t="s">
+        <v>562</v>
       </c>
       <c r="F95" s="11"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="B96" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="B96" s="11" t="s">
-        <v>449</v>
-      </c>
       <c r="C96" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E96" s="12" t="s">
-        <v>540</v>
+      <c r="E96" s="17" t="s">
+        <v>563</v>
       </c>
       <c r="F96" s="11"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="13" t="s">
-        <v>454</v>
+      <c r="A97" s="12" t="s">
+        <v>453</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>553</v>
+        <v>514</v>
       </c>
       <c r="C97" s="11" t="s">
         <v>0</v>
@@ -7427,263 +7487,263 @@
       <c r="D97" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="12" t="s">
-        <v>554</v>
+      <c r="E97" s="15" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="B98" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="B98" s="11" t="s">
-        <v>456</v>
-      </c>
       <c r="C98" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
+      </c>
+      <c r="E98" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="B99" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="B99" s="14" t="s">
-        <v>458</v>
-      </c>
-      <c r="C99" s="14" t="s">
-        <v>458</v>
-      </c>
-      <c r="D99" s="14" t="s">
-        <v>458</v>
-      </c>
-      <c r="E99" s="14" t="s">
-        <v>458</v>
+      <c r="C99" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="D99" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="E99" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="15" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="16" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="12" t="s">
+        <v>519</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="16" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="28.8">
+      <c r="A106" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="43.2">
+      <c r="A107" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="17" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="43.2">
+      <c r="A108" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="17" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="43.2">
+      <c r="A109" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="17" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="43.2">
+      <c r="A110" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="17" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="28.8">
+      <c r="A111" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="17" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="28.8">
+      <c r="A112" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="B112" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="B100" s="13" t="s">
-        <v>551</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D100" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="15" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="13" t="s">
-        <v>548</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>552</v>
-      </c>
-      <c r="C101" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D101" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E101" s="15" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="13" t="s">
-        <v>557</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>561</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D102" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="13" t="s">
-        <v>556</v>
-      </c>
-      <c r="B103" s="13" t="s">
-        <v>555</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D103" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E103" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
-      <c r="A104" s="13" t="s">
-        <v>558</v>
-      </c>
-      <c r="B104" s="13" t="s">
-        <v>560</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D104" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E104" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="13" t="s">
-        <v>559</v>
-      </c>
-      <c r="B105" s="13" t="s">
-        <v>562</v>
-      </c>
-      <c r="C105" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D105" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E105" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="28.8">
-      <c r="A106" s="13" t="s">
-        <v>576</v>
-      </c>
-      <c r="B106" s="11" t="s">
-        <v>577</v>
-      </c>
-      <c r="C106" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D106" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="28.8">
-      <c r="A107" s="13" t="s">
-        <v>579</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>583</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D107" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="28.8">
-      <c r="A108" s="13" t="s">
-        <v>582</v>
-      </c>
-      <c r="B108" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="C108" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D108" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="28.8">
-      <c r="A109" s="13" t="s">
-        <v>580</v>
-      </c>
-      <c r="B109" s="11" t="s">
-        <v>584</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D109" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="28.8">
-      <c r="A110" s="13" t="s">
-        <v>581</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>585</v>
-      </c>
-      <c r="C110" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D110" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="28.8">
-      <c r="A111" s="13" t="s">
-        <v>586</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>589</v>
-      </c>
-      <c r="C111" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E111" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="28.8">
-      <c r="A112" s="13" t="s">
-        <v>587</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>588</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D112" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="13" t="s">
-        <v>0</v>
+      <c r="C112" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 7 scenarios for nicosia
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="872">
   <si>
     <t>XXXX</t>
   </si>
@@ -2756,12 +2756,315 @@
   <si>
     <t>Despite the police patrol boat only has rescued two fishermen, the rest of the drowned fishermen are rescued by the pleasure boats</t>
   </si>
+  <si>
+    <t>SCENARIO_1_INDEX_8</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_9</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_10</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_11</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_12</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_INDEX_13</t>
+  </si>
+  <si>
+    <t>SCENARIO_4_INDEX_8</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_INDEX_12</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_INDEX_9</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_8</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_9</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_10</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_11</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_INDEX_12</t>
+  </si>
+  <si>
+    <t>A neighbor complains about noise from nearby house</t>
+  </si>
+  <si>
+    <t>A neighbor's dog is barking</t>
+  </si>
+  <si>
+    <t>As a result of the fight a woman is screaming out of her lungs to her husband regarding a difference they had related to their child.</t>
+  </si>
+  <si>
+    <t>A citizen reports that a kid is heard crying produsely from the back side of the house looking through the slightly open door</t>
+  </si>
+  <si>
+    <t>As soon as the parents realise the absense of the kid they decide to file a report through the INSPEC2T app.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The woman rushes out of the house gets in the car and starts looking for the kid; she is in panic mode and drives recklessly. As a result she hits an electricity pillar</t>
+  </si>
+  <si>
+    <t>The police surrounds the area to avoid any chances of electrocution or the generation of fire</t>
+  </si>
+  <si>
+    <t>returned to the nearby police station</t>
+  </si>
+  <si>
+    <t>The officer visited the reported location and resolved the issue. A couple was arguing in the precense of a 9 yr old kid. None of the parents wanted to file the incident.</t>
+  </si>
+  <si>
+    <t>The officer visited the reported location and resolved the issue. A couple was arguing in the precense of a 9 yr old kid. However the officer needed to transfer the child to the social services and ensure that everything is ok</t>
+  </si>
+  <si>
+    <t>Officers find the kid and they immediately contact hs parents</t>
+  </si>
+  <si>
+    <t>The situation escalated with no reason. The woman was saved by miracle and the boy was found by citizens</t>
+  </si>
+  <si>
+    <t>The situation escalated with no reason. The woman was saved by miracle and the boy was found by officers</t>
+  </si>
+  <si>
+    <t>A citizen reported littering in around his neighbourhood. His newly moved neighbors do not seem to respect others' space</t>
+  </si>
+  <si>
+    <t>The citizen's trust in police is decreased</t>
+  </si>
+  <si>
+    <t>A citizen reported littering in around his neighbourhood for the second time</t>
+  </si>
+  <si>
+    <t>The two neighbours are involved in an argument</t>
+  </si>
+  <si>
+    <t>The argument escalated on a fight which required the intervention of the police.  The two neighbours seem to be unfriendly with each other with the issue between them still unresolved</t>
+  </si>
+  <si>
+    <t>A police officer resolves the issue and the two neighbours restored their trust in police and managed to build a strong relationship</t>
+  </si>
+  <si>
+    <t>A citizen reported that her dog got sick after their walk around the neighbourhood and claimed the existence of pet poison around the area</t>
+  </si>
+  <si>
+    <t>Multiple citizens reported the existense of pet poison through the use of the INSPEC2T app. Some of them also associated the event with a number of locations. Thanks to the spatiotemporal processing in INSPEC2T. The system suggested the correlation of some reports and provided an estimation of the location.</t>
+  </si>
+  <si>
+    <t>Thanks to system indications and the contribution of citizens the officer managed to find and remove the poison within the area</t>
+  </si>
+  <si>
+    <t>The officers spent a long time on this but it paid off. They have managed to identify the poison and cleared the area.</t>
+  </si>
+  <si>
+    <t>Broadcasted a message to the area and urged anyone knowing anything about the event to contact the police or file a report. The case is not closed until the perpetrator is found</t>
+  </si>
+  <si>
+    <t>Multiple citizens provided key information to the police about a person that seems to be responsible for putting the poison to the area</t>
+  </si>
+  <si>
+    <t>The suspect is being arrested and is sent for questioning</t>
+  </si>
+  <si>
+    <t>The public seems to be losing trust in the police. They feel that the system does not work and get discouraged in providing input in the future</t>
+  </si>
+  <si>
+    <t>Report from user George names a suspect and reports multiple harassment events and damages on his asstes</t>
+  </si>
+  <si>
+    <t>George who has previously filed a report called a suspect messing with his parck car. George comes in arguments outside his hhouse and a neighbour files an anonymous report</t>
+  </si>
+  <si>
+    <t>The two officers managed to trace down the suspect who declines allegations.</t>
+  </si>
+  <si>
+    <t>Ignoring the case resulted in the generation of even more aggressive hostile reaction on behalf of the two parties</t>
+  </si>
+  <si>
+    <t>The citizens provide valuable information to the police, such information has helped to resolve the issue</t>
+  </si>
+  <si>
+    <t>Affter a lot of effort the officers managed to calm down the situation and suggested the intervention of consulting for resolving their issues</t>
+  </si>
+  <si>
+    <t>Progress on the investigation revealed that George and the reported suspect have a long run of financial differences. The police suggests the invasion of lawyers for resolving the issue</t>
+  </si>
+  <si>
+    <t>A report from a user states race discrimination in employment. Their employer does not treat them equally</t>
+  </si>
+  <si>
+    <t>The reporter is in the process of forming an awareness campaign against their employer, clearly stating the ignorance of police,. Dedicate some forces to minimise the dissatisfaction</t>
+  </si>
+  <si>
+    <t>The officer approached the employer and the apporpriate public body and explained the policies behind equal rights. You are now presented with an option to find the employer</t>
+  </si>
+  <si>
+    <t>You ignored the case and the public lost their trust in you. They believe that these things should matter</t>
+  </si>
+  <si>
+    <t>Your officer tried to exploain the restrictions of police when it comes to their resources but it wasn't enough</t>
+  </si>
+  <si>
+    <t>Your actions weren't transparent to the public and the victim dim not come to closure</t>
+  </si>
+  <si>
+    <t>You have broadcasted messages through the INSPEC2T Platform and social media stating that such behaviours are not acceptable and should not be tolerated. The offender however has left unpunished</t>
+  </si>
+  <si>
+    <t>You have fined the employer and broadcasted messages through the INSPEC2T platform and the social media stating that such behaviours are not acceptable and should not be tolerated</t>
+  </si>
+  <si>
+    <t>A report has been received from a hotel manager stating that a suspicious substance has been found in a room</t>
+  </si>
+  <si>
+    <t>Your officers have visited the hotel, carefully collected the substance which was sent to the appropriate lab which confirmed the existence of large amounts of drugs. The room tenant has gone missing</t>
+  </si>
+  <si>
+    <t>You have requested citizens contribution. Through which you managed to get valuable information. allowing you to trace down the suspec's location</t>
+  </si>
+  <si>
+    <t>The room tenant returns to the room after the police has departed from the area. The hotel manager was assaulted while damages were caused in the reception area. The manager ended up in the nearest hospital with a serious concussion</t>
+  </si>
+  <si>
+    <t>The officer managed to trace down the suspect after organised efforts he was apprehended and was sent to questioning. The hotel manager is satisfied and the citizens' trust in the police has increased due to transparency</t>
+  </si>
+  <si>
+    <t>The officers manage to trace down the suspect and after organised efforts he was apprehended and was sent to questioning. The hotel manager is satisfied</t>
+  </si>
+  <si>
+    <t>A report has been received from a third country national anonymous user indicating that they are mistreated by their employer being forced to work too many hours every week</t>
+  </si>
+  <si>
+    <t>You have chosen not to take active action at this time but took the time to raise some awareness of the matter</t>
+  </si>
+  <si>
+    <t>An officer investigates the situation and finds out that the employer hires the victim's services to their relatives</t>
+  </si>
+  <si>
+    <t>Working together with public services resulted in finding a new home for the victim and filing charges to the offender. The extra time you have taken did not cause any significant consequences</t>
+  </si>
+  <si>
+    <t>You decided to ignore the case. The victim could not find an escape and ran away from their home. A person has now gone missing and the initial issue is still pending</t>
+  </si>
+  <si>
+    <t>Working together with public services resulted in finding a new home for the victim and filing charges to the offender.</t>
+  </si>
+  <si>
+    <t>Intelligence coming from citizens reports that the reporting victim was found on the streets in apretty bad shape. The public opinion in negative and does not support your actions</t>
+  </si>
+  <si>
+    <t>Your officers did not manage to solve the issues. The issues are still pending. You can either dedicate more forces and solve the matters or ask for citizen intelligence</t>
+  </si>
+  <si>
+    <t>The public returns valuable information that results in tracing down the missing person. It is now time to deal with the offender</t>
+  </si>
+  <si>
+    <t>Your officers managed to apprehend the offending employer and are in search of the missing person</t>
+  </si>
+  <si>
+    <t>You decided to ignore the case. Th public opinion is negative and does not support your actions</t>
+  </si>
+  <si>
+    <t>Your officers managed to apprehend the offending employer. Well done, you have managed to dela with the situation in resonable time</t>
+  </si>
+  <si>
+    <t>A report has been received from a registered citizen indicating that a car on Griva Digeni Ave. has just caught on fire. The fire department has already been called and dispatched resources</t>
+  </si>
+  <si>
+    <t>You selected to ignore the case. You are putting citizens in danger</t>
+  </si>
+  <si>
+    <t>Messages have been broadcasted to the citizens with information about the event. Take some security measures or wait to close the case</t>
+  </si>
+  <si>
+    <t>Two officers were sent to ensure public safety during the process. The police officers capture images from the site. Dedicate some resources to ensure the area is secure for use by the public</t>
+  </si>
+  <si>
+    <t>The case is now closed. You have left the area unsecured through and citizens are in danger</t>
+  </si>
+  <si>
+    <t>Messages have been broadcasted to the citizens with diverting instructions and pictoral content for avoiding any accidents. You have left the area unsecured though</t>
+  </si>
+  <si>
+    <t>The area is now open for use by the public. You are now faced with the choice to inform the publice about the event or close the case</t>
+  </si>
+  <si>
+    <t>The case is successfully closed. You have taken the right precautions. Well Done</t>
+  </si>
+  <si>
+    <t>Messages have been broadcasted to the citizens for their information. You are gaining their trust</t>
+  </si>
+  <si>
+    <t>A suspicious person is seen inside a green van outside a pharmacy in the middle of the night. The filed report contains the van's number plate</t>
+  </si>
+  <si>
+    <t>A robbery has been reported. The alarm of the pharmacy was activated. The pharmacist who was resting at the back of the room is wounded. A quantity of drugs have gone missing</t>
+  </si>
+  <si>
+    <t>Gathered citizen intelligence! Citizens confirm that there is indeed an unknown and suspicious person in the area. They even mention that this person was previously seen with 2 other parties</t>
+  </si>
+  <si>
+    <t>The officer went to the area. The suspicious person pretended to be busy on their phone. The officer approached the suspect who claimed that he parker there to speak on the phone and he immediately drove away</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Citizens point the direction of suspects. Along with vehicle number plates. The number plates match the initial report</t>
+  </si>
+  <si>
+    <t>The officers investigate the area and gather evidence. The investigation of the crime is forwarded to the appropriate department</t>
+  </si>
+  <si>
+    <t>You check the van's number plate and find out that they do not belong to that vehicle.</t>
+  </si>
+  <si>
+    <t>The suspect was apprehended and was sent for questioning. Well done</t>
+  </si>
+  <si>
+    <t>The suspect was arrested and it was proved that he was involved in a planned robbery. Good Job!</t>
+  </si>
+  <si>
+    <t>A report mentions that a car is left on the side of a field a few days now. parked in a messy way. They also provide the number plates.</t>
+  </si>
+  <si>
+    <t>You decided to do nothing on the matter. No major backlash is caused but you certainly did not satisfy the reporter and victim's immediate community</t>
+  </si>
+  <si>
+    <t>The number plates point to the owner who was contacted and mentioned that his daughter, who is studying in a nearby city, drives the car. The concerned parent mentions that his daughter suffers from memory problems</t>
+  </si>
+  <si>
+    <t>You decided to ask more information from citizens on the abandoned car. Citizens managed to provide you with some useful information</t>
+  </si>
+  <si>
+    <t>An officer visited the abandoned car and gathered some evidence They also managed to trace down the girl. Who mentioned that a few days ago she went to a party and on the way back she lost her orientation and forgot where she left her car</t>
+  </si>
+  <si>
+    <t>Great Job! You managed to solve the problem</t>
+  </si>
+  <si>
+    <t>Thank the citizen for their participation in bringing the matter to the plice's attention</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2823,6 +3126,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri  "/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2874,7 +3188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2959,6 +3273,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4729,7 +5064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -5635,19 +5970,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="49.1328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62.9296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="48.46484375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.9296875" style="30" customWidth="1"/>
+    <col min="3" max="3" width="10.86328125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
@@ -5655,33 +5990,33 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1">
+    <row r="2" spans="1:6" s="30" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="B2" s="31" t="s">
+        <v>786</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="35" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5689,30 +6024,30 @@
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B4" s="31" t="s">
+        <v>788</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -5723,218 +6058,218 @@
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B5" s="31" t="s">
+        <v>789</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="28.5">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B6" s="32" t="s">
+        <v>790</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B7" s="31" t="s">
+        <v>791</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6" ht="25.5">
       <c r="A8" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B8" s="31" t="s">
+        <v>792</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>793</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="38.25">
+      <c r="A10" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>794</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="38.25">
+      <c r="A11" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>796</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5">
+      <c r="A13" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5">
+      <c r="A14" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>798</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25.5">
+      <c r="A15" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="26.25">
-      <c r="A10" s="1" t="s">
+      <c r="B15" s="33" t="s">
+        <v>799</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="26.25">
-      <c r="A11" s="1" t="s">
+      <c r="B16" s="33" t="s">
+        <v>800</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="26.25">
-      <c r="A12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="26.25">
-      <c r="A14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="26.25">
-      <c r="A15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" ht="25.5">
-      <c r="A16" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="26.25">
-      <c r="A17" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="B17" s="33" t="s">
+        <v>801</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -5943,287 +6278,287 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>802</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="38.25">
+      <c r="A19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>803</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="25.5">
+      <c r="A20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>804</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="25.5">
+      <c r="A21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>805</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="63.75">
+      <c r="A22" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>806</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="25.5">
+      <c r="A23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="27.75">
-      <c r="A19" s="1" t="s">
+      <c r="B23" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="25.5">
+      <c r="A24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="26.25">
-      <c r="A20" s="1" t="s">
+      <c r="B24" s="31" t="s">
+        <v>808</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="38.25">
+      <c r="A25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="25.5">
-      <c r="A21" s="1" t="s">
+      <c r="B25" s="31" t="s">
+        <v>809</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="25.5">
+      <c r="A26" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="39">
-      <c r="A22" s="1" t="s">
+      <c r="B26" s="31" t="s">
+        <v>810</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="26.25">
-      <c r="A23" s="1" t="s">
+      <c r="B27" s="31" t="s">
+        <v>811</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="25.5">
+      <c r="A28" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="26.25">
-      <c r="A24" s="3" t="s">
+      <c r="B28" s="31" t="s">
+        <v>812</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25.5">
+      <c r="A29" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="26.25">
-      <c r="A25" s="1" t="s">
+      <c r="B29" s="34" t="s">
+        <v>813</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="38.25">
+      <c r="A30" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="26.25">
-      <c r="A26" s="1" t="s">
+      <c r="B30" s="34" t="s">
+        <v>814</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="25.5">
+      <c r="A31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="26.25">
-      <c r="A27" s="1" t="s">
+      <c r="B31" s="34" t="s">
+        <v>815</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="25.5">
+      <c r="A32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="39">
-      <c r="A28" s="1" t="s">
+      <c r="B32" s="34" t="s">
+        <v>815</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="25.5">
+      <c r="A33" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
+      <c r="B33" s="34" t="s">
+        <v>816</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="25.5">
+      <c r="A34" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="26.25">
-      <c r="A30" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="3" customFormat="1">
-      <c r="A31" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="27.75">
-      <c r="A34" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="B34" s="34" t="s">
+        <v>817</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -6232,307 +6567,970 @@
     </row>
     <row r="35" spans="1:5" ht="25.5">
       <c r="A35" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>818</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="38.25">
+      <c r="A36" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>819</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="25.5">
+      <c r="A37" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>820</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="38.25">
+      <c r="A38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>821</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="38.25">
+      <c r="A39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>822</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="25.5">
+      <c r="A40" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>823</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="25.5">
+      <c r="A41" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="25.5">
-      <c r="A36" s="1" t="s">
+      <c r="B41" s="34" t="s">
+        <v>824</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="25.5">
+      <c r="A42" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="26.25">
-      <c r="A37" s="1" t="s">
+      <c r="B42" s="34" t="s">
+        <v>825</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="38.25">
+      <c r="A43" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="25.5">
-      <c r="A38" s="1" t="s">
+      <c r="B43" s="34" t="s">
+        <v>826</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="38.25">
+      <c r="A44" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="26.25">
-      <c r="A39" s="3" t="s">
+      <c r="B44" s="34" t="s">
+        <v>827</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="25.5">
+      <c r="A45" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="26.25">
-      <c r="A40" s="1" t="s">
+      <c r="B45" s="34" t="s">
+        <v>828</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25.5">
+      <c r="A46" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>828</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="38.25">
+      <c r="A47" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15">
-      <c r="A41" s="1" t="s">
+      <c r="B47" s="34" t="s">
+        <v>829</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="25.5">
+      <c r="A48" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="26.25">
-      <c r="A42" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="26.25">
-      <c r="A43" s="1" t="s">
+      <c r="B48" s="34" t="s">
+        <v>830</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="51">
+      <c r="A49" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="39">
-      <c r="A44" s="1" t="s">
+      <c r="B49" s="34" t="s">
+        <v>831</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="51">
+      <c r="A50" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" ht="26.25">
-      <c r="A45" s="3" t="s">
+      <c r="B50" s="34" t="s">
+        <v>832</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="38.25">
+      <c r="A51" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>833</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="38.25">
+      <c r="A52" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="s">
+      <c r="B52" s="34" t="s">
+        <v>834</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="25.5">
+      <c r="A53" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1" t="s">
+      <c r="B53" s="34" t="s">
+        <v>835</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="25.5">
+      <c r="A54" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="26.25">
-      <c r="A48" s="1" t="s">
+      <c r="B54" s="34" t="s">
+        <v>836</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="38.25">
+      <c r="A55" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="53.25">
-      <c r="A49" s="1" t="s">
+      <c r="B55" s="34" t="s">
+        <v>837</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="38.25">
+      <c r="A56" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="26.25">
-      <c r="A50" s="1" t="s">
+      <c r="B56" s="34" t="s">
+        <v>838</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="25.5">
+      <c r="A57" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="26.25">
-      <c r="A51" s="1" t="s">
+      <c r="B57" s="34" t="s">
+        <v>839</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="38.25">
+      <c r="A58" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="s">
+      <c r="B58" s="34" t="s">
+        <v>840</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="38.25">
+      <c r="A59" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="10" t="s">
+      <c r="B59" s="34" t="s">
+        <v>841</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="25.5">
+      <c r="A60" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>842</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="25.5">
+      <c r="A61" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>843</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="25.5">
+      <c r="A62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>844</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="25.5">
+      <c r="A63" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>845</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="38.25">
+      <c r="A64" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>846</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>847</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="25.5">
+      <c r="A66" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>848</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="38.25">
+      <c r="A67" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>849</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="25.5">
+      <c r="A68" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>850</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="38.25">
+      <c r="A69" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>851</v>
+      </c>
+      <c r="C69" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="25.5">
+      <c r="A70" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>852</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="25.5">
+      <c r="A71" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B71" s="34" t="s">
+        <v>853</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="25.5">
+      <c r="A72" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B72" s="34" t="s">
+        <v>854</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="25.5">
+      <c r="A73" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B73" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="C73" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="38.25">
+      <c r="A74" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B74" s="34" t="s">
+        <v>856</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="38.25">
+      <c r="A75" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B75" s="34" t="s">
+        <v>857</v>
+      </c>
+      <c r="C75" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="38.25">
+      <c r="A76" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B76" s="34" t="s">
+        <v>858</v>
+      </c>
+      <c r="C76" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="34" t="s">
+        <v>859</v>
+      </c>
+      <c r="C77" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="25.5">
+      <c r="A78" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B78" s="34" t="s">
+        <v>860</v>
+      </c>
+      <c r="C78" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="25.5">
+      <c r="A79" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B79" s="34" t="s">
+        <v>861</v>
+      </c>
+      <c r="C79" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="25.5">
+      <c r="A80" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>862</v>
+      </c>
+      <c r="C80" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>859</v>
+      </c>
+      <c r="C81" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>863</v>
+      </c>
+      <c r="C82" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B83" s="34" t="s">
+        <v>859</v>
+      </c>
+      <c r="C83" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="25.5">
+      <c r="A84" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B84" s="34" t="s">
+        <v>864</v>
+      </c>
+      <c r="C84" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="25.5">
+      <c r="A85" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B85" s="34" t="s">
+        <v>865</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="25.5">
+      <c r="A86" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B86" s="34" t="s">
+        <v>866</v>
+      </c>
+      <c r="C86" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="38.25">
+      <c r="A87" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>867</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="25.5">
+      <c r="A88" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B88" s="34" t="s">
+        <v>868</v>
+      </c>
+      <c r="C88" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="51">
+      <c r="A89" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B89" s="34" t="s">
+        <v>869</v>
+      </c>
+      <c r="C89" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B90" s="34" t="s">
+        <v>870</v>
+      </c>
+      <c r="C90" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="25.5">
+      <c r="A91" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B91" s="34" t="s">
+        <v>871</v>
+      </c>
+      <c r="C91" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="10" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8479,7 +9477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -8859,7 +9857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove quit to menu button on pause when in menu and adda ability to replay tutorial
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2555" uniqueCount="874">
   <si>
     <t>XXXX</t>
   </si>
@@ -3058,6 +3058,12 @@
   </si>
   <si>
     <t>Thank the citizen for their participation in bringing the matter to the plice's attention</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_REPLAY_TUTORIAL</t>
+  </si>
+  <si>
+    <t>Replay Tutorial</t>
   </si>
 </sst>
 </file>
@@ -5972,7 +5978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -7542,10 +7548,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -9213,62 +9219,62 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="11" t="s">
-        <v>454</v>
+      <c r="A98" s="12" t="s">
+        <v>872</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>455</v>
+        <v>873</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>455</v>
+        <v>0</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="E98" t="s">
-        <v>455</v>
+        <v>0</v>
+      </c>
+      <c r="E98" s="15" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="E99" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="B99" s="13" t="s">
+      <c r="B100" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="C99" s="13" t="s">
+      <c r="C100" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="D99" s="13" t="s">
+      <c r="D100" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>457</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="12" t="s">
-        <v>509</v>
-      </c>
-      <c r="B100" s="12" t="s">
-        <v>512</v>
-      </c>
-      <c r="C100" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D100" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="17" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>0</v>
@@ -9276,16 +9282,16 @@
       <c r="D101" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E101" s="15" t="s">
-        <v>511</v>
+      <c r="E101" s="17" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="12" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>554</v>
+        <v>513</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>0</v>
@@ -9293,16 +9299,16 @@
       <c r="D102" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E102" s="16" t="s">
-        <v>597</v>
+      <c r="E102" s="15" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="12" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>0</v>
@@ -9311,15 +9317,15 @@
         <v>0</v>
       </c>
       <c r="E103" s="16" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>520</v>
+        <v>553</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>0</v>
@@ -9327,67 +9333,67 @@
       <c r="D104" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E104" s="17" t="s">
-        <v>599</v>
+      <c r="E104" s="16" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="12" t="s">
         <v>519</v>
       </c>
-      <c r="B105" s="12" t="s">
+      <c r="B106" s="12" t="s">
         <v>521</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E105" s="16" t="s">
+      <c r="C106" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="16" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="28.5">
-      <c r="A106" s="12" t="s">
+    <row r="107" spans="1:5" ht="28.5">
+      <c r="A107" s="12" t="s">
         <v>535</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="B107" s="11" t="s">
         <v>536</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D106" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="16" t="s">
+      <c r="C107" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="16" t="s">
         <v>601</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="42.75">
-      <c r="A107" s="12" t="s">
-        <v>538</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>542</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D107" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E107" s="17" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="42.75">
       <c r="A108" s="12" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>0</v>
@@ -9396,15 +9402,15 @@
         <v>0</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="42.75">
       <c r="A109" s="12" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>0</v>
@@ -9413,57 +9419,74 @@
         <v>0</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="42.75">
       <c r="A110" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="17" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="42.75">
+      <c r="A111" s="12" t="s">
         <v>540</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="B111" s="11" t="s">
         <v>544</v>
       </c>
-      <c r="C110" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="17" t="s">
+      <c r="C111" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="17" t="s">
         <v>605</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="28.5">
-      <c r="A111" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>548</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E111" s="17" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="28.5">
       <c r="A112" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="17" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="28.5">
+      <c r="A113" s="12" t="s">
         <v>546</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="B113" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="C112" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="16" t="s">
+      <c r="C113" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E113" s="16" t="s">
         <v>607</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add structure for localised feedback strings
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -8457,8 +8457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F144"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -10922,6 +10922,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10930,7 +10931,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A114" sqref="A114:XFD114"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add remaining preston scenarios and change check for if there is feedback rating rather than using the text as we are now changing the text to be localized
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3440" uniqueCount="1250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3805" uniqueCount="1316">
   <si>
     <t>XXXX</t>
   </si>
@@ -4478,6 +4478,204 @@
   </si>
   <si>
     <t>Sending officers will help to resolve the missing girl issue but will also improve relations with community members</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_INDEX_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_INDEX_8</t>
+  </si>
+  <si>
+    <t>Report of a drunken male causing problems inside a hotel foyer</t>
+  </si>
+  <si>
+    <t>Male soils himself and becomes abusive towards staff</t>
+  </si>
+  <si>
+    <t>Male identified as known individual who has caused similar problems</t>
+  </si>
+  <si>
+    <t>Male Removed from the premises without issue and returned to partner agencies to address long term issue</t>
+  </si>
+  <si>
+    <t>Male eventually arrested and prosecuted for public order</t>
+  </si>
+  <si>
+    <t>Male becomes violent towards staff and assualts one of them</t>
+  </si>
+  <si>
+    <t>Male arrested and charged with pulblic order &amp; section 39 assault</t>
+  </si>
+  <si>
+    <t>Male makes off due to lack of response and unable to progress further as there is no CCTV</t>
+  </si>
+  <si>
+    <t>A report has been received regarding a small child who has been separated from their mother in a busy city centre shop</t>
+  </si>
+  <si>
+    <t>Officers begin searching the city centre shops for a child</t>
+  </si>
+  <si>
+    <t>Child is hit by a bus trying to cross a busy road</t>
+  </si>
+  <si>
+    <t>Picture of the child was circulated on the INSPEC2T platform and as such, the child was found nearby a shop. Mother and Child have been reunited</t>
+  </si>
+  <si>
+    <t>After much time used by your officers, mother and child have been reunited</t>
+  </si>
+  <si>
+    <t>Report received regarding a large amount of musical noise coming from a neighbouring property. The informant says to the call taker that if the police doesn't sort it, they'll do it themselves</t>
+  </si>
+  <si>
+    <t>Officers attend and ask the problematic property to turn the music down</t>
+  </si>
+  <si>
+    <t>Due to the delay in responding, the informant goes to the problematic address and confronts the occupants, which results in the informant getting assaulted</t>
+  </si>
+  <si>
+    <t>Offender arrested for assault and noise has been turned down</t>
+  </si>
+  <si>
+    <t>Informant reacts to the assault and smashes a window due to frustration of having to wait</t>
+  </si>
+  <si>
+    <t>Numerous officers deployed resulting in 2 arrests being made and music being turned down</t>
+  </si>
+  <si>
+    <t>Due to lack of deployment a serious assault occurs due to increasing tensions</t>
+  </si>
+  <si>
+    <t>Report of a group of youths causing havoc on a small residential estate. The report can only describe the youths as "the usual ones"</t>
+  </si>
+  <si>
+    <t>On arrival, the youths who have their faces concealed, run away.</t>
+  </si>
+  <si>
+    <t>Issue subsides without police intervention. The community are very unhappy with the lack of response and no long term solution</t>
+  </si>
+  <si>
+    <t>Information provided from a neighbour gives the identity of several of the youths</t>
+  </si>
+  <si>
+    <t>Officer deals with incident and is able to provide high quality evidence toward court orders to prevent future issues</t>
+  </si>
+  <si>
+    <t>Issues subside without police intervention, the community are unhappy but with help from citizens some evidence came forward and court orders are obtained</t>
+  </si>
+  <si>
+    <t>Report regarding concerns for the welfare of a family member who is elderly and lives on their own and not answering the telephone. Informant lives in another part of the country and is unable to visit them</t>
+  </si>
+  <si>
+    <t>Officer discovers elderly person has fallen inside the property and cannot get up but requires assistance in gaining entry to help them</t>
+  </si>
+  <si>
+    <t>Due to lack of deployment the elderly person has had to be admitted to hospital for a fall in the house. The community are not happy with this outcome</t>
+  </si>
+  <si>
+    <t>Request locates a close friend that the informant is not aware of. The friend confirms that the elderly family member is safe and well but has broken their phone.</t>
+  </si>
+  <si>
+    <t>Patrols gain entry and help the elderly person get medical assistance.</t>
+  </si>
+  <si>
+    <t>The condition of the elderly person deteriorates and requires considerably more medical assistance</t>
+  </si>
+  <si>
+    <t>Report received that there are a group of males fighting outside a shop on a residential estate with weapons. The informant is unable to provide any ID or further information on the weapons as they're driving past</t>
+  </si>
+  <si>
+    <t>Officers attend and makes several arrests and the community are satisfied, however, as specifics regarding which weapons were being used an officer is hurt</t>
+  </si>
+  <si>
+    <t>Citizen gives names of males involved and provides specifics of weapons being used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to lack of deployment, one of the males fighting is critically injured, resulting in community outrage </t>
+  </si>
+  <si>
+    <t>Officers deal with the incident by making several arrests without any significant harm to officers or the public</t>
+  </si>
+  <si>
+    <t>Report received regarding a transit van driving recklessly and at high speeds around a residential area. There is significant concern as a local primary school is due to finish for the day and pupils will be walking home</t>
+  </si>
+  <si>
+    <t>Due to lack of deployment the behaviour of the driver becomes more reckless, serveral other calls are received which provide direction of travel</t>
+  </si>
+  <si>
+    <t>Information is gathered about the travel direction and number plate of the vehicle</t>
+  </si>
+  <si>
+    <t>A vehicle matching the description is found abandoned nearby. However without a registration it's not possible to confirm that this is the vehicle.</t>
+  </si>
+  <si>
+    <t>Vehicle is involved in a high speed collision with a child crossing the road</t>
+  </si>
+  <si>
+    <t>Vehicle stopped near home address. Driver is found to be under the infulence of alcohol and arrested.</t>
+  </si>
+  <si>
+    <t>Patrols deal with collision, it comes to light that the friver is under the influence of alcohol is arrested. The chile receives meddical assistance</t>
+  </si>
+  <si>
+    <t>Driver does not wait and drives off, focusing on the wellbeing of the child, nobody takes note of the registration of the vehicle, no further action can be taken</t>
+  </si>
+  <si>
+    <t>Report received that there is a dangerous dog out of control in a local park. Nearby there is a play area which is currently very busy</t>
+  </si>
+  <si>
+    <t>Due to the delay in finding the dog, a further report in made that a dog has bitten a small child in the play area and ran away</t>
+  </si>
+  <si>
+    <t>Information provided on the location of the dog and the person who is believed to be the owner</t>
+  </si>
+  <si>
+    <t>No one is able to provide any information regarding the dog or its owner.</t>
+  </si>
+  <si>
+    <t>Park is searched but no one is able to provide any more information regarding the dog or its owner, and so, is not located</t>
+  </si>
+  <si>
+    <t>Park is searched, but the dog is not found, however, due to the owner information being known, officers go to the address and advise owner on controlling their dog in the future</t>
+  </si>
+  <si>
+    <t>Disruption</t>
+  </si>
+  <si>
+    <t>Search Started</t>
+  </si>
+  <si>
+    <t>Noise Complaint</t>
+  </si>
+  <si>
+    <t>Property Damage</t>
+  </si>
+  <si>
+    <t>Concern Raised</t>
+  </si>
+  <si>
+    <t>Assistance Required</t>
+  </si>
+  <si>
+    <t>Armed Assault</t>
+  </si>
+  <si>
+    <t>Reckless Driving</t>
+  </si>
+  <si>
+    <t>Information Gathered</t>
+  </si>
+  <si>
+    <t>Collision</t>
+  </si>
+  <si>
+    <t>Dangerous Dog</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_TITLE_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_TITLE_5</t>
   </si>
 </sst>
 </file>
@@ -5033,10 +5231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -6512,733 +6710,1974 @@
       </c>
     </row>
     <row r="87" spans="1:5" s="3" customFormat="1">
-      <c r="A87" s="35" t="s">
+      <c r="A87" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B88" s="20" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="25.5">
+      <c r="A90" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B90" s="20" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B91" s="20" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B92" s="20" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="25.5">
+      <c r="A94" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="3" customFormat="1" ht="25.5">
+      <c r="A95" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B96" s="20" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="25.5">
+      <c r="A98" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="3" customFormat="1" ht="38.25">
+      <c r="A100" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="38.25">
+      <c r="A102" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="25.5">
+      <c r="A104" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="25.5">
+      <c r="A105" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="25.5">
+      <c r="A106" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B106" s="20" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="3" customFormat="1" ht="25.5">
+      <c r="A107" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="25.5">
+      <c r="A109" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="25.5">
+      <c r="A110" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="25.5">
+      <c r="A111" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B111" s="20" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="38.25">
+      <c r="A112" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="B112" s="20" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="3" customFormat="1" ht="38.25">
+      <c r="A113" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="25.5">
+      <c r="A114" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="38.25">
+      <c r="A115" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="38.25">
+      <c r="A116" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B117" s="20" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="25.5">
+      <c r="A118" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B118" s="20" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" s="3" customFormat="1" ht="38.25">
+      <c r="A119" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="38.25">
+      <c r="A120" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B120" s="20" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="25.5">
+      <c r="A121" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B121" s="20" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="25.5">
+      <c r="A122" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="B122" s="20" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="25.5">
+      <c r="A123" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B123" s="20" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="3" customFormat="1" ht="38.25">
+      <c r="A124" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="B124" s="20" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="25.5">
+      <c r="A125" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B125" s="20" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="25.5">
+      <c r="A126" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="B126" s="20" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="25.5">
+      <c r="A127" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B127" s="20" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="B128" s="20" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="25.5">
+      <c r="A129" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B129" s="20" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="25.5">
+      <c r="A130" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B130" s="20" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="38.25">
+      <c r="A131" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B131" s="20" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="3" customFormat="1" ht="25.5">
+      <c r="A132" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="B132" s="20" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="25.5">
+      <c r="A133" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B133" s="20" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="25.5">
+      <c r="A134" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B134" s="20" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B135" s="20" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="25.5">
+      <c r="A136" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B136" s="20" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="38.25">
+      <c r="A137" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B137" s="20" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" s="3" customFormat="1">
+      <c r="A138" s="35" t="s">
         <v>1038</v>
       </c>
-      <c r="B87" s="35" t="s">
+      <c r="B138" s="35" t="s">
         <v>1172</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="20" t="s">
+      <c r="C138" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="20" t="s">
         <v>1040</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B139" s="20" t="s">
         <v>1173</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="20" t="s">
+      <c r="C139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="20" t="s">
         <v>1041</v>
       </c>
-      <c r="B89" s="20" t="s">
+      <c r="B140" s="20" t="s">
         <v>1174</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="3" customFormat="1">
-      <c r="A90" s="35" t="s">
+      <c r="C140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" s="3" customFormat="1">
+      <c r="A141" s="35" t="s">
         <v>1043</v>
       </c>
-      <c r="B90" s="35" t="s">
+      <c r="B141" s="35" t="s">
         <v>1175</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="20" t="s">
+      <c r="C141" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="20" t="s">
         <v>1044</v>
       </c>
-      <c r="B91" s="20" t="s">
+      <c r="B142" s="20" t="s">
         <v>1176</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="20" t="s">
+      <c r="C142" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="20" t="s">
         <v>1045</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="B143" s="20" t="s">
         <v>1177</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="20" t="s">
+      <c r="C143" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="20" t="s">
         <v>1046</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="B144" s="20" t="s">
         <v>1177</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="20" t="s">
+      <c r="C144" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="20" t="s">
         <v>1153</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B145" s="20" t="s">
         <v>1174</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="20" t="s">
+      <c r="C145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="20" t="s">
         <v>1154</v>
       </c>
-      <c r="B95" s="20" t="s">
+      <c r="B146" s="20" t="s">
         <v>1174</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="3" customFormat="1">
-      <c r="A96" s="35" t="s">
+      <c r="C146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" s="3" customFormat="1">
+      <c r="A147" s="35" t="s">
         <v>1047</v>
       </c>
-      <c r="B96" s="35" t="s">
+      <c r="B147" s="35" t="s">
         <v>1178</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="20" t="s">
+      <c r="C147" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="20" t="s">
         <v>1049</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B148" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="20" t="s">
+      <c r="C148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="20" t="s">
         <v>1155</v>
       </c>
-      <c r="B98" s="20" t="s">
+      <c r="B149" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" s="3" customFormat="1">
-      <c r="A99" s="35" t="s">
+      <c r="C149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" s="3" customFormat="1">
+      <c r="A150" s="35" t="s">
         <v>1051</v>
       </c>
-      <c r="B99" s="35" t="s">
+      <c r="B150" s="35" t="s">
         <v>1180</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="20" t="s">
+      <c r="C150" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="20" t="s">
         <v>1054</v>
       </c>
-      <c r="B100" s="20" t="s">
+      <c r="B151" s="20" t="s">
         <v>1180</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" s="3" customFormat="1">
-      <c r="A101" s="35" t="s">
+      <c r="C151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" s="3" customFormat="1">
+      <c r="A152" s="35" t="s">
         <v>1055</v>
       </c>
-      <c r="B101" s="35" t="s">
+      <c r="B152" s="35" t="s">
         <v>1181</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="20" t="s">
+      <c r="C152" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="20" t="s">
         <v>1057</v>
       </c>
-      <c r="B102" s="20" t="s">
+      <c r="B153" s="20" t="s">
         <v>1181</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="20" t="s">
+      <c r="C153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="20" t="s">
         <v>1189</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B154" s="20" t="s">
         <v>1181</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" s="3" customFormat="1">
-      <c r="A104" s="35" t="s">
+      <c r="C154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" s="3" customFormat="1">
+      <c r="A155" s="35" t="s">
         <v>1059</v>
       </c>
-      <c r="B104" s="35" t="s">
+      <c r="B155" s="35" t="s">
         <v>1182</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="20" t="s">
+      <c r="C155" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="20" t="s">
         <v>1060</v>
       </c>
-      <c r="B105" s="20" t="s">
+      <c r="B156" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="20" t="s">
+      <c r="C156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="20" t="s">
         <v>1159</v>
       </c>
-      <c r="B106" s="20" t="s">
+      <c r="B157" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="20" t="s">
+      <c r="C157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="20" t="s">
         <v>1190</v>
       </c>
-      <c r="B107" s="20" t="s">
+      <c r="B158" s="20" t="s">
         <v>1182</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" s="3" customFormat="1">
-      <c r="A108" s="35" t="s">
+      <c r="C158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="3" customFormat="1">
+      <c r="A159" s="35" t="s">
         <v>1062</v>
       </c>
-      <c r="B108" s="35" t="s">
+      <c r="B159" s="35" t="s">
         <v>1183</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="20" t="s">
+      <c r="C159" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="20" t="s">
         <v>1063</v>
       </c>
-      <c r="B109" s="20" t="s">
+      <c r="B160" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="20" t="s">
+      <c r="C160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="20" t="s">
         <v>1064</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B161" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="20" t="s">
+      <c r="C161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="20" t="s">
         <v>1065</v>
       </c>
-      <c r="B111" s="20" t="s">
+      <c r="B162" s="20" t="s">
         <v>1184</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="20" t="s">
+      <c r="C162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="20" t="s">
         <v>1160</v>
       </c>
-      <c r="B112" s="20" t="s">
+      <c r="B163" s="20" t="s">
         <v>1184</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="20" t="s">
+      <c r="C163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="20" t="s">
         <v>1161</v>
       </c>
-      <c r="B113" s="20" t="s">
+      <c r="B164" s="20" t="s">
         <v>1184</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
-      <c r="A114" s="20" t="s">
+      <c r="C164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="20" t="s">
         <v>1163</v>
       </c>
-      <c r="B114" s="20" t="s">
+      <c r="B165" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="20" t="s">
+      <c r="C165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="20" t="s">
         <v>1164</v>
       </c>
-      <c r="B115" s="20" t="s">
+      <c r="B166" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" s="3" customFormat="1">
-      <c r="A116" s="35" t="s">
+      <c r="C166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="3" customFormat="1">
+      <c r="A167" s="35" t="s">
         <v>1066</v>
       </c>
-      <c r="B116" s="35" t="s">
+      <c r="B167" s="35" t="s">
         <v>1185</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="A117" s="20" t="s">
+      <c r="C167" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="20" t="s">
         <v>1068</v>
       </c>
-      <c r="B117" s="20" t="s">
+      <c r="B168" s="20" t="s">
         <v>1185</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="20" t="s">
+      <c r="C168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="20" t="s">
         <v>1165</v>
       </c>
-      <c r="B118" s="20" t="s">
+      <c r="B169" s="20" t="s">
         <v>970</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
-      <c r="A119" s="20" t="s">
+      <c r="C169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="20" t="s">
         <v>1166</v>
       </c>
-      <c r="B119" s="20" t="s">
+      <c r="B170" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" s="3" customFormat="1">
-      <c r="A120" s="35" t="s">
+      <c r="C170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" s="3" customFormat="1">
+      <c r="A171" s="35" t="s">
         <v>1070</v>
       </c>
-      <c r="B120" s="35" t="s">
+      <c r="B171" s="35" t="s">
         <v>1186</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
-      <c r="A121" s="20" t="s">
+      <c r="C171" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="20" t="s">
         <v>1071</v>
       </c>
-      <c r="B121" s="20" t="s">
+      <c r="B172" s="20" t="s">
         <v>1172</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
-      <c r="A122" s="20" t="s">
+      <c r="C172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="20" t="s">
         <v>1168</v>
       </c>
-      <c r="B122" s="20" t="s">
+      <c r="B173" s="20" t="s">
         <v>1172</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="20" t="s">
+      <c r="C173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="20" t="s">
         <v>1169</v>
       </c>
-      <c r="B123" s="20" t="s">
+      <c r="B174" s="20" t="s">
         <v>1172</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" s="3" customFormat="1">
-      <c r="A124" s="35" t="s">
+      <c r="C174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" s="3" customFormat="1">
+      <c r="A175" s="35" t="s">
         <v>1073</v>
       </c>
-      <c r="B124" s="35" t="s">
+      <c r="B175" s="35" t="s">
         <v>1180</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" s="3" customFormat="1">
-      <c r="A125" s="35" t="s">
+      <c r="C175" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" s="3" customFormat="1">
+      <c r="A176" s="35" t="s">
         <v>1078</v>
       </c>
-      <c r="B125" s="35" t="s">
+      <c r="B176" s="35" t="s">
         <v>1180</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5">
-      <c r="A126" s="20" t="s">
+      <c r="C176" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="20" t="s">
         <v>1080</v>
       </c>
-      <c r="B126" s="20" t="s">
+      <c r="B177" s="20" t="s">
         <v>1187</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="20" t="s">
+      <c r="C177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="20" t="s">
         <v>1082</v>
       </c>
-      <c r="B127" s="20" t="s">
+      <c r="B178" s="20" t="s">
         <v>1187</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" s="3" customFormat="1">
-      <c r="A128" s="35" t="s">
+      <c r="C178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" s="3" customFormat="1">
+      <c r="A179" s="35" t="s">
         <v>1083</v>
       </c>
-      <c r="B128" s="35" t="s">
+      <c r="B179" s="35" t="s">
         <v>1188</v>
       </c>
-      <c r="C128" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="20" t="s">
+      <c r="C179" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="20" t="s">
         <v>1084</v>
       </c>
-      <c r="B129" s="20" t="s">
+      <c r="B180" s="20" t="s">
         <v>1183</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E129" s="1" t="s">
+      <c r="C180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" s="3" customFormat="1">
+      <c r="A181" s="35" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B181" s="35" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="20" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B182" s="20" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="20" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B183" s="20" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="20" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B184" s="20" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" s="3" customFormat="1">
+      <c r="A185" s="35" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B185" s="35" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="20" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B186" s="20" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" s="3" customFormat="1">
+      <c r="A187" s="35" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B187" s="35" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="20" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B188" s="20" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="20" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B189" s="20" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" s="3" customFormat="1">
+      <c r="A190" s="35" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B190" s="35" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="20" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B191" s="20" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" s="3" customFormat="1">
+      <c r="A192" s="35" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B192" s="35" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="20" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B193" s="20" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" s="3" customFormat="1">
+      <c r="A194" s="35" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B194" s="35" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="20" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B195" s="20" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="3" customFormat="1">
+      <c r="A196" s="35" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B196" s="35" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="20" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B197" s="20" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="20" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B198" s="20" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="20" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B199" s="20" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" s="3" customFormat="1">
+      <c r="A200" s="35" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B200" s="35" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="20" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B201" s="20" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="20" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B202" s="20" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E202" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7252,7 +8691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update tutorial setup add skip button to tutorial
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3845" uniqueCount="1340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3850" uniqueCount="1343">
   <si>
     <t>XXXX</t>
   </si>
@@ -4748,6 +4748,15 @@
   </si>
   <si>
     <t>Total de casos</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SKIP</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>Omitir</t>
   </si>
 </sst>
 </file>
@@ -12045,10 +12054,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -13132,12 +13141,12 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="7" customFormat="1" ht="28.5">
+    <row r="64" spans="1:5" s="7" customFormat="1">
       <c r="A64" s="7" t="s">
-        <v>139</v>
+        <v>1340</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>140</v>
+        <v>1341</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>0</v>
@@ -13145,135 +13154,135 @@
       <c r="D64" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E64" s="13" t="s">
-        <v>571</v>
+      <c r="E64" s="40" t="s">
+        <v>1342</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="7" customFormat="1" ht="28.5">
       <c r="A65" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="7" customFormat="1" ht="28.5">
+      <c r="A66" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B66" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="C65" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="13" t="s">
+      <c r="C66" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="13" t="s">
         <v>570</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="7" customFormat="1">
-      <c r="A66" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="7" customFormat="1">
       <c r="A67" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="7" customFormat="1">
+      <c r="A68" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B68" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C67" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" s="11" t="s">
+      <c r="C68" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="11" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" ht="57">
-      <c r="A68" s="7" t="s">
+    <row r="69" spans="1:5" s="7" customFormat="1" ht="57">
+      <c r="A69" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C68" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="13" t="s">
+      <c r="C69" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="13" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" ht="42.75">
-      <c r="A69" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="13" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="7" customFormat="1" ht="42.75">
       <c r="A70" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="7" customFormat="1" ht="42.75">
+      <c r="A71" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" s="12" t="s">
+      <c r="C71" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>567</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="7" customFormat="1" ht="28.5">
-      <c r="A71" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="7" customFormat="1" ht="28.5">
       <c r="A72" s="7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>0</v>
@@ -13281,169 +13290,169 @@
       <c r="D72" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E72" s="12" t="s">
-        <v>565</v>
+      <c r="E72" s="13" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="7" customFormat="1" ht="28.5">
       <c r="A73" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="7" customFormat="1" ht="28.5">
+      <c r="A74" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B74" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C73" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="13" t="s">
+      <c r="C74" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="13" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="7" customFormat="1" ht="71.25">
-      <c r="A74" s="7" t="s">
-        <v>512</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>517</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" ht="71.25">
       <c r="A75" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="7" customFormat="1" ht="71.25">
+      <c r="A76" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B76" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75" s="12" t="s">
+      <c r="C76" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="12" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="7" customFormat="1" ht="57">
-      <c r="A76" s="7" t="s">
+    <row r="77" spans="1:5" s="7" customFormat="1" ht="57">
+      <c r="A77" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B77" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="C76" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" s="13" t="s">
+      <c r="C77" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="13" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="7" customFormat="1" ht="42.75">
-      <c r="A77" s="7" t="s">
+    <row r="78" spans="1:5" s="7" customFormat="1" ht="42.75">
+      <c r="A78" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B78" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C77" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="11" t="s">
+      <c r="C78" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="11" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="28.5">
-      <c r="A78" s="7" t="s">
+    <row r="79" spans="1:5" ht="28.5">
+      <c r="A79" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B79" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="C78" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="13" t="s">
+      <c r="C79" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="13" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="7" t="s">
+    <row r="80" spans="1:5">
+      <c r="A80" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B80" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="11" t="s">
+      <c r="C80" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="8" t="s">
+    <row r="81" spans="1:5">
+      <c r="A81" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B81" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="11" t="s">
+      <c r="C81" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="11" t="s">
         <v>471</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="13" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>442</v>
+        <v>390</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>0</v>
@@ -13451,50 +13460,50 @@
       <c r="D82" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E82" s="11" t="s">
-        <v>494</v>
+      <c r="E82" s="13" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B84" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="C83" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="11" t="s">
+      <c r="C84" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="11" t="s">
         <v>495</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="28.5">
-      <c r="A84" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="28.5">
       <c r="A85" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>0</v>
@@ -13503,15 +13512,15 @@
         <v>0</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="28.5">
       <c r="A86" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>0</v>
@@ -13520,151 +13529,151 @@
         <v>0</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="28.5">
       <c r="A87" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="28.5">
+      <c r="A88" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B88" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="C87" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="13" t="s">
+      <c r="C88" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="13" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="42.75">
-      <c r="A88" s="7" t="s">
+    <row r="89" spans="1:5" ht="42.75">
+      <c r="A89" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B89" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="C88" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="13" t="s">
+      <c r="C89" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="13" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="28.5">
-      <c r="A89" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="13" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.5">
       <c r="A90" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="28.5">
+      <c r="A91" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B91" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="C90" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="13" t="s">
+      <c r="C91" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="13" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="28.5">
-      <c r="A91" s="8" t="s">
+    <row r="92" spans="1:5" ht="28.5">
+      <c r="A92" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B92" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="C91" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="13" t="s">
+      <c r="C92" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="42.75">
-      <c r="A92" s="8" t="s">
+    <row r="93" spans="1:5" ht="42.75">
+      <c r="A93" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B93" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="C92" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E92" s="13" t="s">
+      <c r="C93" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="13" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="28.5">
-      <c r="A93" s="8" t="s">
+    <row r="94" spans="1:5" ht="28.5">
+      <c r="A94" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B94" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="C93" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E93" s="13" t="s">
+      <c r="C94" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>546</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" s="7" customFormat="1" ht="42.75">
-      <c r="A94" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="13" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="7" customFormat="1" ht="42.75">
       <c r="A95" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>0</v>
@@ -13673,49 +13682,49 @@
         <v>0</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="7" customFormat="1" ht="42.75">
       <c r="A96" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" s="7" customFormat="1" ht="42.75">
+      <c r="A97" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B97" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="C96" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="12" t="s">
+      <c r="C97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="12" t="s">
         <v>543</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" s="7" customFormat="1" ht="28.5">
-      <c r="A97" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="13" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="7" customFormat="1" ht="28.5">
       <c r="A98" s="7" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>0</v>
@@ -13724,50 +13733,49 @@
         <v>0</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="99" spans="1:6" s="7" customFormat="1" ht="28.5">
       <c r="A99" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" s="7" customFormat="1" ht="28.5">
+      <c r="A100" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B100" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="C99" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E99" s="13" t="s">
+      <c r="C100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="13" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="12" t="s">
-        <v>547</v>
-      </c>
-      <c r="F100" s="7"/>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>0</v>
@@ -13775,17 +13783,17 @@
       <c r="D101" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E101" s="13" t="s">
-        <v>548</v>
+      <c r="E101" s="12" t="s">
+        <v>547</v>
       </c>
       <c r="F101" s="7"/>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>0</v>
@@ -13793,17 +13801,17 @@
       <c r="D102" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E102" s="12" t="s">
-        <v>549</v>
+      <c r="E102" s="13" t="s">
+        <v>548</v>
       </c>
       <c r="F102" s="7"/>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>0</v>
@@ -13811,120 +13819,121 @@
       <c r="D103" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E103" s="13" t="s">
-        <v>550</v>
+      <c r="E103" s="12" t="s">
+        <v>549</v>
       </c>
       <c r="F103" s="7"/>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="13" t="s">
+        <v>550</v>
+      </c>
+      <c r="F104" s="7"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B105" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="C104" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E104" s="13" t="s">
+      <c r="C105" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="13" t="s">
         <v>551</v>
       </c>
-      <c r="F104" s="7"/>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E105" s="11" t="s">
-        <v>505</v>
-      </c>
+      <c r="F105" s="7"/>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="11" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="8" t="s">
         <v>855</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B107" s="7" t="s">
         <v>856</v>
       </c>
-      <c r="C106" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="29" t="s">
+      <c r="C107" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="29" t="s">
         <v>856</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="E107" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="E108" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B109" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C109" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="D108" s="9" t="s">
+      <c r="D109" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E109" t="s">
         <v>447</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" s="8" t="s">
-        <v>499</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109" s="13" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>0</v>
@@ -13932,16 +13941,16 @@
       <c r="D110" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E110" s="11" t="s">
-        <v>501</v>
+      <c r="E110" s="13" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="8" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>542</v>
+        <v>503</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>0</v>
@@ -13949,16 +13958,16 @@
       <c r="D111" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="12" t="s">
-        <v>584</v>
+      <c r="E111" s="11" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>0</v>
@@ -13967,15 +13976,15 @@
         <v>0</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>510</v>
+        <v>541</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>0</v>
@@ -13983,67 +13992,67 @@
       <c r="D113" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E113" s="13" t="s">
-        <v>586</v>
+      <c r="E113" s="12" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="8" t="s">
         <v>509</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="B115" s="8" t="s">
         <v>511</v>
       </c>
-      <c r="C114" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E114" s="12" t="s">
+      <c r="C115" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="12" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="28.5">
-      <c r="A115" s="8" t="s">
+    <row r="116" spans="1:5" ht="28.5">
+      <c r="A116" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="B115" s="7" t="s">
+      <c r="B116" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="C115" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E115" s="12" t="s">
+      <c r="C116" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="12" t="s">
         <v>588</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="42.75">
-      <c r="A116" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="B116" s="7" t="s">
-        <v>532</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E116" s="13" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="42.75">
       <c r="A117" s="8" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>0</v>
@@ -14052,15 +14061,15 @@
         <v>0</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="42.75">
       <c r="A118" s="8" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>858</v>
+        <v>527</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>0</v>
@@ -14069,74 +14078,91 @@
         <v>0</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="42.75">
       <c r="A119" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E119" s="13" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="42.75">
+      <c r="A120" s="8" t="s">
         <v>530</v>
       </c>
-      <c r="B119" s="7" t="s">
+      <c r="B120" s="7" t="s">
         <v>859</v>
       </c>
-      <c r="C119" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E119" s="13" t="s">
+      <c r="C120" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E120" s="13" t="s">
         <v>592</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="28.5">
-      <c r="A120" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E120" s="13" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="28.5">
       <c r="A121" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E121" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="28.5">
+      <c r="A122" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="B121" s="7" t="s">
+      <c r="B122" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="C121" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E121" s="12" t="s">
+      <c r="C122" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122" s="12" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="17" customFormat="1">
-      <c r="A122" s="34" t="s">
+    <row r="123" spans="1:5" s="17" customFormat="1">
+      <c r="A123" s="34" t="s">
         <v>1039</v>
       </c>
-      <c r="B122" s="16" t="s">
+      <c r="B123" s="16" t="s">
         <v>974</v>
       </c>
-      <c r="C122" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D122" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E122" s="1" t="s">
+      <c r="C123" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D123" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add scenario tracker to keep a history of the scenarios a player has seen so that they can report issues as they find them Add feedback screen to use elastic email to send information as api request rather than using email. Add scenario and general feedback
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3850" uniqueCount="1343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3875" uniqueCount="1357">
   <si>
     <t>XXXX</t>
   </si>
@@ -4757,6 +4757,48 @@
   </si>
   <si>
     <t>Omitir</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SEND_FEEDBACK</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SUBJECT</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CANCEL</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SEND</t>
+  </si>
+  <si>
+    <t>Send Feedback</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Send</t>
+  </si>
+  <si>
+    <t>Resolución</t>
+  </si>
+  <si>
+    <t>Enviar comentarios</t>
+  </si>
+  <si>
+    <t>Cancelar</t>
+  </si>
+  <si>
+    <t>Enviar</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_REPORT_SCENARIO</t>
+  </si>
+  <si>
+    <t>Problema del escenario del informe</t>
+  </si>
+  <si>
+    <t>Report Scenario problem</t>
   </si>
 </sst>
 </file>
@@ -12054,10 +12096,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -14153,7 +14195,7 @@
       <c r="A123" s="34" t="s">
         <v>1039</v>
       </c>
-      <c r="B123" s="16" t="s">
+      <c r="B123" t="s">
         <v>974</v>
       </c>
       <c r="C123" s="17" t="s">
@@ -14162,8 +14204,93 @@
       <c r="D123" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E123" s="1" t="s">
-        <v>0</v>
+      <c r="E123" s="40" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="8" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124" s="40" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="8" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E125" s="40" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="8" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E126" s="40" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="8" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E127" s="40" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="8" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="40" t="s">
+        <v>1355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ensure playing tutorial for first time does not break the game Save language selection over multiple plays
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3875" uniqueCount="1357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3875" uniqueCount="1358">
   <si>
     <t>XXXX</t>
   </si>
@@ -4799,6 +4799,9 @@
   </si>
   <si>
     <t>Here you will see all your active incidents, coloured by severity, with red being the most severe</t>
+  </si>
+  <si>
+    <t>Tutorial de repetición</t>
   </si>
 </sst>
 </file>
@@ -4960,7 +4963,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5046,7 +5049,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -7703,10 +7705,10 @@
       </c>
     </row>
     <row r="138" spans="1:5" s="3" customFormat="1">
-      <c r="A138" s="35" t="s">
+      <c r="A138" s="34" t="s">
         <v>1037</v>
       </c>
-      <c r="B138" s="35" t="s">
+      <c r="B138" s="34" t="s">
         <v>1171</v>
       </c>
       <c r="C138" s="3" t="s">
@@ -7754,10 +7756,10 @@
       </c>
     </row>
     <row r="141" spans="1:5" s="3" customFormat="1">
-      <c r="A141" s="35" t="s">
+      <c r="A141" s="34" t="s">
         <v>1042</v>
       </c>
-      <c r="B141" s="35" t="s">
+      <c r="B141" s="34" t="s">
         <v>1174</v>
       </c>
       <c r="C141" s="3" t="s">
@@ -7856,10 +7858,10 @@
       </c>
     </row>
     <row r="147" spans="1:5" s="3" customFormat="1">
-      <c r="A147" s="35" t="s">
+      <c r="A147" s="34" t="s">
         <v>1046</v>
       </c>
-      <c r="B147" s="35" t="s">
+      <c r="B147" s="34" t="s">
         <v>1177</v>
       </c>
       <c r="C147" s="3" t="s">
@@ -7907,10 +7909,10 @@
       </c>
     </row>
     <row r="150" spans="1:5" s="3" customFormat="1">
-      <c r="A150" s="35" t="s">
+      <c r="A150" s="34" t="s">
         <v>1050</v>
       </c>
-      <c r="B150" s="35" t="s">
+      <c r="B150" s="34" t="s">
         <v>1179</v>
       </c>
       <c r="C150" s="3" t="s">
@@ -7941,10 +7943,10 @@
       </c>
     </row>
     <row r="152" spans="1:5" s="3" customFormat="1">
-      <c r="A152" s="35" t="s">
+      <c r="A152" s="34" t="s">
         <v>1054</v>
       </c>
-      <c r="B152" s="35" t="s">
+      <c r="B152" s="34" t="s">
         <v>1180</v>
       </c>
       <c r="C152" s="3" t="s">
@@ -7992,10 +7994,10 @@
       </c>
     </row>
     <row r="155" spans="1:5" s="3" customFormat="1">
-      <c r="A155" s="35" t="s">
+      <c r="A155" s="34" t="s">
         <v>1058</v>
       </c>
-      <c r="B155" s="35" t="s">
+      <c r="B155" s="34" t="s">
         <v>1181</v>
       </c>
       <c r="C155" s="3" t="s">
@@ -8060,10 +8062,10 @@
       </c>
     </row>
     <row r="159" spans="1:5" s="3" customFormat="1">
-      <c r="A159" s="35" t="s">
+      <c r="A159" s="34" t="s">
         <v>1061</v>
       </c>
-      <c r="B159" s="35" t="s">
+      <c r="B159" s="34" t="s">
         <v>1182</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -8196,10 +8198,10 @@
       </c>
     </row>
     <row r="167" spans="1:5" s="3" customFormat="1">
-      <c r="A167" s="35" t="s">
+      <c r="A167" s="34" t="s">
         <v>1065</v>
       </c>
-      <c r="B167" s="35" t="s">
+      <c r="B167" s="34" t="s">
         <v>1184</v>
       </c>
       <c r="C167" s="3" t="s">
@@ -8264,10 +8266,10 @@
       </c>
     </row>
     <row r="171" spans="1:5" s="3" customFormat="1">
-      <c r="A171" s="35" t="s">
+      <c r="A171" s="34" t="s">
         <v>1069</v>
       </c>
-      <c r="B171" s="35" t="s">
+      <c r="B171" s="34" t="s">
         <v>1185</v>
       </c>
       <c r="C171" s="3" t="s">
@@ -8332,10 +8334,10 @@
       </c>
     </row>
     <row r="175" spans="1:5" s="3" customFormat="1">
-      <c r="A175" s="35" t="s">
+      <c r="A175" s="34" t="s">
         <v>1072</v>
       </c>
-      <c r="B175" s="35" t="s">
+      <c r="B175" s="34" t="s">
         <v>1179</v>
       </c>
       <c r="C175" s="3" t="s">
@@ -8349,10 +8351,10 @@
       </c>
     </row>
     <row r="176" spans="1:5" s="3" customFormat="1">
-      <c r="A176" s="35" t="s">
+      <c r="A176" s="34" t="s">
         <v>1077</v>
       </c>
-      <c r="B176" s="35" t="s">
+      <c r="B176" s="34" t="s">
         <v>1179</v>
       </c>
       <c r="C176" s="3" t="s">
@@ -8400,10 +8402,10 @@
       </c>
     </row>
     <row r="179" spans="1:5" s="3" customFormat="1">
-      <c r="A179" s="35" t="s">
+      <c r="A179" s="34" t="s">
         <v>1082</v>
       </c>
-      <c r="B179" s="35" t="s">
+      <c r="B179" s="34" t="s">
         <v>1187</v>
       </c>
       <c r="C179" s="3" t="s">
@@ -8434,10 +8436,10 @@
       </c>
     </row>
     <row r="181" spans="1:5" s="3" customFormat="1">
-      <c r="A181" s="35" t="s">
+      <c r="A181" s="34" t="s">
         <v>1088</v>
       </c>
-      <c r="B181" s="35" t="s">
+      <c r="B181" s="34" t="s">
         <v>1302</v>
       </c>
       <c r="C181" s="3" t="s">
@@ -8502,10 +8504,10 @@
       </c>
     </row>
     <row r="185" spans="1:5" s="3" customFormat="1">
-      <c r="A185" s="35" t="s">
+      <c r="A185" s="34" t="s">
         <v>1094</v>
       </c>
-      <c r="B185" s="35" t="s">
+      <c r="B185" s="34" t="s">
         <v>1171</v>
       </c>
       <c r="C185" s="3" t="s">
@@ -8536,10 +8538,10 @@
       </c>
     </row>
     <row r="187" spans="1:5" s="3" customFormat="1">
-      <c r="A187" s="35" t="s">
+      <c r="A187" s="34" t="s">
         <v>1098</v>
       </c>
-      <c r="B187" s="35" t="s">
+      <c r="B187" s="34" t="s">
         <v>1304</v>
       </c>
       <c r="C187" s="3" t="s">
@@ -8587,10 +8589,10 @@
       </c>
     </row>
     <row r="190" spans="1:5" s="3" customFormat="1">
-      <c r="A190" s="35" t="s">
+      <c r="A190" s="34" t="s">
         <v>1102</v>
       </c>
-      <c r="B190" s="35" t="s">
+      <c r="B190" s="34" t="s">
         <v>1184</v>
       </c>
       <c r="C190" s="3" t="s">
@@ -8621,10 +8623,10 @@
       </c>
     </row>
     <row r="192" spans="1:5" s="3" customFormat="1">
-      <c r="A192" s="35" t="s">
+      <c r="A192" s="34" t="s">
         <v>1107</v>
       </c>
-      <c r="B192" s="35" t="s">
+      <c r="B192" s="34" t="s">
         <v>1306</v>
       </c>
       <c r="C192" s="3" t="s">
@@ -8655,10 +8657,10 @@
       </c>
     </row>
     <row r="194" spans="1:5" s="3" customFormat="1">
-      <c r="A194" s="35" t="s">
+      <c r="A194" s="34" t="s">
         <v>1111</v>
       </c>
-      <c r="B194" s="35" t="s">
+      <c r="B194" s="34" t="s">
         <v>1308</v>
       </c>
       <c r="C194" s="3" t="s">
@@ -8689,10 +8691,10 @@
       </c>
     </row>
     <row r="196" spans="1:5" s="3" customFormat="1">
-      <c r="A196" s="35" t="s">
+      <c r="A196" s="34" t="s">
         <v>1116</v>
       </c>
-      <c r="B196" s="35" t="s">
+      <c r="B196" s="34" t="s">
         <v>1309</v>
       </c>
       <c r="C196" s="3" t="s">
@@ -8757,10 +8759,10 @@
       </c>
     </row>
     <row r="200" spans="1:5" s="3" customFormat="1">
-      <c r="A200" s="35" t="s">
+      <c r="A200" s="34" t="s">
         <v>1120</v>
       </c>
-      <c r="B200" s="35" t="s">
+      <c r="B200" s="34" t="s">
         <v>1312</v>
       </c>
       <c r="C200" s="3" t="s">
@@ -8852,7 +8854,7 @@
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>1190</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -8869,7 +8871,7 @@
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>1191</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -8886,7 +8888,7 @@
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>1192</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -8903,7 +8905,7 @@
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>1193</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -8920,7 +8922,7 @@
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>1194</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -8938,7 +8940,7 @@
       <c r="A7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>1195</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -8956,7 +8958,7 @@
       <c r="A8" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>1196</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -8973,7 +8975,7 @@
       <c r="A9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>1197</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -8990,7 +8992,7 @@
       <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>1198</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -9007,7 +9009,7 @@
       <c r="A11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>1199</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -9024,7 +9026,7 @@
       <c r="A12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>1200</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -9041,7 +9043,7 @@
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>1201</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -9058,7 +9060,7 @@
       <c r="A14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>1202</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -9075,7 +9077,7 @@
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>1203</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -9088,28 +9090,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="37" customFormat="1">
-      <c r="A16" s="36" t="s">
+    <row r="16" spans="1:6" s="36" customFormat="1">
+      <c r="A16" s="35" t="s">
         <v>1037</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>1187</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="38" t="s">
+      <c r="C16" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="37" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>1039</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>1204</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -9123,10 +9125,10 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>1040</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>1205</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -9140,10 +9142,10 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="29" t="s">
         <v>1041</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>1204</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -9157,10 +9159,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="3" customFormat="1">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="29" t="s">
         <v>1148</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
         <v>1206</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -9173,28 +9175,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="37" customFormat="1">
-      <c r="A21" s="36" t="s">
+    <row r="21" spans="1:5" s="36" customFormat="1">
+      <c r="A21" s="35" t="s">
         <v>1042</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="35" t="s">
         <v>1207</v>
       </c>
-      <c r="C21" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="38" t="s">
+      <c r="C21" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="37" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="3" customFormat="1">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="29" t="s">
         <v>1043</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>1204</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -9208,10 +9210,10 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="29" t="s">
         <v>1044</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>1204</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -9225,10 +9227,10 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="29" t="s">
         <v>1045</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>1208</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -9242,10 +9244,10 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="29" t="s">
         <v>1152</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>999</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -9262,7 +9264,7 @@
       <c r="A26" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="35" t="s">
         <v>1213</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -9279,7 +9281,7 @@
       <c r="A27" s="1" t="s">
         <v>1212</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>1214</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -9296,7 +9298,7 @@
       <c r="A28" s="1" t="s">
         <v>1211</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="29" t="s">
         <v>1215</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -9313,7 +9315,7 @@
       <c r="A29" s="1" t="s">
         <v>1216</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="29" t="s">
         <v>1217</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -9330,7 +9332,7 @@
       <c r="A30" s="1" t="s">
         <v>1218</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="29" t="s">
         <v>1219</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -9347,7 +9349,7 @@
       <c r="A31" s="1" t="s">
         <v>1210</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="29" t="s">
         <v>1220</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -9364,7 +9366,7 @@
       <c r="A32" s="1" t="s">
         <v>1221</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="29" t="s">
         <v>1223</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -9381,7 +9383,7 @@
       <c r="A33" s="1" t="s">
         <v>1222</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="29" t="s">
         <v>1224</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -9398,7 +9400,7 @@
       <c r="A34" s="1" t="s">
         <v>1225</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="29" t="s">
         <v>1227</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -9415,7 +9417,7 @@
       <c r="A35" s="1" t="s">
         <v>1226</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="29" t="s">
         <v>1224</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -9432,7 +9434,7 @@
       <c r="A36" s="3" t="s">
         <v>1228</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="35" t="s">
         <v>1231</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -9449,7 +9451,7 @@
       <c r="A37" s="1" t="s">
         <v>1229</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="29" t="s">
         <v>1232</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -9466,7 +9468,7 @@
       <c r="A38" s="1" t="s">
         <v>1230</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="29" t="s">
         <v>1233</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -9483,7 +9485,7 @@
       <c r="A39" s="1" t="s">
         <v>1234</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="29" t="s">
         <v>1236</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -9500,7 +9502,7 @@
       <c r="A40" s="1" t="s">
         <v>1235</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="29" t="s">
         <v>1237</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -9517,7 +9519,7 @@
       <c r="A41" s="1" t="s">
         <v>1238</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="29" t="s">
         <v>1240</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -9534,7 +9536,7 @@
       <c r="A42" s="1" t="s">
         <v>1239</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="29" t="s">
         <v>1241</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -9551,7 +9553,7 @@
       <c r="A43" s="1" t="s">
         <v>1242</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="29" t="s">
         <v>1243</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -9568,7 +9570,7 @@
       <c r="A44" s="1" t="s">
         <v>1244</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="29" t="s">
         <v>1237</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -9585,7 +9587,7 @@
       <c r="A45" s="1" t="s">
         <v>1245</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="29" t="s">
         <v>1247</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -9602,7 +9604,7 @@
       <c r="A46" s="1" t="s">
         <v>1246</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="29" t="s">
         <v>1248</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -11187,7 +11189,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" customFormat="1">
-      <c r="A92" s="33" t="s">
+      <c r="A92" s="32" t="s">
         <v>1037</v>
       </c>
       <c r="B92" t="s">
@@ -11323,7 +11325,7 @@
       </c>
     </row>
     <row r="100" spans="1:5" customFormat="1">
-      <c r="A100" s="33" t="s">
+      <c r="A100" s="32" t="s">
         <v>1042</v>
       </c>
       <c r="B100" t="s">
@@ -11408,7 +11410,7 @@
       </c>
     </row>
     <row r="105" spans="1:5" customFormat="1">
-      <c r="A105" s="33" t="s">
+      <c r="A105" s="32" t="s">
         <v>1046</v>
       </c>
       <c r="B105" t="s">
@@ -11544,7 +11546,7 @@
       </c>
     </row>
     <row r="113" spans="1:5" customFormat="1">
-      <c r="A113" s="33" t="s">
+      <c r="A113" s="32" t="s">
         <v>1050</v>
       </c>
       <c r="B113" t="s">
@@ -11612,7 +11614,7 @@
       </c>
     </row>
     <row r="117" spans="1:5" customFormat="1">
-      <c r="A117" s="33" t="s">
+      <c r="A117" s="32" t="s">
         <v>1054</v>
       </c>
       <c r="B117" t="s">
@@ -11663,7 +11665,7 @@
       </c>
     </row>
     <row r="120" spans="1:5" customFormat="1">
-      <c r="A120" s="33" t="s">
+      <c r="A120" s="32" t="s">
         <v>1058</v>
       </c>
       <c r="B120" t="s">
@@ -11731,7 +11733,7 @@
       </c>
     </row>
     <row r="124" spans="1:5" customFormat="1">
-      <c r="A124" s="33" t="s">
+      <c r="A124" s="32" t="s">
         <v>1061</v>
       </c>
       <c r="B124" t="s">
@@ -11833,7 +11835,7 @@
       </c>
     </row>
     <row r="130" spans="1:5" customFormat="1">
-      <c r="A130" s="33" t="s">
+      <c r="A130" s="32" t="s">
         <v>1065</v>
       </c>
       <c r="B130" t="s">
@@ -11901,7 +11903,7 @@
       </c>
     </row>
     <row r="134" spans="1:5" customFormat="1">
-      <c r="A134" s="33" t="s">
+      <c r="A134" s="32" t="s">
         <v>1069</v>
       </c>
       <c r="B134" t="s">
@@ -12003,7 +12005,7 @@
       </c>
     </row>
     <row r="140" spans="1:5" customFormat="1">
-      <c r="A140" s="33" t="s">
+      <c r="A140" s="32" t="s">
         <v>1072</v>
       </c>
       <c r="B140" t="s">
@@ -12098,8 +12100,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -13060,7 +13062,7 @@
       <c r="D56" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E56" s="40" t="s">
+      <c r="E56" s="39" t="s">
         <v>1338</v>
       </c>
     </row>
@@ -13077,7 +13079,7 @@
       <c r="D57" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E57" s="40" t="s">
+      <c r="E57" s="39" t="s">
         <v>1326</v>
       </c>
     </row>
@@ -13094,7 +13096,7 @@
       <c r="D58" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E58" s="40" t="s">
+      <c r="E58" s="39" t="s">
         <v>1327</v>
       </c>
     </row>
@@ -13111,7 +13113,7 @@
       <c r="D59" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="40" t="s">
+      <c r="E59" s="39" t="s">
         <v>1328</v>
       </c>
     </row>
@@ -13128,7 +13130,7 @@
       <c r="D60" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E60" s="40" t="s">
+      <c r="E60" s="39" t="s">
         <v>1329</v>
       </c>
     </row>
@@ -13145,7 +13147,7 @@
       <c r="D61" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E61" s="40" t="s">
+      <c r="E61" s="39" t="s">
         <v>1330</v>
       </c>
     </row>
@@ -13162,7 +13164,7 @@
       <c r="D62" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E62" s="40" t="s">
+      <c r="E62" s="39" t="s">
         <v>1333</v>
       </c>
     </row>
@@ -13179,7 +13181,7 @@
       <c r="D63" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E63" s="40" t="s">
+      <c r="E63" s="39" t="s">
         <v>1336</v>
       </c>
     </row>
@@ -13196,7 +13198,7 @@
       <c r="D64" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E64" s="40" t="s">
+      <c r="E64" s="39" t="s">
         <v>1341</v>
       </c>
     </row>
@@ -13932,8 +13934,8 @@
       <c r="D107" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E107" s="29" t="s">
-        <v>855</v>
+      <c r="E107" s="39" t="s">
+        <v>1357</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -14192,7 +14194,7 @@
       </c>
     </row>
     <row r="123" spans="1:5" s="17" customFormat="1">
-      <c r="A123" s="34" t="s">
+      <c r="A123" s="33" t="s">
         <v>1038</v>
       </c>
       <c r="B123" t="s">
@@ -14204,7 +14206,7 @@
       <c r="D123" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E123" s="40" t="s">
+      <c r="E123" s="39" t="s">
         <v>1349</v>
       </c>
     </row>
@@ -14221,7 +14223,7 @@
       <c r="D124" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E124" s="40" t="s">
+      <c r="E124" s="39" t="s">
         <v>1350</v>
       </c>
     </row>
@@ -14238,7 +14240,7 @@
       <c r="D125" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="40" t="s">
+      <c r="E125" s="39" t="s">
         <v>465</v>
       </c>
     </row>
@@ -14255,7 +14257,7 @@
       <c r="D126" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E126" s="40" t="s">
+      <c r="E126" s="39" t="s">
         <v>1351</v>
       </c>
     </row>
@@ -14272,7 +14274,7 @@
       <c r="D127" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E127" s="40" t="s">
+      <c r="E127" s="39" t="s">
         <v>1352</v>
       </c>
     </row>
@@ -14289,7 +14291,7 @@
       <c r="D128" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E128" s="40" t="s">
+      <c r="E128" s="39" t="s">
         <v>1354</v>
       </c>
     </row>
@@ -14715,7 +14717,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -14834,7 +14836,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -14953,7 +14955,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.5">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>140</v>
       </c>
       <c r="B16" s="19" t="s">
@@ -15089,7 +15091,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.5">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="32" t="s">
         <v>152</v>
       </c>
       <c r="B24" s="19" t="s">
@@ -15208,7 +15210,7 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="32" t="s">
         <v>161</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -15344,7 +15346,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="42.75">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="32" t="s">
         <v>174</v>
       </c>
       <c r="B39" s="19" t="s">
@@ -15446,7 +15448,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="57">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="32" t="s">
         <v>190</v>
       </c>
       <c r="B45" s="19" t="s">
@@ -15582,7 +15584,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.5">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="32" t="s">
         <v>210</v>
       </c>
       <c r="B53" s="14" t="s">
@@ -15701,7 +15703,7 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="32" t="s">
         <v>226</v>
       </c>
       <c r="B60" s="14" t="s">
@@ -15803,7 +15805,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="28.5">
-      <c r="A66" s="33" t="s">
+      <c r="A66" s="32" t="s">
         <v>238</v>
       </c>
       <c r="B66" s="14" t="s">
@@ -15922,7 +15924,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="28.5">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="32" t="s">
         <v>243</v>
       </c>
       <c r="B73" s="14" t="s">
@@ -15939,7 +15941,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="57">
-      <c r="A74" s="34" t="s">
+      <c r="A74" s="33" t="s">
         <v>244</v>
       </c>
       <c r="B74" s="16" t="s">
@@ -16058,7 +16060,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="28.5">
-      <c r="A81" s="33" t="s">
+      <c r="A81" s="32" t="s">
         <v>255</v>
       </c>
       <c r="B81" s="14" t="s">
@@ -16211,7 +16213,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="42.75">
-      <c r="A90" s="33" t="s">
+      <c r="A90" s="32" t="s">
         <v>647</v>
       </c>
       <c r="B90" s="16" t="s">
@@ -16364,7 +16366,7 @@
       </c>
     </row>
     <row r="99" spans="1:5" ht="42.75">
-      <c r="A99" s="33" t="s">
+      <c r="A99" s="32" t="s">
         <v>656</v>
       </c>
       <c r="B99" s="15" t="s">
@@ -16483,7 +16485,7 @@
       </c>
     </row>
     <row r="106" spans="1:5" ht="28.5">
-      <c r="A106" s="33" t="s">
+      <c r="A106" s="32" t="s">
         <v>670</v>
       </c>
       <c r="B106" s="16" t="s">
@@ -16585,7 +16587,7 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="28.5">
-      <c r="A112" s="33" t="s">
+      <c r="A112" s="32" t="s">
         <v>681</v>
       </c>
       <c r="B112" s="16" t="s">
@@ -16721,7 +16723,7 @@
       </c>
     </row>
     <row r="120" spans="1:5" ht="28.5">
-      <c r="A120" s="33" t="s">
+      <c r="A120" s="32" t="s">
         <v>696</v>
       </c>
       <c r="B120" s="16" t="s">
@@ -16840,7 +16842,7 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="28.5">
-      <c r="A127" s="33" t="s">
+      <c r="A127" s="32" t="s">
         <v>710</v>
       </c>
       <c r="B127" s="16" t="s">
@@ -16976,7 +16978,7 @@
       </c>
     </row>
     <row r="135" spans="1:5" ht="28.5">
-      <c r="A135" s="33" t="s">
+      <c r="A135" s="32" t="s">
         <v>726</v>
       </c>
       <c r="B135" s="16" t="s">
@@ -17095,7 +17097,7 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="28.5">
-      <c r="A142" s="33" t="s">
+      <c r="A142" s="32" t="s">
         <v>739</v>
       </c>
       <c r="B142" s="16" t="s">
@@ -17214,10 +17216,10 @@
       </c>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="33" t="s">
+      <c r="A149" s="32" t="s">
         <v>1037</v>
       </c>
-      <c r="B149" s="30" t="s">
+      <c r="B149" s="29" t="s">
         <v>969</v>
       </c>
       <c r="C149" s="17" t="s">
@@ -17234,7 +17236,7 @@
       <c r="A150" t="s">
         <v>1039</v>
       </c>
-      <c r="B150" s="30" t="s">
+      <c r="B150" s="29" t="s">
         <v>970</v>
       </c>
       <c r="C150" s="17" t="s">
@@ -17251,7 +17253,7 @@
       <c r="A151" t="s">
         <v>1040</v>
       </c>
-      <c r="B151" s="30" t="s">
+      <c r="B151" s="29" t="s">
         <v>971</v>
       </c>
       <c r="C151" s="17" t="s">
@@ -17268,7 +17270,7 @@
       <c r="A152" t="s">
         <v>1041</v>
       </c>
-      <c r="B152" s="30" t="s">
+      <c r="B152" s="29" t="s">
         <v>972</v>
       </c>
       <c r="C152" s="17" t="s">
@@ -17282,10 +17284,10 @@
       </c>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="33" t="s">
+      <c r="A153" s="32" t="s">
         <v>1042</v>
       </c>
-      <c r="B153" s="31" t="s">
+      <c r="B153" s="30" t="s">
         <v>974</v>
       </c>
       <c r="C153" s="17" t="s">
@@ -17302,7 +17304,7 @@
       <c r="A154" t="s">
         <v>1043</v>
       </c>
-      <c r="B154" s="31" t="s">
+      <c r="B154" s="30" t="s">
         <v>975</v>
       </c>
       <c r="C154" s="17" t="s">
@@ -17319,7 +17321,7 @@
       <c r="A155" t="s">
         <v>1044</v>
       </c>
-      <c r="B155" s="31" t="s">
+      <c r="B155" s="30" t="s">
         <v>976</v>
       </c>
       <c r="C155" s="17" t="s">
@@ -17336,7 +17338,7 @@
       <c r="A156" t="s">
         <v>1045</v>
       </c>
-      <c r="B156" s="31" t="s">
+      <c r="B156" s="30" t="s">
         <v>977</v>
       </c>
       <c r="C156" s="17" t="s">
@@ -17350,10 +17352,10 @@
       </c>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="33" t="s">
+      <c r="A157" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="B157" s="30" t="s">
+      <c r="B157" s="29" t="s">
         <v>978</v>
       </c>
       <c r="C157" s="17" t="s">
@@ -17370,7 +17372,7 @@
       <c r="A158" t="s">
         <v>1047</v>
       </c>
-      <c r="B158" s="30" t="s">
+      <c r="B158" s="29" t="s">
         <v>979</v>
       </c>
       <c r="C158" s="17" t="s">
@@ -17387,7 +17389,7 @@
       <c r="A159" t="s">
         <v>1048</v>
       </c>
-      <c r="B159" s="30" t="s">
+      <c r="B159" s="29" t="s">
         <v>980</v>
       </c>
       <c r="C159" s="17" t="s">
@@ -17404,7 +17406,7 @@
       <c r="A160" t="s">
         <v>1049</v>
       </c>
-      <c r="B160" s="30" t="s">
+      <c r="B160" s="29" t="s">
         <v>977</v>
       </c>
       <c r="C160" s="17" t="s">
@@ -17418,10 +17420,10 @@
       </c>
     </row>
     <row r="161" spans="1:5">
-      <c r="A161" s="33" t="s">
+      <c r="A161" s="32" t="s">
         <v>1050</v>
       </c>
-      <c r="B161" s="30" t="s">
+      <c r="B161" s="29" t="s">
         <v>981</v>
       </c>
       <c r="C161" s="17" t="s">
@@ -17438,7 +17440,7 @@
       <c r="A162" t="s">
         <v>1051</v>
       </c>
-      <c r="B162" s="30" t="s">
+      <c r="B162" s="29" t="s">
         <v>982</v>
       </c>
       <c r="C162" s="17" t="s">
@@ -17455,7 +17457,7 @@
       <c r="A163" t="s">
         <v>1052</v>
       </c>
-      <c r="B163" s="30" t="s">
+      <c r="B163" s="29" t="s">
         <v>983</v>
       </c>
       <c r="C163" s="17" t="s">
@@ -17472,7 +17474,7 @@
       <c r="A164" t="s">
         <v>1053</v>
       </c>
-      <c r="B164" s="30" t="s">
+      <c r="B164" s="29" t="s">
         <v>977</v>
       </c>
       <c r="C164" s="17" t="s">
@@ -17486,10 +17488,10 @@
       </c>
     </row>
     <row r="165" spans="1:5">
-      <c r="A165" s="33" t="s">
+      <c r="A165" s="32" t="s">
         <v>1054</v>
       </c>
-      <c r="B165" s="30" t="s">
+      <c r="B165" s="29" t="s">
         <v>984</v>
       </c>
       <c r="C165" s="17" t="s">
@@ -17506,7 +17508,7 @@
       <c r="A166" t="s">
         <v>1055</v>
       </c>
-      <c r="B166" s="30" t="s">
+      <c r="B166" s="29" t="s">
         <v>985</v>
       </c>
       <c r="C166" s="17" t="s">
@@ -17523,7 +17525,7 @@
       <c r="A167" t="s">
         <v>1056</v>
       </c>
-      <c r="B167" s="30" t="s">
+      <c r="B167" s="29" t="s">
         <v>986</v>
       </c>
       <c r="C167" s="17" t="s">
@@ -17540,7 +17542,7 @@
       <c r="A168" t="s">
         <v>1057</v>
       </c>
-      <c r="B168" s="30" t="s">
+      <c r="B168" s="29" t="s">
         <v>987</v>
       </c>
       <c r="C168" s="17" t="s">
@@ -17554,10 +17556,10 @@
       </c>
     </row>
     <row r="169" spans="1:5">
-      <c r="A169" s="33" t="s">
+      <c r="A169" s="32" t="s">
         <v>1058</v>
       </c>
-      <c r="B169" s="30" t="s">
+      <c r="B169" s="29" t="s">
         <v>988</v>
       </c>
       <c r="C169" s="17" t="s">
@@ -17574,7 +17576,7 @@
       <c r="A170" t="s">
         <v>1059</v>
       </c>
-      <c r="B170" s="30" t="s">
+      <c r="B170" s="29" t="s">
         <v>989</v>
       </c>
       <c r="C170" s="17" t="s">
@@ -17591,7 +17593,7 @@
       <c r="A171" t="s">
         <v>1060</v>
       </c>
-      <c r="B171" s="30" t="s">
+      <c r="B171" s="29" t="s">
         <v>987</v>
       </c>
       <c r="C171" s="17" t="s">
@@ -17605,10 +17607,10 @@
       </c>
     </row>
     <row r="172" spans="1:5">
-      <c r="A172" s="33" t="s">
+      <c r="A172" s="32" t="s">
         <v>1061</v>
       </c>
-      <c r="B172" s="30" t="s">
+      <c r="B172" s="29" t="s">
         <v>990</v>
       </c>
       <c r="C172" s="17" t="s">
@@ -17625,7 +17627,7 @@
       <c r="A173" t="s">
         <v>1062</v>
       </c>
-      <c r="B173" s="30" t="s">
+      <c r="B173" s="29" t="s">
         <v>991</v>
       </c>
       <c r="C173" s="17" t="s">
@@ -17642,7 +17644,7 @@
       <c r="A174" t="s">
         <v>1063</v>
       </c>
-      <c r="B174" s="30" t="s">
+      <c r="B174" s="29" t="s">
         <v>987</v>
       </c>
       <c r="C174" s="17" t="s">
@@ -17659,7 +17661,7 @@
       <c r="A175" t="s">
         <v>1064</v>
       </c>
-      <c r="B175" s="30" t="s">
+      <c r="B175" s="29" t="s">
         <v>987</v>
       </c>
       <c r="C175" s="17" t="s">
@@ -17673,7 +17675,7 @@
       </c>
     </row>
     <row r="176" spans="1:5">
-      <c r="A176" s="33" t="s">
+      <c r="A176" s="32" t="s">
         <v>1065</v>
       </c>
       <c r="B176" s="14" t="s">
@@ -17741,7 +17743,7 @@
       </c>
     </row>
     <row r="180" spans="1:5">
-      <c r="A180" s="33" t="s">
+      <c r="A180" s="32" t="s">
         <v>1069</v>
       </c>
       <c r="B180" s="14" t="s">
@@ -17792,7 +17794,7 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="33" t="s">
+      <c r="A183" s="32" t="s">
         <v>1072</v>
       </c>
       <c r="B183" s="14" t="s">
@@ -17877,7 +17879,7 @@
       </c>
     </row>
     <row r="188" spans="1:5">
-      <c r="A188" s="33" t="s">
+      <c r="A188" s="32" t="s">
         <v>1077</v>
       </c>
       <c r="B188" s="14" t="s">
@@ -17962,7 +17964,7 @@
       </c>
     </row>
     <row r="193" spans="1:5">
-      <c r="A193" s="33" t="s">
+      <c r="A193" s="32" t="s">
         <v>1082</v>
       </c>
       <c r="B193" s="14" t="s">
@@ -18064,7 +18066,7 @@
       </c>
     </row>
     <row r="199" spans="1:5">
-      <c r="A199" s="33" t="s">
+      <c r="A199" s="32" t="s">
         <v>1088</v>
       </c>
       <c r="B199" s="14" t="s">
@@ -18166,7 +18168,7 @@
       </c>
     </row>
     <row r="205" spans="1:5">
-      <c r="A205" s="33" t="s">
+      <c r="A205" s="32" t="s">
         <v>1094</v>
       </c>
       <c r="B205" s="14" t="s">
@@ -18234,7 +18236,7 @@
       </c>
     </row>
     <row r="209" spans="1:5">
-      <c r="A209" s="33" t="s">
+      <c r="A209" s="32" t="s">
         <v>1098</v>
       </c>
       <c r="B209" s="14" t="s">
@@ -18302,7 +18304,7 @@
       </c>
     </row>
     <row r="213" spans="1:5">
-      <c r="A213" s="33" t="s">
+      <c r="A213" s="32" t="s">
         <v>1102</v>
       </c>
       <c r="B213" s="14" t="s">
@@ -18387,7 +18389,7 @@
       </c>
     </row>
     <row r="218" spans="1:5">
-      <c r="A218" s="33" t="s">
+      <c r="A218" s="32" t="s">
         <v>1107</v>
       </c>
       <c r="B218" s="14" t="s">
@@ -18455,7 +18457,7 @@
       </c>
     </row>
     <row r="222" spans="1:5">
-      <c r="A222" s="33" t="s">
+      <c r="A222" s="32" t="s">
         <v>1111</v>
       </c>
       <c r="B222" s="14" t="s">
@@ -18540,7 +18542,7 @@
       </c>
     </row>
     <row r="227" spans="1:5">
-      <c r="A227" s="33" t="s">
+      <c r="A227" s="32" t="s">
         <v>1116</v>
       </c>
       <c r="B227" s="14" t="s">
@@ -18608,10 +18610,10 @@
       </c>
     </row>
     <row r="231" spans="1:5">
-      <c r="A231" s="33" t="s">
+      <c r="A231" s="32" t="s">
         <v>1120</v>
       </c>
-      <c r="B231" s="32" t="s">
+      <c r="B231" s="31" t="s">
         <v>1035</v>
       </c>
       <c r="C231" s="17" t="s">
@@ -18628,7 +18630,7 @@
       <c r="A232" t="s">
         <v>1121</v>
       </c>
-      <c r="B232" s="32" t="s">
+      <c r="B232" s="31" t="s">
         <v>1030</v>
       </c>
       <c r="C232" s="17" t="s">
@@ -18645,7 +18647,7 @@
       <c r="A233" t="s">
         <v>1122</v>
       </c>
-      <c r="B233" s="32" t="s">
+      <c r="B233" s="31" t="s">
         <v>1036</v>
       </c>
       <c r="C233" s="17" t="s">
@@ -18662,7 +18664,7 @@
       <c r="A234" t="s">
         <v>1123</v>
       </c>
-      <c r="B234" s="32" t="s">
+      <c r="B234" s="31" t="s">
         <v>987</v>
       </c>
       <c r="C234" s="17" t="s">

</xml_diff>

<commit_message>
add default krys for feedback to make the addition of the strings easier
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17263" windowHeight="5580" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17263" windowHeight="5580" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5090" uniqueCount="1665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6440" uniqueCount="1695">
   <si>
     <t>XXXX</t>
   </si>
@@ -5723,6 +5723,96 @@
   </si>
   <si>
     <t>Resumen del final del turno</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_14_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_14_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_14_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_16_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_16_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_16_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_17_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_17_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_17_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_18_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_18_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_18_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_CITIZEN_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_20_WAIT_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_20_OFFICER_FEEDBACK_1</t>
+  </si>
+  <si>
+    <t>SCENARIO_20_CITIZEN_FEEDBACK_1</t>
   </si>
 </sst>
 </file>
@@ -6288,10 +6378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E262"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E262" sqref="A203:E262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -9738,6 +9828,1026 @@
         <v>0</v>
       </c>
     </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="32" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="32" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="32" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="1" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="1" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="32" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="1" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="32" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="1" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="32" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="1" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="1" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="32" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" s="1" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" s="32" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" s="1" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" s="32" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" s="1" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" s="32" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" s="1" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" s="32" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" s="32" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239" s="32" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" s="32" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245" s="32" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" s="32" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" s="32" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5">
+      <c r="A253" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
+      <c r="A254" s="32" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5">
+      <c r="A255" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
+      <c r="A256" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5">
+      <c r="A257" s="32" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
+      <c r="A258" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5">
+      <c r="A260" s="32" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5">
+      <c r="A261" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5">
+      <c r="A262" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9746,10 +10856,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -10546,6 +11656,1026 @@
         <v>0</v>
       </c>
     </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="32" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="32" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="32" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="32" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="32" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="32" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="32" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="32" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="32" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="32" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="32" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="32" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="32" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="32" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="32" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="32" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="32" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="32" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="32" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="32" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10553,10 +12683,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145:E204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -13018,6 +15148,1026 @@
         <v>0</v>
       </c>
     </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="32" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="32" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="32" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="1" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="1" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="32" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="1" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="32" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="1" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="32" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="1" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="1" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="32" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="1" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="32" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="1" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="32" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="1" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="32" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="1" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="32" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="32" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="32" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="32" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="32" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="32" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="32" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="32" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="32" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="32" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13029,7 +16179,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
@@ -15232,10 +18382,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q267"/>
+  <dimension ref="A1:Q294"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I252" sqref="I251:I252"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I260" sqref="I260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -20016,11 +23166,21 @@
       <c r="H264"/>
     </row>
     <row r="265" spans="1:17">
-      <c r="A265"/>
-      <c r="B265"/>
-      <c r="C265"/>
-      <c r="D265"/>
-      <c r="E265"/>
+      <c r="A265" s="32" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F265"/>
       <c r="G265"/>
       <c r="H265"/>
@@ -20035,11 +23195,21 @@
       <c r="Q265"/>
     </row>
     <row r="266" spans="1:17">
-      <c r="A266"/>
-      <c r="B266"/>
-      <c r="C266"/>
-      <c r="D266"/>
-      <c r="E266"/>
+      <c r="A266" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F266"/>
       <c r="G266"/>
       <c r="H266"/>
@@ -20054,11 +23224,21 @@
       <c r="Q266"/>
     </row>
     <row r="267" spans="1:17">
-      <c r="A267"/>
-      <c r="B267"/>
-      <c r="C267"/>
-      <c r="D267"/>
-      <c r="E267"/>
+      <c r="A267" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F267"/>
       <c r="G267"/>
       <c r="H267"/>
@@ -20072,6 +23252,465 @@
       <c r="P267"/>
       <c r="Q267"/>
     </row>
+    <row r="268" spans="1:17">
+      <c r="A268" s="32" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:17">
+      <c r="A269" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:17">
+      <c r="A270" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:17">
+      <c r="A271" s="32" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:17">
+      <c r="A272" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5">
+      <c r="A274" s="32" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5">
+      <c r="A275" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5">
+      <c r="A276" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5">
+      <c r="A277" s="32" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5">
+      <c r="A278" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5">
+      <c r="A279" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5">
+      <c r="A280" s="32" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5">
+      <c r="A281" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5">
+      <c r="A282" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5">
+      <c r="A283" s="32" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5">
+      <c r="A284" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5">
+      <c r="A285" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5">
+      <c r="A286" s="32" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5">
+      <c r="A287" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5">
+      <c r="A288" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5">
+      <c r="A289" s="32" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5">
+      <c r="A290" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5">
+      <c r="A291" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5">
+      <c r="A292" s="32" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5">
+      <c r="A293" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5">
+      <c r="A294" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20079,10 +23718,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E294"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149:XFD149"/>
+    <sheetView topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="E294" sqref="A265:E294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -24073,6 +27712,1026 @@
         <v>0</v>
       </c>
     </row>
+    <row r="235" spans="1:5">
+      <c r="A235" s="32" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" s="32" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" s="32" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" s="1" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" s="1" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" s="32" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246" s="1" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" s="32" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" s="1" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" s="32" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" s="1" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" s="1" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5">
+      <c r="A253" s="32" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
+      <c r="A254" s="1" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5">
+      <c r="A255" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
+      <c r="A256" s="32" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5">
+      <c r="A257" s="1" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
+      <c r="A258" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" s="32" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5">
+      <c r="A260" s="1" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5">
+      <c r="A261" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5">
+      <c r="A262" s="32" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" s="1" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5">
+      <c r="A264" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" s="32" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" s="32" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" s="32" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5">
+      <c r="A274" s="32" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5">
+      <c r="A275" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5">
+      <c r="A276" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5">
+      <c r="A277" s="32" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5">
+      <c r="A278" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5">
+      <c r="A279" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5">
+      <c r="A280" s="32" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5">
+      <c r="A281" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5">
+      <c r="A282" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5">
+      <c r="A283" s="32" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5">
+      <c r="A284" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5">
+      <c r="A285" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5">
+      <c r="A286" s="32" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5">
+      <c r="A287" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5">
+      <c r="A288" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5">
+      <c r="A289" s="32" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5">
+      <c r="A290" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5">
+      <c r="A291" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5">
+      <c r="A292" s="32" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5">
+      <c r="A293" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5">
+      <c r="A294" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add updated Nicosia scenarios
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17263" windowHeight="5580" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17263" windowHeight="5580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6275" uniqueCount="1596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6630" uniqueCount="1704">
   <si>
     <t>XXXX</t>
   </si>
@@ -5517,12 +5517,384 @@
   <si>
     <t>{0}% Citizen Satisfaction*n*Keep the valude above 10% by making good choices</t>
   </si>
+  <si>
+    <t>SCENARIO_1_OFFICER_FEEDBACK_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_CITIZEN_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_WAIT_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_OFFICER_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_WAIT_FEEDBACK_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_OFFICER_FEEDBACK_7</t>
+  </si>
+  <si>
+    <t>SCENARIO_1_WAIT_FEEDBACK_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well this is quite common in this neighborhood… I do not blame you for holding off for a bit. </t>
+  </si>
+  <si>
+    <t>Great choice, this case is likely to be resolved soon</t>
+  </si>
+  <si>
+    <t>There is yet another hint, something might be going on here</t>
+  </si>
+  <si>
+    <t>You should be more responsive. It seems that things are going out of hand.</t>
+  </si>
+  <si>
+    <t>Requesting for citizen information is a great idea. The neighbors could shed some light to the situation.</t>
+  </si>
+  <si>
+    <t>You must do something very shortly</t>
+  </si>
+  <si>
+    <t>Better late than never. Sending officers earlier could help reserving some precious resources</t>
+  </si>
+  <si>
+    <t>Your lack of action can lead the event escalating to a highest rank.</t>
+  </si>
+  <si>
+    <t>The event will likely escalate now and will take substantial resources to set things under control</t>
+  </si>
+  <si>
+    <t>Well requesting citizen information at this stage is a waste of precious time. Take action!</t>
+  </si>
+  <si>
+    <t>It seems that you don’t care at all about your citizens</t>
+  </si>
+  <si>
+    <t>Ok, officers will be able to help the situation</t>
+  </si>
+  <si>
+    <t>Events are still happening, waiting for progress may be a good choice, or could escalate further</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You are running out of chances to find the kid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>You have to hope the kid is found successfully</t>
+  </si>
+  <si>
+    <t>SCENARIO_2_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>This seems to be reasonable action. You might be reserving resources for later incidents but being on top of things is very important</t>
+  </si>
+  <si>
+    <t>Being proactive is the best practice</t>
+  </si>
+  <si>
+    <t>Take action promptly. Things could easily get out of hand</t>
+  </si>
+  <si>
+    <t>Great choice. This incident seems to be trivial not many resources are needed.</t>
+  </si>
+  <si>
+    <t>Hmm you have turned a simple situation into something unmanageable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well things didn’t turn out as good.  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Great choice. This incident seems to be trivial not many resources are needed. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>SCENARIO_3_WAIT_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_WAIT_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_3_OFFICER_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>An incident like this might impose significant health danger</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It was tough call but you did an excellent job </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Think about your decisions, bad decisions will cost you the game</t>
+  </si>
+  <si>
+    <t>Well this is quite a commitment, but I’m sure it will turn out for the good.</t>
+  </si>
+  <si>
+    <t>This is an excellent call. Citizens may provide very useful information</t>
+  </si>
+  <si>
+    <t>We are almost there. Keep it up</t>
+  </si>
+  <si>
+    <t>You might not be cut out for this at the end of the day.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wow that was truly impressive </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>SCENARIO_4_OFFICER_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>Ignoring reported incidents is never a good idea, they could easily escalate out of hand</t>
+  </si>
+  <si>
+    <t>Good Choice, under these circumstances this seems to be the most appropriate choice</t>
+  </si>
+  <si>
+    <t>Keep ignoring and citizens will not be very happy with you.</t>
+  </si>
+  <si>
+    <t>Sending an officer now seems to be a good choice. This could lead to a resolution</t>
+  </si>
+  <si>
+    <t>Asking citizens for information under these circumstances seems to be a great choice</t>
+  </si>
+  <si>
+    <t>Waiting is your only option as you need more information</t>
+  </si>
+  <si>
+    <t>Questionable choice</t>
+  </si>
+  <si>
+    <t>SCENARIO_5_CITIZEN_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>You may not think that this case is an urgent incident, but things could escalate quikcly</t>
+  </si>
+  <si>
+    <t>Sending an officer seems reasonable, It could help to keep everyone happy</t>
+  </si>
+  <si>
+    <t>I don’t think citizens will be happy with your choices</t>
+  </si>
+  <si>
+    <t>At this time, this appears to be the best choice, but previous actions did not impress the public</t>
+  </si>
+  <si>
+    <t>Try valuing the citizens' opinions next time. Keeping the public informed does not cost anything</t>
+  </si>
+  <si>
+    <t>Excellent, this will help at resolving the case</t>
+  </si>
+  <si>
+    <t>Good choice, citizens will appreciate your efforts in keeping them informed</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>You may not have thought this is an urgent incident, but the substance could endanger the lives of citizens</t>
+  </si>
+  <si>
+    <t>Great choice, its worth dedicating some resources to the incident</t>
+  </si>
+  <si>
+    <t>The case is likely to get out of hand as a result of ignoring it</t>
+  </si>
+  <si>
+    <t>Interesting, 3 officers is quite a lot to use here, next time try using citizen help</t>
+  </si>
+  <si>
+    <t>That was probably the best option.</t>
+  </si>
+  <si>
+    <t>You have done a great job so far, keep it up.</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_CITIZEN_FEEDBACK_8</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_OFFICER_FEEDBACK_9</t>
+  </si>
+  <si>
+    <t>Great option, it is very important to investigate even seemingly simple cases</t>
+  </si>
+  <si>
+    <t>Things are getting out of hand, was that really the best decision?</t>
+  </si>
+  <si>
+    <t>Good job, you cannot hold off the incident any more</t>
+  </si>
+  <si>
+    <t>Excellent choice</t>
+  </si>
+  <si>
+    <t>Great, things will now get worse</t>
+  </si>
+  <si>
+    <t>It might not be too late, but citizens will be disappointed.</t>
+  </si>
+  <si>
+    <t>Using your resources here was a good decision</t>
+  </si>
+  <si>
+    <t>That seems to be a reasonable choice, saving resources by asking citzens could help you elsewhere</t>
+  </si>
+  <si>
+    <t>If you keep ignoring citizens' reports, they will no longer trust you</t>
+  </si>
+  <si>
+    <t>Good job, you have chosen well</t>
+  </si>
+  <si>
+    <t>SCENARIO_8_OFFICER_FEEDBACK_7</t>
+  </si>
+  <si>
+    <t>Really? Is this the best you can do? Eved if you didn’t have the resources you could communicated with citizens</t>
+  </si>
+  <si>
+    <t>Great, citizen safety is priority</t>
+  </si>
+  <si>
+    <t>This is OK</t>
+  </si>
+  <si>
+    <t>You should make sure to have officers available to help solve incidents</t>
+  </si>
+  <si>
+    <t>Great, citizens will appreciate your presence.</t>
+  </si>
+  <si>
+    <t>This seems to be a reasonable action, you might want to save resources for other incidents</t>
+  </si>
+  <si>
+    <t>You did well to handle this case</t>
+  </si>
+  <si>
+    <t>Excellent, you made really good decisions on this case</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_WAIT_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_OFFICER_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_WAIT_FEEDBACK_8</t>
+  </si>
+  <si>
+    <t>SCENARIO_9_OFFICER_FEEDBACK_8</t>
+  </si>
+  <si>
+    <t>Is that the best you can do?</t>
+  </si>
+  <si>
+    <t>OK, not the best choice but not the worst either</t>
+  </si>
+  <si>
+    <t>You don't have sufficient information to make a call to send officers</t>
+  </si>
+  <si>
+    <t>Good choice, citizen input may provide valuable information</t>
+  </si>
+  <si>
+    <t>Ok, this could potentially save time</t>
+  </si>
+  <si>
+    <t>Collaborating with citizen intelligence has prover helpful previously</t>
+  </si>
+  <si>
+    <t>Things have not gone very well on this case</t>
+  </si>
+  <si>
+    <t>Excellent , you make great decisions on this case</t>
+  </si>
+  <si>
+    <t>SCENARIO_10_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>Quickly ignoring incidents may not have been the best idea</t>
+  </si>
+  <si>
+    <t>Ok, but seeking citizen participation could assist in this case</t>
+  </si>
+  <si>
+    <t>Excellent, this could save you some resources</t>
+  </si>
+  <si>
+    <t>Really? Is this the best you can do? Eved if you didn’t have the resources you could have communicated with citizens</t>
+  </si>
+  <si>
+    <t>Good choice,  a citizen's life might be on the line</t>
+  </si>
+  <si>
+    <t>That’s a shame, a citizens' life could be on the line</t>
+  </si>
+  <si>
+    <t>Ok, waiting for the case to close will save resources</t>
+  </si>
+  <si>
+    <t>Great! You chose wisely for this case, citizens are happy with your actions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5634,6 +6006,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -5673,7 +6052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5792,6 +6171,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -12378,10 +12763,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F204"/>
+  <dimension ref="A1:F275"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145:E204"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -13942,11 +14327,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:5" customFormat="1">
-      <c r="A92" s="31" t="s">
+    <row r="92" spans="1:5">
+      <c r="A92" s="3" t="s">
         <v>936</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>1023</v>
       </c>
       <c r="C92" s="22" t="s">
@@ -13959,11 +14344,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" customFormat="1">
-      <c r="A93" t="s">
+    <row r="93" spans="1:5">
+      <c r="A93" s="1" t="s">
         <v>938</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>1023</v>
       </c>
       <c r="C93" s="22" t="s">
@@ -13976,11 +14361,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" customFormat="1">
-      <c r="A94" t="s">
+    <row r="94" spans="1:5">
+      <c r="A94" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>1024</v>
       </c>
       <c r="C94" s="22" t="s">
@@ -13993,11 +14378,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" customFormat="1">
-      <c r="A95" t="s">
+    <row r="95" spans="1:5">
+      <c r="A95" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>1025</v>
       </c>
       <c r="C95" s="22" t="s">
@@ -14010,11 +14395,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" customFormat="1">
-      <c r="A96" t="s">
+    <row r="96" spans="1:5">
+      <c r="A96" s="1" t="s">
         <v>1047</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>1026</v>
       </c>
       <c r="C96" s="22" t="s">
@@ -14027,11 +14412,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:5" customFormat="1">
-      <c r="A97" t="s">
+    <row r="97" spans="1:5">
+      <c r="A97" s="1" t="s">
         <v>1048</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>1027</v>
       </c>
       <c r="C97" s="22" t="s">
@@ -14044,11 +14429,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" customFormat="1">
-      <c r="A98" t="s">
+    <row r="98" spans="1:5">
+      <c r="A98" s="1" t="s">
         <v>1049</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>1028</v>
       </c>
       <c r="C98" s="22" t="s">
@@ -14061,11 +14446,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:5" customFormat="1">
-      <c r="A99" t="s">
+    <row r="99" spans="1:5">
+      <c r="A99" s="1" t="s">
         <v>1050</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>1029</v>
       </c>
       <c r="C99" s="22" t="s">
@@ -14078,11 +14463,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5" customFormat="1">
-      <c r="A100" s="31" t="s">
+    <row r="100" spans="1:5">
+      <c r="A100" s="3" t="s">
         <v>941</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>1030</v>
       </c>
       <c r="C100" s="22" t="s">
@@ -14095,11 +14480,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" customFormat="1">
-      <c r="A101" t="s">
+    <row r="101" spans="1:5">
+      <c r="A101" s="1" t="s">
         <v>942</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
         <v>1031</v>
       </c>
       <c r="C101" s="22" t="s">
@@ -14112,11 +14497,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" customFormat="1">
-      <c r="A102" t="s">
+    <row r="102" spans="1:5">
+      <c r="A102" s="1" t="s">
         <v>943</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="1" t="s">
         <v>1030</v>
       </c>
       <c r="C102" s="22" t="s">
@@ -14129,11 +14514,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5" customFormat="1">
-      <c r="A103" t="s">
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="1" t="s">
         <v>1032</v>
       </c>
       <c r="C103" s="22" t="s">
@@ -14146,11 +14531,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" customFormat="1">
-      <c r="A104" t="s">
+    <row r="104" spans="1:5">
+      <c r="A104" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="1" t="s">
         <v>1033</v>
       </c>
       <c r="C104" s="22" t="s">
@@ -14163,11 +14548,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" customFormat="1">
-      <c r="A105" s="31" t="s">
+    <row r="105" spans="1:5">
+      <c r="A105" s="3" t="s">
         <v>945</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="1" t="s">
         <v>1034</v>
       </c>
       <c r="C105" s="22" t="s">
@@ -14180,11 +14565,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" customFormat="1">
-      <c r="A106" t="s">
+    <row r="106" spans="1:5">
+      <c r="A106" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="1" t="s">
         <v>1035</v>
       </c>
       <c r="C106" s="22" t="s">
@@ -14197,11 +14582,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" customFormat="1">
-      <c r="A107" t="s">
+    <row r="107" spans="1:5">
+      <c r="A107" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="1" t="s">
         <v>1036</v>
       </c>
       <c r="C107" s="22" t="s">
@@ -14214,11 +14599,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:5" customFormat="1">
-      <c r="A108" t="s">
+    <row r="108" spans="1:5">
+      <c r="A108" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="1" t="s">
         <v>872</v>
       </c>
       <c r="C108" s="22" t="s">
@@ -14231,11 +14616,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5" customFormat="1">
-      <c r="A109" t="s">
+    <row r="109" spans="1:5">
+      <c r="A109" s="1" t="s">
         <v>1053</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="1" t="s">
         <v>1037</v>
       </c>
       <c r="C109" s="22" t="s">
@@ -14248,11 +14633,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" customFormat="1">
-      <c r="A110" t="s">
+    <row r="110" spans="1:5">
+      <c r="A110" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="1" t="s">
         <v>1038</v>
       </c>
       <c r="C110" s="22" t="s">
@@ -14265,11 +14650,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" customFormat="1">
-      <c r="A111" t="s">
+    <row r="111" spans="1:5">
+      <c r="A111" s="1" t="s">
         <v>1055</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="s">
         <v>1039</v>
       </c>
       <c r="C111" s="22" t="s">
@@ -14282,11 +14667,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" customFormat="1">
-      <c r="A112" t="s">
+    <row r="112" spans="1:5">
+      <c r="A112" s="1" t="s">
         <v>1056</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="1" t="s">
         <v>1040</v>
       </c>
       <c r="C112" s="22" t="s">
@@ -14299,11 +14684,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5" customFormat="1">
-      <c r="A113" s="31" t="s">
+    <row r="113" spans="1:5">
+      <c r="A113" s="3" t="s">
         <v>949</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="1" t="s">
         <v>1041</v>
       </c>
       <c r="C113" s="22" t="s">
@@ -14316,11 +14701,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" customFormat="1">
-      <c r="A114" t="s">
+    <row r="114" spans="1:5">
+      <c r="A114" s="1" t="s">
         <v>950</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="1" t="s">
         <v>1041</v>
       </c>
       <c r="C114" s="22" t="s">
@@ -14333,11 +14718,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5" customFormat="1">
-      <c r="A115" t="s">
+    <row r="115" spans="1:5">
+      <c r="A115" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="1" t="s">
         <v>1041</v>
       </c>
       <c r="C115" s="22" t="s">
@@ -14350,11 +14735,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" customFormat="1">
-      <c r="A116" t="s">
+    <row r="116" spans="1:5">
+      <c r="A116" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="1" t="s">
         <v>1041</v>
       </c>
       <c r="C116" s="22" t="s">
@@ -14367,11 +14752,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" customFormat="1">
-      <c r="A117" s="31" t="s">
+    <row r="117" spans="1:5">
+      <c r="A117" s="3" t="s">
         <v>953</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="1" t="s">
         <v>1042</v>
       </c>
       <c r="C117" s="22" t="s">
@@ -14384,11 +14769,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" customFormat="1">
-      <c r="A118" t="s">
+    <row r="118" spans="1:5">
+      <c r="A118" s="1" t="s">
         <v>954</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="1" t="s">
         <v>1042</v>
       </c>
       <c r="C118" s="22" t="s">
@@ -14401,11 +14786,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" customFormat="1">
-      <c r="A119" t="s">
+    <row r="119" spans="1:5">
+      <c r="A119" s="1" t="s">
         <v>955</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="1" t="s">
         <v>1042</v>
       </c>
       <c r="C119" s="22" t="s">
@@ -14418,11 +14803,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" customFormat="1">
-      <c r="A120" s="31" t="s">
+    <row r="120" spans="1:5">
+      <c r="A120" s="3" t="s">
         <v>957</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="s">
         <v>1043</v>
       </c>
       <c r="C120" s="22" t="s">
@@ -14435,11 +14820,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5" customFormat="1">
-      <c r="A121" t="s">
+    <row r="121" spans="1:5">
+      <c r="A121" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="1" t="s">
         <v>1043</v>
       </c>
       <c r="C121" s="22" t="s">
@@ -14452,11 +14837,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:5" customFormat="1">
-      <c r="A122" t="s">
+    <row r="122" spans="1:5">
+      <c r="A122" s="1" t="s">
         <v>959</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="1" t="s">
         <v>1043</v>
       </c>
       <c r="C122" s="22" t="s">
@@ -14469,11 +14854,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" customFormat="1">
-      <c r="A123" t="s">
+    <row r="123" spans="1:5">
+      <c r="A123" s="1" t="s">
         <v>1057</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="1" t="s">
         <v>1043</v>
       </c>
       <c r="C123" s="22" t="s">
@@ -14486,11 +14871,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" customFormat="1">
-      <c r="A124" s="31" t="s">
+    <row r="124" spans="1:5">
+      <c r="A124" s="3" t="s">
         <v>960</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="1" t="s">
         <v>1044</v>
       </c>
       <c r="C124" s="22" t="s">
@@ -14503,11 +14888,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5" customFormat="1">
-      <c r="A125" t="s">
+    <row r="125" spans="1:5">
+      <c r="A125" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="1" t="s">
         <v>1044</v>
       </c>
       <c r="C125" s="22" t="s">
@@ -14520,11 +14905,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" customFormat="1">
-      <c r="A126" t="s">
+    <row r="126" spans="1:5">
+      <c r="A126" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="1" t="s">
         <v>1044</v>
       </c>
       <c r="C126" s="22" t="s">
@@ -14537,11 +14922,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5" customFormat="1">
-      <c r="A127" t="s">
+    <row r="127" spans="1:5">
+      <c r="A127" s="1" t="s">
         <v>1058</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="1" t="s">
         <v>1044</v>
       </c>
       <c r="C127" s="22" t="s">
@@ -14554,11 +14939,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:5" customFormat="1">
-      <c r="A128" t="s">
+    <row r="128" spans="1:5">
+      <c r="A128" s="1" t="s">
         <v>1060</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="1" t="s">
         <v>1044</v>
       </c>
       <c r="C128" s="22" t="s">
@@ -14571,11 +14956,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" customFormat="1">
-      <c r="A129" t="s">
+    <row r="129" spans="1:5">
+      <c r="A129" s="1" t="s">
         <v>1061</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="1" t="s">
         <v>1044</v>
       </c>
       <c r="C129" s="22" t="s">
@@ -14588,11 +14973,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:5" customFormat="1">
-      <c r="A130" s="31" t="s">
+    <row r="130" spans="1:5">
+      <c r="A130" s="3" t="s">
         <v>964</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="1" t="s">
         <v>926</v>
       </c>
       <c r="C130" s="22" t="s">
@@ -14605,11 +14990,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:5" customFormat="1">
-      <c r="A131" t="s">
+    <row r="131" spans="1:5">
+      <c r="A131" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="1" t="s">
         <v>926</v>
       </c>
       <c r="C131" s="22" t="s">
@@ -14622,11 +15007,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" customFormat="1">
-      <c r="A132" t="s">
+    <row r="132" spans="1:5">
+      <c r="A132" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="1" t="s">
         <v>926</v>
       </c>
       <c r="C132" s="22" t="s">
@@ -14639,11 +15024,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5" customFormat="1">
-      <c r="A133" t="s">
+    <row r="133" spans="1:5">
+      <c r="A133" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="1" t="s">
         <v>926</v>
       </c>
       <c r="C133" s="22" t="s">
@@ -14656,11 +15041,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" customFormat="1">
-      <c r="A134" s="31" t="s">
+    <row r="134" spans="1:5">
+      <c r="A134" s="3" t="s">
         <v>968</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="C134" s="22" t="s">
@@ -14673,11 +15058,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" customFormat="1">
-      <c r="A135" t="s">
+    <row r="135" spans="1:5">
+      <c r="A135" s="1" t="s">
         <v>969</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="C135" s="22" t="s">
@@ -14690,11 +15075,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:5" customFormat="1">
-      <c r="A136" t="s">
+    <row r="136" spans="1:5">
+      <c r="A136" s="1" t="s">
         <v>970</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="C136" s="22" t="s">
@@ -14707,11 +15092,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" customFormat="1">
-      <c r="A137" t="s">
+    <row r="137" spans="1:5">
+      <c r="A137" s="1" t="s">
         <v>1066</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="C137" s="22" t="s">
@@ -14724,11 +15109,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" customFormat="1">
-      <c r="A138" t="s">
+    <row r="138" spans="1:5">
+      <c r="A138" s="1" t="s">
         <v>1067</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="C138" s="22" t="s">
@@ -14741,11 +15126,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:5" customFormat="1">
-      <c r="A139" t="s">
+    <row r="139" spans="1:5">
+      <c r="A139" s="1" t="s">
         <v>1068</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="C139" s="22" t="s">
@@ -14758,11 +15143,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" customFormat="1">
-      <c r="A140" s="31" t="s">
+    <row r="140" spans="1:5">
+      <c r="A140" s="3" t="s">
         <v>971</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="1" t="s">
         <v>1046</v>
       </c>
       <c r="C140" s="22" t="s">
@@ -14775,11 +15160,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5" customFormat="1">
-      <c r="A141" t="s">
+    <row r="141" spans="1:5">
+      <c r="A141" s="1" t="s">
         <v>973</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="1" t="s">
         <v>1046</v>
       </c>
       <c r="C141" s="22" t="s">
@@ -14792,11 +15177,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:5" customFormat="1">
-      <c r="A142" t="s">
+    <row r="142" spans="1:5">
+      <c r="A142" s="1" t="s">
         <v>974</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="1" t="s">
         <v>1046</v>
       </c>
       <c r="C142" s="22" t="s">
@@ -14809,11 +15194,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" customFormat="1">
-      <c r="A143" t="s">
+    <row r="143" spans="1:5">
+      <c r="A143" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="1" t="s">
         <v>1046</v>
       </c>
       <c r="C143" s="22" t="s">
@@ -14826,11 +15211,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:5" customFormat="1">
-      <c r="A144" t="s">
+    <row r="144" spans="1:5">
+      <c r="A144" s="1" t="s">
         <v>1069</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="1" t="s">
         <v>1045</v>
       </c>
       <c r="C144" s="22" t="s">
@@ -14843,12 +15228,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
-      <c r="A145" s="31" t="s">
+    <row r="145" spans="1:5" ht="29.15">
+      <c r="A145" s="3" t="s">
         <v>1108</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>0</v>
+      <c r="B145" s="42" t="s">
+        <v>1603</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>0</v>
@@ -14864,8 +15249,8 @@
       <c r="A146" s="1" t="s">
         <v>1111</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>0</v>
+      <c r="B146" s="42" t="s">
+        <v>1604</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>0</v>
@@ -14878,11 +15263,11 @@
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="1" t="s">
-        <v>1110</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>0</v>
+      <c r="A147" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B147" s="42" t="s">
+        <v>1605</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>0</v>
@@ -14895,11 +15280,11 @@
       </c>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="31" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>0</v>
+      <c r="A148" s="1" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B148" s="42" t="s">
+        <v>1604</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>0</v>
@@ -14911,12 +15296,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
-      <c r="A149" s="1" t="s">
-        <v>1128</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>0</v>
+    <row r="149" spans="1:5" ht="29.15">
+      <c r="A149" s="3" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B149" s="42" t="s">
+        <v>1606</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>0</v>
@@ -14930,10 +15315,10 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="1" t="s">
-        <v>1129</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>0</v>
+        <v>1117</v>
+      </c>
+      <c r="B150" s="42" t="s">
+        <v>1604</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>0</v>
@@ -14945,12 +15330,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
-      <c r="A151" s="31" t="s">
-        <v>1454</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>0</v>
+    <row r="151" spans="1:5" ht="29.15">
+      <c r="A151" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B151" s="43" t="s">
+        <v>1607</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>0</v>
@@ -14963,11 +15348,11 @@
       </c>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="1" t="s">
-        <v>1499</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>0</v>
+      <c r="A152" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B152" s="43" t="s">
+        <v>1608</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>0</v>
@@ -14979,12 +15364,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" ht="29.15">
       <c r="A153" s="1" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>0</v>
+        <v>1596</v>
+      </c>
+      <c r="B153" s="42" t="s">
+        <v>1609</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>0</v>
@@ -14997,11 +15382,11 @@
       </c>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="31" t="s">
-        <v>1459</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>0</v>
+      <c r="A154" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B154" s="43" t="s">
+        <v>1610</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>0</v>
@@ -15013,12 +15398,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" ht="29.15">
       <c r="A155" s="1" t="s">
-        <v>1500</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>0</v>
+        <v>1125</v>
+      </c>
+      <c r="B155" s="43" t="s">
+        <v>1611</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>0</v>
@@ -15030,12 +15415,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" ht="29.15">
       <c r="A156" s="1" t="s">
-        <v>1536</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>0</v>
+        <v>1597</v>
+      </c>
+      <c r="B156" s="43" t="s">
+        <v>1612</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>0</v>
@@ -15048,11 +15433,11 @@
       </c>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="31" t="s">
-        <v>1458</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>0</v>
+      <c r="A157" s="3" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B157" s="43" t="s">
+        <v>1613</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>0</v>
@@ -15066,10 +15451,10 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="1" t="s">
-        <v>1506</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>0</v>
+        <v>1599</v>
+      </c>
+      <c r="B158" s="42" t="s">
+        <v>1614</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>0</v>
@@ -15081,12 +15466,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="1" t="s">
-        <v>1539</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>0</v>
+    <row r="159" spans="1:5" ht="29.15">
+      <c r="A159" s="3" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B159" s="43" t="s">
+        <v>1615</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>0</v>
@@ -15099,11 +15484,11 @@
       </c>
     </row>
     <row r="160" spans="1:5">
-      <c r="A160" s="31" t="s">
-        <v>1465</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>0</v>
+      <c r="A160" s="1" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B160" s="43" t="s">
+        <v>1616</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>0</v>
@@ -15116,11 +15501,11 @@
       </c>
     </row>
     <row r="161" spans="1:5">
-      <c r="A161" s="1" t="s">
-        <v>1509</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>0</v>
+      <c r="A161" s="3" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B161" s="42" t="s">
+        <v>1617</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>0</v>
@@ -15132,12 +15517,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="1" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>0</v>
+    <row r="162" spans="1:5" ht="29.15">
+      <c r="A162" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B162" s="43" t="s">
+        <v>1619</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>0</v>
@@ -15149,12 +15534,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="31" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>0</v>
+    <row r="163" spans="1:5" ht="29.15">
+      <c r="A163" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B163" s="43" t="s">
+        <v>1625</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>0</v>
@@ -15167,11 +15552,11 @@
       </c>
     </row>
     <row r="164" spans="1:5">
-      <c r="A164" s="1" t="s">
-        <v>1513</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>0</v>
+      <c r="A164" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B164" s="43" t="s">
+        <v>1620</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>0</v>
@@ -15184,11 +15569,11 @@
       </c>
     </row>
     <row r="165" spans="1:5">
-      <c r="A165" s="1" t="s">
-        <v>1545</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>0</v>
+      <c r="A165" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B165" s="43" t="s">
+        <v>1621</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>0</v>
@@ -15200,12 +15585,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
-      <c r="A166" s="31" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>0</v>
+    <row r="166" spans="1:5" ht="29.15">
+      <c r="A166" s="1" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B166" s="43" t="s">
+        <v>1622</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>0</v>
@@ -15218,11 +15603,11 @@
       </c>
     </row>
     <row r="167" spans="1:5">
-      <c r="A167" s="1" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>0</v>
+      <c r="A167" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B167" s="42" t="s">
+        <v>1623</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>0</v>
@@ -15236,10 +15621,10 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="1" t="s">
-        <v>1550</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>0</v>
+        <v>1143</v>
+      </c>
+      <c r="B168" s="43" t="s">
+        <v>1624</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>0</v>
@@ -15252,11 +15637,11 @@
       </c>
     </row>
     <row r="169" spans="1:5">
-      <c r="A169" s="31" t="s">
-        <v>1487</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>0</v>
+      <c r="A169" s="3" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B169" s="43" t="s">
+        <v>1629</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>0</v>
@@ -15270,10 +15655,10 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="1" t="s">
-        <v>1525</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>0</v>
+        <v>1499</v>
+      </c>
+      <c r="B170" s="42" t="s">
+        <v>1630</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>0</v>
@@ -15286,11 +15671,11 @@
       </c>
     </row>
     <row r="171" spans="1:5">
-      <c r="A171" s="1" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>0</v>
+      <c r="A171" s="3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B171" s="42" t="s">
+        <v>1631</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>0</v>
@@ -15303,11 +15688,11 @@
       </c>
     </row>
     <row r="172" spans="1:5">
-      <c r="A172" s="31" t="s">
-        <v>1491</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>0</v>
+      <c r="A172" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B172" s="43" t="s">
+        <v>1632</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>0</v>
@@ -15321,10 +15706,10 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>1528</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>0</v>
+        <v>1535</v>
+      </c>
+      <c r="B173" s="42" t="s">
+        <v>1633</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>0</v>
@@ -15337,11 +15722,11 @@
       </c>
     </row>
     <row r="174" spans="1:5">
-      <c r="A174" s="1" t="s">
-        <v>1559</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>0</v>
+      <c r="A174" s="3" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B174" s="43" t="s">
+        <v>1634</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>0</v>
@@ -15354,11 +15739,11 @@
       </c>
     </row>
     <row r="175" spans="1:5">
-      <c r="A175" s="31" t="s">
-        <v>1565</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>0</v>
+      <c r="A175" s="3" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B175" s="43" t="s">
+        <v>1635</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>0</v>
@@ -15372,10 +15757,10 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>0</v>
+        <v>1628</v>
+      </c>
+      <c r="B176" s="42" t="s">
+        <v>1636</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>0</v>
@@ -15387,12 +15772,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="1" t="s">
-        <v>1567</v>
+    <row r="177" spans="1:5" ht="29.15">
+      <c r="A177" s="3" t="s">
+        <v>1459</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>0</v>
+        <v>1638</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>0</v>
@@ -15404,12 +15789,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="31" t="s">
-        <v>1568</v>
+    <row r="178" spans="1:5" ht="29.15">
+      <c r="A178" s="1" t="s">
+        <v>1500</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>0</v>
+        <v>1639</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>0</v>
@@ -15422,11 +15807,11 @@
       </c>
     </row>
     <row r="179" spans="1:5">
-      <c r="A179" s="1" t="s">
-        <v>1569</v>
+      <c r="A179" s="3" t="s">
+        <v>1460</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>0</v>
+        <v>1640</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>0</v>
@@ -15438,12 +15823,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" ht="29.15">
       <c r="A180" s="1" t="s">
-        <v>1570</v>
+        <v>1637</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>0</v>
+        <v>1641</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>0</v>
@@ -15455,12 +15840,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="31" t="s">
-        <v>1571</v>
+    <row r="181" spans="1:5" ht="29.15">
+      <c r="A181" s="1" t="s">
+        <v>1537</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>0</v>
+        <v>1642</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>0</v>
@@ -15473,11 +15858,11 @@
       </c>
     </row>
     <row r="182" spans="1:5">
-      <c r="A182" s="1" t="s">
-        <v>1573</v>
+      <c r="A182" s="3" t="s">
+        <v>1461</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>0</v>
+        <v>1643</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>0</v>
@@ -15490,11 +15875,11 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="1" t="s">
-        <v>1572</v>
+      <c r="A183" s="3" t="s">
+        <v>1462</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>0</v>
+        <v>1644</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>0</v>
@@ -15506,12 +15891,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="31" t="s">
-        <v>1574</v>
+    <row r="184" spans="1:5" ht="29.15">
+      <c r="A184" s="1" t="s">
+        <v>1503</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>0</v>
+        <v>1641</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>0</v>
@@ -15523,12 +15908,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="1" t="s">
-        <v>1575</v>
+    <row r="185" spans="1:5" ht="29.15">
+      <c r="A185" s="3" t="s">
+        <v>1458</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>0</v>
+        <v>1646</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>0</v>
@@ -15540,12 +15925,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" ht="29.15">
       <c r="A186" s="1" t="s">
-        <v>1576</v>
+        <v>1506</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>0</v>
+        <v>1647</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>0</v>
@@ -15558,11 +15943,11 @@
       </c>
     </row>
     <row r="187" spans="1:5">
-      <c r="A187" s="31" t="s">
-        <v>1577</v>
+      <c r="A187" s="3" t="s">
+        <v>1463</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>0</v>
+        <v>1648</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>0</v>
@@ -15574,12 +15959,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" ht="29.15">
       <c r="A188" s="1" t="s">
-        <v>1578</v>
+        <v>1507</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>0</v>
+        <v>1649</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>0</v>
@@ -15591,12 +15976,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="1" t="s">
-        <v>1579</v>
+    <row r="189" spans="1:5" ht="29.15">
+      <c r="A189" s="3" t="s">
+        <v>1464</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>0</v>
+        <v>1650</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>0</v>
@@ -15609,11 +15994,11 @@
       </c>
     </row>
     <row r="190" spans="1:5">
-      <c r="A190" s="31" t="s">
-        <v>1580</v>
+      <c r="A190" s="1" t="s">
+        <v>1508</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>0</v>
+        <v>1651</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>0</v>
@@ -15625,12 +16010,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" ht="29.15">
       <c r="A191" s="1" t="s">
-        <v>1581</v>
+        <v>1645</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>0</v>
+        <v>1652</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>0</v>
@@ -15642,12 +16027,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="1" t="s">
-        <v>1582</v>
+    <row r="192" spans="1:5" ht="29.15">
+      <c r="A192" s="3" t="s">
+        <v>1465</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>0</v>
+        <v>1654</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>0</v>
@@ -15660,11 +16045,11 @@
       </c>
     </row>
     <row r="193" spans="1:5">
-      <c r="A193" s="31" t="s">
-        <v>1583</v>
+      <c r="A193" s="1" t="s">
+        <v>1509</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>0</v>
+        <v>1655</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>0</v>
@@ -15676,12 +16061,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="1" t="s">
-        <v>1584</v>
+    <row r="194" spans="1:5" ht="29.15">
+      <c r="A194" s="3" t="s">
+        <v>1466</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>0</v>
+        <v>1654</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>0</v>
@@ -15695,10 +16080,10 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="1" t="s">
-        <v>1585</v>
+        <v>1510</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>0</v>
+        <v>1655</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>0</v>
@@ -15711,11 +16096,11 @@
       </c>
     </row>
     <row r="196" spans="1:5">
-      <c r="A196" s="31" t="s">
-        <v>1586</v>
+      <c r="A196" s="3" t="s">
+        <v>1467</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>0</v>
+        <v>1656</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>0</v>
@@ -15727,12 +16112,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" ht="29.15">
       <c r="A197" s="1" t="s">
-        <v>1587</v>
+        <v>1653</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>0</v>
+        <v>1657</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>0</v>
@@ -15746,10 +16131,10 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="1" t="s">
-        <v>1588</v>
+        <v>1543</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>0</v>
+        <v>1658</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>0</v>
@@ -15762,11 +16147,11 @@
       </c>
     </row>
     <row r="199" spans="1:5">
-      <c r="A199" s="31" t="s">
-        <v>1589</v>
+      <c r="A199" s="3" t="s">
+        <v>1468</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>0</v>
+        <v>1656</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>0</v>
@@ -15780,10 +16165,10 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1" t="s">
-        <v>1590</v>
+        <v>1511</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>0</v>
+        <v>1659</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>0</v>
@@ -15795,12 +16180,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="1" t="s">
-        <v>1591</v>
+    <row r="201" spans="1:5" ht="29.15">
+      <c r="A201" s="3" t="s">
+        <v>1470</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>0</v>
+        <v>1619</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>0</v>
@@ -15812,12 +16197,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="31" t="s">
-        <v>1592</v>
+    <row r="202" spans="1:5" ht="29.15">
+      <c r="A202" s="1" t="s">
+        <v>1513</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>0</v>
+        <v>1663</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>0</v>
@@ -15830,11 +16215,11 @@
       </c>
     </row>
     <row r="203" spans="1:5">
-      <c r="A203" s="1" t="s">
-        <v>1593</v>
+      <c r="A203" s="3" t="s">
+        <v>1471</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>0</v>
+        <v>1664</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>0</v>
@@ -15848,18 +16233,1225 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="1" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="3" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="1" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="3" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="1" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="29.15">
+      <c r="A210" s="1" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="3" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="1" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="29.15">
+      <c r="A213" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="3" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="1" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" ht="29.15">
+      <c r="A219" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="3" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" s="3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" s="3" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" s="1" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" s="3" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" s="1" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" s="3" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" s="3" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" s="3" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" s="1" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" s="1" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" ht="29.15">
+      <c r="A239" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" s="3" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" s="3" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246" s="3" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" s="1" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" s="3" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" s="1" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" s="3" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5">
+      <c r="A253" s="1" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
+      <c r="A254" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5">
+      <c r="A255" s="3" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
+      <c r="A256" s="1" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5">
+      <c r="A257" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
+      <c r="A258" s="3" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5">
+      <c r="A260" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5">
+      <c r="A261" s="3" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5">
+      <c r="A262" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5">
+      <c r="A264" s="3" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" s="3" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" s="1" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" s="3" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" s="1" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" s="1" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="3" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5">
+      <c r="A274" s="1" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5">
+      <c r="A275" s="1" t="s">
         <v>1594</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D204" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E204" s="1" t="s">
+      <c r="B275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E275" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15874,7 +17466,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change game over to contain more information on the players' game and add score accordingly
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6630" uniqueCount="1704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6640" uniqueCount="1710">
   <si>
     <t>XXXX</t>
   </si>
@@ -5888,6 +5888,24 @@
   </si>
   <si>
     <t>Casos cerrados</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CASES_CLOSED_POSITIVE</t>
+  </si>
+  <si>
+    <t>Cases Closed Positively</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CASES_CLOSED_NEGATIVE</t>
+  </si>
+  <si>
+    <t>Cases Closed Negatively</t>
+  </si>
+  <si>
+    <t>Casos cerrados positivamente</t>
+  </si>
+  <si>
+    <t>Casos cerrados negativamente</t>
   </si>
 </sst>
 </file>
@@ -17464,10 +17482,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
@@ -18043,1055 +18061,1089 @@
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1">
       <c r="A34" s="7" t="s">
-        <v>451</v>
+        <v>1704</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>346</v>
+        <v>1705</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>346</v>
+        <v>1705</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="s">
-        <v>480</v>
+      <c r="E34" s="38" t="s">
+        <v>1708</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1">
       <c r="A35" s="7" t="s">
-        <v>97</v>
+        <v>1706</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>98</v>
+        <v>1707</v>
       </c>
       <c r="C35" s="40" t="s">
-        <v>98</v>
+        <v>1707</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>417</v>
+      <c r="E35" s="38" t="s">
+        <v>1709</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="7" customFormat="1">
       <c r="A36" s="7" t="s">
-        <v>99</v>
+        <v>451</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>100</v>
+        <v>346</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>100</v>
+        <v>346</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E36" s="10" t="s">
-        <v>418</v>
+      <c r="E36" s="12" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="7" customFormat="1">
       <c r="A37" s="7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="7" customFormat="1">
       <c r="A38" s="7" t="s">
-        <v>344</v>
+        <v>99</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>345</v>
+        <v>100</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>345</v>
+        <v>100</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E38" s="11" t="s">
-        <v>479</v>
+      <c r="E38" s="10" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1">
       <c r="A39" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="7" customFormat="1">
       <c r="A40" s="7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>447</v>
+        <v>345</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>447</v>
+        <v>345</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="10" t="s">
-        <v>421</v>
+      <c r="E40" s="11" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="7" customFormat="1">
       <c r="A41" s="7" t="s">
-        <v>349</v>
+        <v>96</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>353</v>
+        <v>95</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>353</v>
+        <v>95</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="7" customFormat="1">
       <c r="A42" s="7" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>354</v>
+        <v>447</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>354</v>
+        <v>447</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1">
       <c r="A43" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="7" customFormat="1">
       <c r="A44" s="7" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="7" customFormat="1">
       <c r="A45" s="7" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="7" customFormat="1">
       <c r="A46" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E46" s="12" t="s">
-        <v>427</v>
+      <c r="E46" s="10" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1">
       <c r="A47" s="7" t="s">
-        <v>448</v>
+        <v>361</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>449</v>
+        <v>362</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>449</v>
+        <v>362</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E47" s="12" t="s">
-        <v>478</v>
+      <c r="E47" s="10" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1">
       <c r="A48" s="7" t="s">
-        <v>1212</v>
+        <v>363</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>1232</v>
+        <v>364</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>1232</v>
+        <v>364</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="38" t="s">
-        <v>1233</v>
+      <c r="E48" s="12" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1">
       <c r="A49" s="7" t="s">
-        <v>1213</v>
+        <v>448</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>1218</v>
+        <v>449</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>1218</v>
+        <v>449</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E49" s="38" t="s">
-        <v>1223</v>
+      <c r="E49" s="12" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="7" customFormat="1">
       <c r="A50" s="7" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>1221</v>
+        <v>1232</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>1221</v>
+        <v>1232</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E50" s="38" t="s">
-        <v>1224</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="7" customFormat="1">
       <c r="A51" s="7" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E51" s="38" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="7" customFormat="1">
       <c r="A52" s="7" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E52" s="38" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1">
       <c r="A53" s="7" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C53" s="40" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E53" s="38" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="7" customFormat="1">
       <c r="A54" s="7" t="s">
-        <v>1228</v>
+        <v>1216</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E54" s="38" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1">
       <c r="A55" s="7" t="s">
-        <v>1231</v>
+        <v>1217</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>1561</v>
+        <v>1220</v>
       </c>
       <c r="C55" s="40" t="s">
-        <v>1561</v>
+        <v>1220</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="41" t="s">
-        <v>1562</v>
+      <c r="E55" s="38" t="s">
+        <v>1227</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="7" customFormat="1">
       <c r="A56" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="38" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="7" customFormat="1">
+      <c r="A57" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="41" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="7" customFormat="1">
+      <c r="A58" s="7" t="s">
         <v>1234</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>1235</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C58" s="40" t="s">
         <v>1235</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="38" t="s">
+      <c r="D58" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="38" t="s">
         <v>1236</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="7" customFormat="1" ht="29.15">
-      <c r="A57" s="7" t="s">
+    <row r="59" spans="1:5" s="7" customFormat="1" ht="29.15">
+      <c r="A59" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C57" s="40" t="s">
+      <c r="C59" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="12" t="s">
+      <c r="D59" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="7" customFormat="1" ht="29.15">
-      <c r="A58" s="7" t="s">
+    <row r="60" spans="1:5" s="7" customFormat="1" ht="29.15">
+      <c r="A60" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="C58" s="40" t="s">
+      <c r="C60" s="40" t="s">
         <v>356</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="12" t="s">
+      <c r="D60" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="7" customFormat="1">
-      <c r="A59" s="7" t="s">
+    <row r="61" spans="1:5" s="7" customFormat="1">
+      <c r="A61" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="C59" s="40" t="s">
+      <c r="C61" s="40" t="s">
         <v>366</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="10" t="s">
+      <c r="D61" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="10" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1">
-      <c r="A60" s="7" t="s">
+    <row r="62" spans="1:5" s="7" customFormat="1">
+      <c r="A62" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C60" s="40" t="s">
+      <c r="C62" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="10" t="s">
+      <c r="D62" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="7" customFormat="1" ht="58.3">
-      <c r="A61" s="7" t="s">
+    <row r="63" spans="1:5" s="7" customFormat="1" ht="58.3">
+      <c r="A63" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C61" s="40" t="s">
+      <c r="C63" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12" t="s">
+      <c r="D63" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="12" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="7" customFormat="1" ht="43.75">
-      <c r="A62" s="7" t="s">
+    <row r="64" spans="1:5" s="7" customFormat="1" ht="43.75">
+      <c r="A64" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B64" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="40" t="s">
+      <c r="C64" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="12" t="s">
+      <c r="D64" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="12" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="7" customFormat="1" ht="43.75">
-      <c r="A63" s="7" t="s">
+    <row r="65" spans="1:5" s="7" customFormat="1" ht="43.75">
+      <c r="A65" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B65" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="40" t="s">
+      <c r="C65" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="11" t="s">
+      <c r="D65" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="11" t="s">
         <v>473</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="7" customFormat="1" ht="29.15">
-      <c r="A64" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" ht="29.15">
-      <c r="A65" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C65" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" ht="29.15">
       <c r="A66" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="7" customFormat="1" ht="29.15">
+      <c r="A67" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="7" customFormat="1" ht="29.15">
+      <c r="A68" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B68" s="7" t="s">
         <v>1251</v>
       </c>
-      <c r="C66" s="40" t="s">
+      <c r="C68" s="40" t="s">
         <v>1251</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="12" t="s">
+      <c r="D68" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="7" customFormat="1" ht="87.45">
-      <c r="A67" s="7" t="s">
+    <row r="69" spans="1:5" s="7" customFormat="1" ht="87.45">
+      <c r="A69" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="C69" s="40" t="s">
         <v>446</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" s="11" t="s">
+      <c r="D69" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="11" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" ht="87.45">
-      <c r="A68" s="7" t="s">
+    <row r="70" spans="1:5" s="7" customFormat="1" ht="87.45">
+      <c r="A70" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B70" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="C68" s="40" t="s">
+      <c r="C70" s="40" t="s">
         <v>445</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="11" t="s">
+      <c r="D70" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" ht="58.3">
-      <c r="A69" s="7" t="s">
+    <row r="71" spans="1:5" s="7" customFormat="1" ht="58.3">
+      <c r="A71" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="C69" s="40" t="s">
+      <c r="C71" s="40" t="s">
         <v>444</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="12" t="s">
+      <c r="D71" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="7" customFormat="1" ht="58.3">
-      <c r="A70" s="7" t="s">
+    <row r="72" spans="1:5" s="7" customFormat="1" ht="58.3">
+      <c r="A72" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B72" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C70" s="40" t="s">
+      <c r="C72" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="D70" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" s="10" t="s">
+      <c r="D72" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="10" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="29.15">
-      <c r="A71" s="7" t="s">
+    <row r="73" spans="1:5" ht="29.15">
+      <c r="A73" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B73" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="C71" s="40" t="s">
+      <c r="C73" s="40" t="s">
         <v>370</v>
       </c>
-      <c r="D71" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="12" t="s">
+      <c r="D73" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="12" t="s">
         <v>466</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="C72" s="40" t="s">
-        <v>369</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C74" s="40" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E74" s="12" t="s">
-        <v>465</v>
+      <c r="E74" s="10" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="7" t="s">
-        <v>374</v>
+      <c r="A75" s="8" t="s">
+        <v>371</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>384</v>
+        <v>37</v>
       </c>
       <c r="C75" s="40" t="s">
-        <v>384</v>
+        <v>37</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C76" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C77" s="40" t="s">
+        <v>384</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B78" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="C76" s="40" t="s">
+      <c r="C78" s="40" t="s">
         <v>383</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" s="10" t="s">
+      <c r="D78" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="10" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="8" t="s">
+    <row r="79" spans="1:5">
+      <c r="A79" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B79" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="C77" s="40" t="s">
+      <c r="C79" s="40" t="s">
         <v>439</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="10" t="s">
+      <c r="D79" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="10" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="8" t="s">
+    <row r="80" spans="1:5">
+      <c r="A80" s="8" t="s">
         <v>752</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B80" s="7" t="s">
         <v>753</v>
       </c>
-      <c r="C78" s="40" t="s">
+      <c r="C80" s="40" t="s">
         <v>753</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="38" t="s">
+      <c r="D80" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="38" t="s">
         <v>1252</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="7" t="s">
+    <row r="81" spans="1:5">
+      <c r="A81" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B81" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C81" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D81" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E81" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="80" spans="1:5" customFormat="1">
-      <c r="A80" t="s">
+    <row r="82" spans="1:5" customFormat="1">
+      <c r="A82" t="s">
         <v>388</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>389</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>389</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D82" t="s">
         <v>389</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E82" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="8" t="s">
+    <row r="83" spans="1:5">
+      <c r="A83" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B83" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="C81" s="39" t="s">
+      <c r="C83" s="39" t="s">
         <v>437</v>
       </c>
-      <c r="D81" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="12" t="s">
+      <c r="D83" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="12" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="8" t="s">
+    <row r="84" spans="1:5">
+      <c r="A84" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B84" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="C82" s="39" t="s">
+      <c r="C84" s="39" t="s">
         <v>438</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="10" t="s">
+      <c r="D84" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="10" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="29.15">
-      <c r="A83" s="8" t="s">
+    <row r="85" spans="1:5" ht="29.15">
+      <c r="A85" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B85" s="7" t="s">
         <v>1593</v>
       </c>
-      <c r="C83" s="40" t="s">
+      <c r="C85" s="40" t="s">
         <v>1593</v>
       </c>
-      <c r="D83" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="11" t="s">
+      <c r="D85" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="11" t="s">
         <v>485</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="43.75">
-      <c r="A84" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="C84" s="40" t="s">
-        <v>459</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="43.75">
-      <c r="A85" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="C85" s="40" t="s">
-        <v>454</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="43.75">
       <c r="A86" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>755</v>
+        <v>459</v>
       </c>
       <c r="C86" s="40" t="s">
-        <v>755</v>
+        <v>459</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="43.75">
       <c r="A87" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C87" s="40" t="s">
+        <v>454</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="43.75">
+      <c r="A88" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C88" s="40" t="s">
+        <v>755</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="43.75">
+      <c r="A89" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B89" s="7" t="s">
         <v>756</v>
       </c>
-      <c r="C87" s="40" t="s">
+      <c r="C89" s="40" t="s">
         <v>756</v>
       </c>
-      <c r="D87" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="12" t="s">
+      <c r="D89" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="12" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="29.15">
-      <c r="A88" s="8" t="s">
+    <row r="90" spans="1:5" ht="29.15">
+      <c r="A90" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B90" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="C88" s="40" t="s">
+      <c r="C90" s="40" t="s">
         <v>463</v>
       </c>
-      <c r="D88" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="12" t="s">
+      <c r="D90" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="12" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="29.15">
-      <c r="A89" s="8" t="s">
+    <row r="91" spans="1:5" ht="29.15">
+      <c r="A91" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B91" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="C89" s="40" t="s">
+      <c r="C91" s="40" t="s">
         <v>462</v>
       </c>
-      <c r="D89" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="12" t="s">
+      <c r="D91" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="12" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="16" customFormat="1">
-      <c r="A90" s="32" t="s">
+    <row r="92" spans="1:5" s="16" customFormat="1">
+      <c r="A92" s="32" t="s">
         <v>935</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B92" t="s">
         <v>870</v>
       </c>
-      <c r="C90" s="16" t="s">
+      <c r="C92" s="16" t="s">
         <v>1342</v>
       </c>
-      <c r="D90" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="38" t="s">
+      <c r="D92" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="38" t="s">
         <v>1244</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="8" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C91" s="39" t="s">
-        <v>1241</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="38" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="8" t="s">
-        <v>1238</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C92" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E92" s="38" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="8" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="C93" s="39" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="38" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="8" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>1243</v>
+        <v>25</v>
       </c>
       <c r="C94" s="39" t="s">
-        <v>1243</v>
+        <v>25</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E94" s="38" t="s">
-        <v>1247</v>
+        <v>405</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="8" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C95" s="39" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="38" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="8" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C96" s="39" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="38" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="8" t="s">
         <v>1248</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B97" s="8" t="s">
         <v>1250</v>
       </c>
-      <c r="C95" s="39" t="s">
+      <c r="C97" s="39" t="s">
         <v>1250</v>
       </c>
-      <c r="D95" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="38" t="s">
+      <c r="D97" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="38" t="s">
         <v>1249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
addition of Preston updated scenarios
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5580" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="StringLocalizations_Preston" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7493" uniqueCount="1891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7933" uniqueCount="2045">
   <si>
     <t>XXXX</t>
   </si>
@@ -6448,6 +6448,468 @@
   </si>
   <si>
     <t>BASIC_TEXT_SENDING_FEEDBACK</t>
+  </si>
+  <si>
+    <t>Bad Choice, person could be in significant danger</t>
+  </si>
+  <si>
+    <t>Great Choice, but citizens could help</t>
+  </si>
+  <si>
+    <t>You should use  the new information, the woman could be in significant danger</t>
+  </si>
+  <si>
+    <t>Citizens could help, but is deployment not best?</t>
+  </si>
+  <si>
+    <t>Great Choice, officers are needed to locate the woman</t>
+  </si>
+  <si>
+    <t>SCENARIO_2_CITIZEN_FEEDBACK_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_2_WAIT_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_2_OFFICER_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>Good choice, other incidents may take priority</t>
+  </si>
+  <si>
+    <t>Should officers really be involved in this case?</t>
+  </si>
+  <si>
+    <t>There may not be a need to send officers, but citizens may feel ignored</t>
+  </si>
+  <si>
+    <t>Good choice, but officers may be needed later, be careful</t>
+  </si>
+  <si>
+    <t>An assault has taken place, now would have been a good time to send officers</t>
+  </si>
+  <si>
+    <t>Good choice, an officer should be able to diffuse the situation</t>
+  </si>
+  <si>
+    <t>Good call, citizens can assist quite a bit with this</t>
+  </si>
+  <si>
+    <t>This type of incident should not be ignored</t>
+  </si>
+  <si>
+    <t>Great choice, this is the best option here</t>
+  </si>
+  <si>
+    <t>Not a good choice, female could be in serious trouble</t>
+  </si>
+  <si>
+    <t>Best Choice, but could citizens help?</t>
+  </si>
+  <si>
+    <t>Not a good choice, this is a serious investigation</t>
+  </si>
+  <si>
+    <t>Great choice, this is a serious investigation</t>
+  </si>
+  <si>
+    <t>Not a good choice, citizens feel their information is ignored</t>
+  </si>
+  <si>
+    <t>Good Choice</t>
+  </si>
+  <si>
+    <t>Good choice as this is not an urgent incident</t>
+  </si>
+  <si>
+    <t>Could this resource be better used</t>
+  </si>
+  <si>
+    <t>Good choice, often citizens can help with issues like this</t>
+  </si>
+  <si>
+    <t>This is not a good choice as this is a high profile incident</t>
+  </si>
+  <si>
+    <t>Good choice, but could other options be explored?</t>
+  </si>
+  <si>
+    <t>Officers should have been sent to detain the offender quickly</t>
+  </si>
+  <si>
+    <t>Good choice, the officer will be able to close this case</t>
+  </si>
+  <si>
+    <t>SCENARIO_6_WAIT_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>Bad Choice, there is a fight on-going</t>
+  </si>
+  <si>
+    <t>Best choice, citizens could provide help but a fight is on-going</t>
+  </si>
+  <si>
+    <t>What were you thinking? Someone has serious injuries</t>
+  </si>
+  <si>
+    <t>Great choice, responding to a serious injury should help close this case</t>
+  </si>
+  <si>
+    <t>The scene has been identifeid as severe, you should have sent officers</t>
+  </si>
+  <si>
+    <t>Great choice, officers need to attend to secure the scene</t>
+  </si>
+  <si>
+    <t>Great choice, officers are needed to close this case and arrest the aggressor</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_WAIT_FEEDBACK_10</t>
+  </si>
+  <si>
+    <t>SCENARIO_7_OFFICER_FEEDBACK_10</t>
+  </si>
+  <si>
+    <t>Not a good choice, this incident could potentially get out of hand</t>
+  </si>
+  <si>
+    <t>Good choice, officers will be able to diffuse the situation</t>
+  </si>
+  <si>
+    <t>Great choice, citizens may be able to help identify the suspect</t>
+  </si>
+  <si>
+    <t>Not a good choice, could get even worse</t>
+  </si>
+  <si>
+    <t>The incident has been left to get out of hand, you should really send an officer soon</t>
+  </si>
+  <si>
+    <t>You should send officers, the incident has developed to an assault</t>
+  </si>
+  <si>
+    <t>Good choice, officers should be able to prevent the incident escalating further</t>
+  </si>
+  <si>
+    <t>Ok, the man was prosecuted but may have more information</t>
+  </si>
+  <si>
+    <t>Listening to the people will help gain confidence and can lead to further arrests</t>
+  </si>
+  <si>
+    <t>The male may have more information that could lead to further arrests, should have sent officers</t>
+  </si>
+  <si>
+    <t>Officers will be able to identify further offenders if there are any</t>
+  </si>
+  <si>
+    <t>The male may have assaulted an officer but there may be more offenders, should have sent officers</t>
+  </si>
+  <si>
+    <t>You had all the information to make an arrest, should have sent an officer</t>
+  </si>
+  <si>
+    <t>Great choice, the officer will be able to make an arrest now</t>
+  </si>
+  <si>
+    <t>Good choice, saving officers for more important incidents is important</t>
+  </si>
+  <si>
+    <t>Sending officers is ok, but there could be a better choice</t>
+  </si>
+  <si>
+    <t>Not a good choice, incident may get out of hand</t>
+  </si>
+  <si>
+    <t>This is a good choice</t>
+  </si>
+  <si>
+    <t>Bad choice, the situation has escalated, you should really react to this</t>
+  </si>
+  <si>
+    <t>Good choice, sending officers to stop the assault is important</t>
+  </si>
+  <si>
+    <t>This is ok, but maybe asking for help would be a better option</t>
+  </si>
+  <si>
+    <t>A male is reported missing and could be in danger</t>
+  </si>
+  <si>
+    <t>Good call, the officer should be able to resolve the situation with the information</t>
+  </si>
+  <si>
+    <t>The male requires further aid, helping would have increased public opinion</t>
+  </si>
+  <si>
+    <t>Great choice, aiding the elderly will help improve relations</t>
+  </si>
+  <si>
+    <t>The information provided could have directed officers to the lost male</t>
+  </si>
+  <si>
+    <t>Good choice, not all incidents should see a deployment</t>
+  </si>
+  <si>
+    <t>With limited resources, consider the incident and decide officer time could be used elsewhere</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_WAIT_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_WAIT_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_11_OFFICER_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>Not the best decision, driver could be in need of assistance</t>
+  </si>
+  <si>
+    <t>Good choice, delayed deployment may cause issues</t>
+  </si>
+  <si>
+    <t>Why would you wait? You risk losing key evidence</t>
+  </si>
+  <si>
+    <t>Good choice, you can't ignore something like this</t>
+  </si>
+  <si>
+    <t>More officers are required to close this case, delaying will cause frustration to other road users</t>
+  </si>
+  <si>
+    <t>Great call, officers will be able to deal with the situation</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_WAIT_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_12_OFFICER_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>Not the best, but not considered urgent, but be aware the situation could get worse</t>
+  </si>
+  <si>
+    <t>Information from citizens may help to prosecute the offender</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_WAIT_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_OFFICER_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_WAIT_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_WAIT_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>SCENARIO_13_OFFICER_FEEDBACK_6</t>
+  </si>
+  <si>
+    <t>Difficult choice, remember to set priorities with other incidents</t>
+  </si>
+  <si>
+    <t>There may have been better choices to help aprehend the male</t>
+  </si>
+  <si>
+    <t>Citizesn may be able to help identify the male</t>
+  </si>
+  <si>
+    <t>Questionable choice, the incidnet has escalated and may escalate further</t>
+  </si>
+  <si>
+    <t>Good call, you do not want the scenario to get any worse</t>
+  </si>
+  <si>
+    <t>Bad choice, you should use the information from citizens, otherwise they will feel ignored</t>
+  </si>
+  <si>
+    <t>Should have sent officers, the male will likely get away without being arrested</t>
+  </si>
+  <si>
+    <t>Sending officers will help to arrest the male. Good choice</t>
+  </si>
+  <si>
+    <t>SCENARIO_14_WAIT_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_14_OFFICER_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>Bad call, you don't know what might happen to the child</t>
+  </si>
+  <si>
+    <t>Great, officers will be able to begin searching for the child</t>
+  </si>
+  <si>
+    <t>This is a great choice, citizens may be able to provide more information as to the location of the child</t>
+  </si>
+  <si>
+    <t>Great, without further information, officers will have to keep searching</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_WAIT_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_WAIT_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_15_OFFICER_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>Tough choice, other incidents may take priority</t>
+  </si>
+  <si>
+    <t>Sending officers will be able to handle the incident quickly</t>
+  </si>
+  <si>
+    <t>There is a chance that the incident may now escalate, consider sending officers</t>
+  </si>
+  <si>
+    <t>Good choice, you do not want the situation getting worse</t>
+  </si>
+  <si>
+    <t>You cannot ignore this incident as it could get worse</t>
+  </si>
+  <si>
+    <t>SCENARIO_16_WAIT_FEEDBACK_4</t>
+  </si>
+  <si>
+    <t>SCENARIO_16_OFFICER_FEEDBACK_4</t>
+  </si>
+  <si>
+    <t>Bad choice, someone is in need</t>
+  </si>
+  <si>
+    <t>Good choice, you don't know if anyone is at risk</t>
+  </si>
+  <si>
+    <t>The information provided could have directed officers to the youths and make arrests</t>
+  </si>
+  <si>
+    <t>Good call, with the identity of the youths, officers will be able to make arrests</t>
+  </si>
+  <si>
+    <t>SCENARIO_17_WAIT_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_17_OFFICER_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>Although it is not obvious, this is a serious incident as the elderly family member may be in need</t>
+  </si>
+  <si>
+    <t>Great choice, this is a serious incident</t>
+  </si>
+  <si>
+    <t>Citizens may be able to help with this case, but it is very serious and officers should be sent</t>
+  </si>
+  <si>
+    <t>The elderly family member requires assistance, leaving them could be very damaging</t>
+  </si>
+  <si>
+    <t>SCENARIO_18_WAIT_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_18_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>Although not corroborated, this is a serious incident</t>
+  </si>
+  <si>
+    <t>Good choice, this is a serious incident</t>
+  </si>
+  <si>
+    <t>Citizens may be able to provide more information, but a location is known and the incident is serious, you should have sent officers</t>
+  </si>
+  <si>
+    <t>A lack of deployment will not solve the crime</t>
+  </si>
+  <si>
+    <t>Good, using the information known and sending officers will help to make arrests</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_WAIT_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_OFFICER_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_CITIZEN_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_WAIT_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_WAIT_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>SCENARIO_19_OFFICER_FEEDBACK_5</t>
+  </si>
+  <si>
+    <t>Bad choice, although the incident is not serious, it is a priority</t>
+  </si>
+  <si>
+    <t>Sending officers is a good idea to help gather information, but maybe citizens could have provided the same information</t>
+  </si>
+  <si>
+    <t>Good choice, citizens will be able to offer more information on the incident</t>
+  </si>
+  <si>
+    <t>Good choice, this behaviour cannot be ignored</t>
+  </si>
+  <si>
+    <t>You should use the information available, your officers could help resolve this case</t>
+  </si>
+  <si>
+    <t>Good choice, officers will have more chance of lacating the vehicle with this information</t>
+  </si>
+  <si>
+    <t>SCENARIO_20_WAIT_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_20_OFFICER_FEEDBACK_2</t>
+  </si>
+  <si>
+    <t>SCENARIO_20_WAIT_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>SCENARIO_20_OFFICER_FEEDBACK_3</t>
+  </si>
+  <si>
+    <t>The incident could get worse, consider your options carefully</t>
+  </si>
+  <si>
+    <t>Sending officers is a good choice, but the inicident is not a priority</t>
+  </si>
+  <si>
+    <t>Great, citizens should be able to provide a lot of information with incidents like this</t>
+  </si>
+  <si>
+    <t>Although this is not a serious incident, it is a priority</t>
+  </si>
+  <si>
+    <t>Sending officers could help locate the dog, but without a known location it may prove difficult</t>
+  </si>
+  <si>
+    <t>You should use the information provided by citizens, ignoring this can make them feel ignored</t>
+  </si>
+  <si>
+    <t>Great, you have the information required to send officers to deal with this incident</t>
   </si>
 </sst>
 </file>
@@ -6612,7 +7074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6740,6 +7202,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -7021,10 +7488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E262"/>
+  <dimension ref="A1:E350"/>
   <sheetViews>
-    <sheetView topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E262" sqref="A203:E262"/>
+    <sheetView tabSelected="1" topLeftCell="A310" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B345" sqref="B345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -10475,8 +10942,8 @@
       <c r="A203" s="31" t="s">
         <v>1104</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>0</v>
+      <c r="B203" s="19" t="s">
+        <v>1891</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>0</v>
@@ -10492,8 +10959,8 @@
       <c r="A204" s="1" t="s">
         <v>1107</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>0</v>
+      <c r="B204" s="19" t="s">
+        <v>1892</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>0</v>
@@ -10505,12 +10972,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
-      <c r="A205" s="1" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>0</v>
+    <row r="205" spans="1:5" ht="25">
+      <c r="A205" s="32" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B205" s="19" t="s">
+        <v>1893</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>0</v>
@@ -10523,11 +10990,11 @@
       </c>
     </row>
     <row r="206" spans="1:5">
-      <c r="A206" s="31" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>0</v>
+      <c r="A206" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B206" s="19" t="s">
+        <v>1892</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>0</v>
@@ -10541,10 +11008,10 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="1" t="s">
-        <v>1123</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>0</v>
+        <v>1111</v>
+      </c>
+      <c r="B207" s="19" t="s">
+        <v>1894</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>0</v>
@@ -10556,12 +11023,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="1" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>0</v>
+    <row r="208" spans="1:5" ht="25">
+      <c r="A208" s="32" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B208" s="19" t="s">
+        <v>1893</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>0</v>
@@ -10574,11 +11041,11 @@
       </c>
     </row>
     <row r="209" spans="1:5">
-      <c r="A209" s="31" t="s">
-        <v>1449</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>0</v>
+      <c r="A209" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B209" s="19" t="s">
+        <v>1895</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>0</v>
@@ -10591,11 +11058,11 @@
       </c>
     </row>
     <row r="210" spans="1:5">
-      <c r="A210" s="1" t="s">
-        <v>1494</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>0</v>
+      <c r="A210" s="31" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B210" s="19" t="s">
+        <v>1899</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>0</v>
@@ -10609,10 +11076,10 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="1" t="s">
-        <v>1528</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>0</v>
+        <v>1123</v>
+      </c>
+      <c r="B211" s="19" t="s">
+        <v>1900</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>0</v>
@@ -10625,11 +11092,11 @@
       </c>
     </row>
     <row r="212" spans="1:5">
-      <c r="A212" s="31" t="s">
-        <v>1454</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>0</v>
+      <c r="A212" s="32" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B212" s="19" t="s">
+        <v>1901</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>0</v>
@@ -10642,11 +11109,11 @@
       </c>
     </row>
     <row r="213" spans="1:5">
-      <c r="A213" s="1" t="s">
-        <v>1495</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>0</v>
+      <c r="A213" s="22" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B213" s="19" t="s">
+        <v>1902</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>0</v>
@@ -10658,12 +11125,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
-      <c r="A214" s="1" t="s">
-        <v>1531</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>0</v>
+    <row r="214" spans="1:5" ht="25">
+      <c r="A214" s="32" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B214" s="19" t="s">
+        <v>1903</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>0</v>
@@ -10676,11 +11143,11 @@
       </c>
     </row>
     <row r="215" spans="1:5">
-      <c r="A215" s="31" t="s">
-        <v>1453</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>0</v>
+      <c r="A215" s="22" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B215" s="19" t="s">
+        <v>1904</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>0</v>
@@ -10693,11 +11160,11 @@
       </c>
     </row>
     <row r="216" spans="1:5">
-      <c r="A216" s="1" t="s">
-        <v>1501</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>0</v>
+      <c r="A216" s="22" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B216" s="19" t="s">
+        <v>1905</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>0</v>
@@ -10710,11 +11177,11 @@
       </c>
     </row>
     <row r="217" spans="1:5">
-      <c r="A217" s="1" t="s">
-        <v>1534</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>0</v>
+      <c r="A217" s="32" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B217" s="19" t="s">
+        <v>1906</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>0</v>
@@ -10727,11 +11194,11 @@
       </c>
     </row>
     <row r="218" spans="1:5">
-      <c r="A218" s="31" t="s">
-        <v>1460</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>0</v>
+      <c r="A218" s="22" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B218" s="19" t="s">
+        <v>1907</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>0</v>
@@ -10744,11 +11211,11 @@
       </c>
     </row>
     <row r="219" spans="1:5">
-      <c r="A219" s="1" t="s">
-        <v>1504</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>0</v>
+      <c r="A219" s="22" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B219" s="19" t="s">
+        <v>1905</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>0</v>
@@ -10761,11 +11228,11 @@
       </c>
     </row>
     <row r="220" spans="1:5">
-      <c r="A220" s="1" t="s">
-        <v>1536</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>0</v>
+      <c r="A220" s="32" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B220" s="19" t="s">
+        <v>1906</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>0</v>
@@ -10778,11 +11245,11 @@
       </c>
     </row>
     <row r="221" spans="1:5">
-      <c r="A221" s="31" t="s">
-        <v>1465</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>0</v>
+      <c r="A221" s="22" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B221" s="19" t="s">
+        <v>1907</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>0</v>
@@ -10795,11 +11262,11 @@
       </c>
     </row>
     <row r="222" spans="1:5">
-      <c r="A222" s="1" t="s">
-        <v>1508</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>0</v>
+      <c r="A222" s="32" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B222" s="19" t="s">
+        <v>1906</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>0</v>
@@ -10812,11 +11279,11 @@
       </c>
     </row>
     <row r="223" spans="1:5">
-      <c r="A223" s="1" t="s">
-        <v>1540</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>0</v>
+      <c r="A223" s="22" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B223" s="19" t="s">
+        <v>1907</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>0</v>
@@ -10830,10 +11297,10 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="31" t="s">
-        <v>1474</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>0</v>
+        <v>1449</v>
+      </c>
+      <c r="B224" s="19" t="s">
+        <v>1908</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>0</v>
@@ -10847,10 +11314,10 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
-        <v>1515</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>0</v>
+        <v>1494</v>
+      </c>
+      <c r="B225" s="19" t="s">
+        <v>1909</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>0</v>
@@ -10864,10 +11331,10 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>1545</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>0</v>
+        <v>1528</v>
+      </c>
+      <c r="B226" s="19" t="s">
+        <v>1894</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>0</v>
@@ -10880,11 +11347,11 @@
       </c>
     </row>
     <row r="227" spans="1:5">
-      <c r="A227" s="31" t="s">
-        <v>1482</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>0</v>
+      <c r="A227" s="32" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B227" s="19" t="s">
+        <v>1910</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>0</v>
@@ -10897,11 +11364,11 @@
       </c>
     </row>
     <row r="228" spans="1:5">
-      <c r="A228" s="1" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>0</v>
+      <c r="A228" s="22" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B228" s="19" t="s">
+        <v>1911</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>0</v>
@@ -10914,11 +11381,11 @@
       </c>
     </row>
     <row r="229" spans="1:5">
-      <c r="A229" s="1" t="s">
-        <v>1550</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>0</v>
+      <c r="A229" s="32" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B229" s="19" t="s">
+        <v>1912</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>0</v>
@@ -10931,11 +11398,11 @@
       </c>
     </row>
     <row r="230" spans="1:5">
-      <c r="A230" s="31" t="s">
-        <v>1486</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>0</v>
+      <c r="A230" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B230" s="19" t="s">
+        <v>1913</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>0</v>
@@ -10948,11 +11415,11 @@
       </c>
     </row>
     <row r="231" spans="1:5">
-      <c r="A231" s="1" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>0</v>
+      <c r="A231" s="31" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B231" s="19" t="s">
+        <v>1914</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>0</v>
@@ -10966,10 +11433,10 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
-        <v>1554</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>0</v>
+        <v>1495</v>
+      </c>
+      <c r="B232" s="19" t="s">
+        <v>1915</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>0</v>
@@ -10982,11 +11449,11 @@
       </c>
     </row>
     <row r="233" spans="1:5">
-      <c r="A233" s="31" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>0</v>
+      <c r="A233" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B233" s="19" t="s">
+        <v>1916</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>0</v>
@@ -10999,11 +11466,11 @@
       </c>
     </row>
     <row r="234" spans="1:5">
-      <c r="A234" s="1" t="s">
-        <v>1561</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>0</v>
+      <c r="A234" s="32" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B234" s="19" t="s">
+        <v>1914</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>0</v>
@@ -11016,11 +11483,11 @@
       </c>
     </row>
     <row r="235" spans="1:5">
-      <c r="A235" s="1" t="s">
-        <v>1562</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>0</v>
+      <c r="A235" s="22" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B235" s="19" t="s">
+        <v>1915</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>0</v>
@@ -11034,10 +11501,10 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="31" t="s">
-        <v>1563</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>0</v>
+        <v>1453</v>
+      </c>
+      <c r="B236" s="19" t="s">
+        <v>1917</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>0</v>
@@ -11051,10 +11518,10 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>1564</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>0</v>
+        <v>1501</v>
+      </c>
+      <c r="B237" s="19" t="s">
+        <v>1918</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>0</v>
@@ -11067,11 +11534,11 @@
       </c>
     </row>
     <row r="238" spans="1:5">
-      <c r="A238" s="1" t="s">
-        <v>1565</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>0</v>
+      <c r="A238" s="22" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B238" s="19" t="s">
+        <v>1916</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>0</v>
@@ -11084,11 +11551,11 @@
       </c>
     </row>
     <row r="239" spans="1:5">
-      <c r="A239" s="31" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>0</v>
+      <c r="A239" s="32" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B239" s="19" t="s">
+        <v>1919</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>0</v>
@@ -11101,11 +11568,11 @@
       </c>
     </row>
     <row r="240" spans="1:5">
-      <c r="A240" s="1" t="s">
-        <v>1568</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>0</v>
+      <c r="A240" s="22" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B240" s="19" t="s">
+        <v>1920</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>0</v>
@@ -11118,11 +11585,11 @@
       </c>
     </row>
     <row r="241" spans="1:5">
-      <c r="A241" s="1" t="s">
-        <v>1567</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>0</v>
+      <c r="A241" s="32" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B241" s="19" t="s">
+        <v>1919</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>0</v>
@@ -11135,11 +11602,11 @@
       </c>
     </row>
     <row r="242" spans="1:5">
-      <c r="A242" s="31" t="s">
-        <v>1569</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>0</v>
+      <c r="A242" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B242" s="19" t="s">
+        <v>1920</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>0</v>
@@ -11152,11 +11619,11 @@
       </c>
     </row>
     <row r="243" spans="1:5">
-      <c r="A243" s="1" t="s">
-        <v>1570</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>0</v>
+      <c r="A243" s="31" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B243" s="19" t="s">
+        <v>1922</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>0</v>
@@ -11170,10 +11637,10 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>1571</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>0</v>
+        <v>1504</v>
+      </c>
+      <c r="B244" s="19" t="s">
+        <v>1923</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>0</v>
@@ -11186,11 +11653,11 @@
       </c>
     </row>
     <row r="245" spans="1:5">
-      <c r="A245" s="31" t="s">
-        <v>1572</v>
-      </c>
-      <c r="B245" s="1" t="s">
-        <v>0</v>
+      <c r="A245" s="22" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B245" s="19" t="s">
+        <v>1894</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>0</v>
@@ -11203,11 +11670,11 @@
       </c>
     </row>
     <row r="246" spans="1:5">
-      <c r="A246" s="1" t="s">
-        <v>1573</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>0</v>
+      <c r="A246" s="32" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B246" s="19" t="s">
+        <v>1924</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>0</v>
@@ -11220,11 +11687,11 @@
       </c>
     </row>
     <row r="247" spans="1:5">
-      <c r="A247" s="1" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>0</v>
+      <c r="A247" s="22" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B247" s="19" t="s">
+        <v>1925</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>0</v>
@@ -11237,11 +11704,11 @@
       </c>
     </row>
     <row r="248" spans="1:5">
-      <c r="A248" s="31" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>0</v>
+      <c r="A248" s="32" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B248" s="19" t="s">
+        <v>1926</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>0</v>
@@ -11254,11 +11721,11 @@
       </c>
     </row>
     <row r="249" spans="1:5">
-      <c r="A249" s="1" t="s">
-        <v>1576</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>0</v>
+      <c r="A249" s="22" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B249" s="19" t="s">
+        <v>1927</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>0</v>
@@ -11271,11 +11738,11 @@
       </c>
     </row>
     <row r="250" spans="1:5">
-      <c r="A250" s="1" t="s">
-        <v>1577</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>0</v>
+      <c r="A250" s="32" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B250" s="19" t="s">
+        <v>1924</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>0</v>
@@ -11287,12 +11754,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
-      <c r="A251" s="31" t="s">
-        <v>1578</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>0</v>
+    <row r="251" spans="1:5" ht="25">
+      <c r="A251" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B251" s="19" t="s">
+        <v>1928</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>0</v>
@@ -11305,11 +11772,11 @@
       </c>
     </row>
     <row r="252" spans="1:5">
-      <c r="A252" s="1" t="s">
-        <v>1579</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>0</v>
+      <c r="A252" s="31" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B252" s="19" t="s">
+        <v>1931</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>0</v>
@@ -11323,171 +11790,1667 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B253" s="19" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
+      <c r="A254" s="1" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B254" s="19" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5">
+      <c r="A255" s="32" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B255" s="19" t="s">
+        <v>1934</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
+      <c r="A256" s="22" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B256" s="19" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" ht="25">
+      <c r="A257" s="32" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B257" s="19" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
+      <c r="A258" s="22" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B258" s="19" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" s="32" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B259" s="19" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" ht="25">
+      <c r="A260" s="22" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B260" s="19" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5">
+      <c r="A261" s="32" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B261" s="19" t="s">
+        <v>1938</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" ht="25">
+      <c r="A262" s="22" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B262" s="19" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" ht="25">
+      <c r="A263" s="32" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B263" s="19" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5">
+      <c r="A264" s="22" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B264" s="19" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" ht="25">
+      <c r="A265" s="32" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B265" s="19" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" s="32" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B266" s="19" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" s="22" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B267" s="19" t="s">
+        <v>1944</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" s="31" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B268" s="19" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" s="22" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B269" s="19" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" s="22" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B270" s="19" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" s="32" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B271" s="19" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" s="22" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B272" s="19" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="32" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B273" s="19" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5">
+      <c r="A274" s="22" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B274" s="19" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5">
+      <c r="A275" s="32" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B275" s="19" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5">
+      <c r="A276" s="22" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B276" s="19" t="s">
+        <v>1950</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5">
+      <c r="A277" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B277" s="19" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5">
+      <c r="A278" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B278" s="19" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5">
+      <c r="A279" s="32" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B279" s="19" t="s">
+        <v>1952</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="25">
+      <c r="A280" s="22" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B280" s="19" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5">
+      <c r="A281" s="32" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B281" s="19" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5">
+      <c r="A282" s="22" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B282" s="19" t="s">
+        <v>1955</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5">
+      <c r="A283" s="32" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B283" s="19" t="s">
+        <v>1956</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" ht="25">
+      <c r="A284" s="22" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B284" s="19" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5">
+      <c r="A285" s="31" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B285" s="19" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" ht="25">
+      <c r="A286" s="22" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B286" s="19" t="s">
+        <v>1958</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5">
+      <c r="A287" s="31" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B287" s="19" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5">
+      <c r="A288" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B288" s="19" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5">
+      <c r="A289" s="22" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B289" s="19" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5">
+      <c r="A290" s="32" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B290" s="19" t="s">
+        <v>1965</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5">
+      <c r="A291" s="22" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B291" s="19" t="s">
+        <v>1966</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" ht="25">
+      <c r="A292" s="32" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B292" s="19" t="s">
+        <v>1967</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5">
+      <c r="A293" s="22" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B293" s="19" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="25">
+      <c r="A294" s="31" t="s">
+        <v>1563</v>
+      </c>
+      <c r="B294" s="19" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5">
+      <c r="A295" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B295" s="19" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5">
+      <c r="A296" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B296" s="19" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" ht="25">
+      <c r="A297" s="32" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B297" s="19" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5">
+      <c r="A298" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B298" s="19" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
+      <c r="A299" s="31" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B299" s="19" t="s">
+        <v>1979</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E299" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5">
+      <c r="A300" s="1" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B300" s="19" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E300" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5">
+      <c r="A301" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B301" s="19" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" s="32" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B302" s="19" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" s="22" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B303" s="19" t="s">
+        <v>1983</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" ht="25">
+      <c r="A304" s="32" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B304" s="19" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E304" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" s="22" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B305" s="19" t="s">
+        <v>1983</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" ht="25">
+      <c r="A306" s="32" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B306" s="19" t="s">
+        <v>1985</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B307" s="19" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" s="31" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B308" s="19" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5">
+      <c r="A309" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B309" s="19" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" ht="25">
+      <c r="A310" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B310" s="19" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5">
+      <c r="A311" s="32" t="s">
+        <v>1987</v>
+      </c>
+      <c r="B311" s="19" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D311" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5">
+      <c r="A312" s="1" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B312" s="19" t="s">
+        <v>1992</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E312" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5">
+      <c r="A313" s="31" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B313" s="19" t="s">
+        <v>1997</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E313" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5">
+      <c r="A314" s="1" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B314" s="19" t="s">
+        <v>1998</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" ht="25">
+      <c r="A315" s="32" t="s">
+        <v>1993</v>
+      </c>
+      <c r="B315" s="19" t="s">
+        <v>1999</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E315" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5">
+      <c r="A316" s="22" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B316" s="19" t="s">
+        <v>2000</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E316" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5">
+      <c r="A317" s="32" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B317" s="19" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5">
+      <c r="A318" s="1" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B318" s="19" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5">
+      <c r="A319" s="31" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B319" s="19" t="s">
+        <v>2004</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5">
+      <c r="A320" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B320" s="19" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5">
+      <c r="A321" s="1" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B321" s="19" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" ht="25">
+      <c r="A322" s="32" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B322" s="19" t="s">
+        <v>2006</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" ht="25">
+      <c r="A323" s="22" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B323" s="19" t="s">
+        <v>2007</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" ht="25">
+      <c r="A324" s="31" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B324" s="19" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E324" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5">
+      <c r="A325" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B325" s="19" t="s">
+        <v>2011</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E325" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" ht="25">
+      <c r="A326" s="1" t="s">
         <v>1580</v>
       </c>
-      <c r="B253" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D253" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5">
-      <c r="A254" s="31" t="s">
+      <c r="B326" s="19" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" ht="25">
+      <c r="A327" s="32" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B327" s="19" t="s">
+        <v>2013</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5">
+      <c r="A328" s="1" t="s">
+        <v>2009</v>
+      </c>
+      <c r="B328" s="19" t="s">
+        <v>2011</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E328" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5">
+      <c r="A329" s="45" t="s">
         <v>1581</v>
       </c>
-      <c r="B254" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5">
-      <c r="A255" s="1" t="s">
+      <c r="B329" s="19" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E329" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5">
+      <c r="A330" s="46" t="s">
         <v>1582</v>
       </c>
-      <c r="B255" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D255" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5">
-      <c r="A256" s="1" t="s">
+      <c r="B330" s="19" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" ht="25">
+      <c r="A331" s="1" t="s">
         <v>1583</v>
       </c>
-      <c r="B256" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D256" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5">
-      <c r="A257" s="31" t="s">
+      <c r="B331" s="19" t="s">
+        <v>2018</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E331" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5">
+      <c r="A332" s="47" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B332" s="19" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E332" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" ht="25">
+      <c r="A333" s="46" t="s">
+        <v>2015</v>
+      </c>
+      <c r="B333" s="19" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E333" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5">
+      <c r="A334" s="31" t="s">
         <v>1584</v>
       </c>
-      <c r="B257" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D257" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5">
-      <c r="A258" s="1" t="s">
+      <c r="B334" s="19" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" ht="25">
+      <c r="A335" s="1" t="s">
         <v>1585</v>
       </c>
-      <c r="B258" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D258" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5">
-      <c r="A259" s="1" t="s">
+      <c r="B335" s="19" t="s">
+        <v>2029</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5">
+      <c r="A336" s="22" t="s">
         <v>1586</v>
       </c>
-      <c r="B259" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C259" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D259" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5">
-      <c r="A260" s="31" t="s">
+      <c r="B336" s="19" t="s">
+        <v>2030</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5">
+      <c r="A337" s="32" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B337" s="19" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5">
+      <c r="A338" s="22" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B338" s="19" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5">
+      <c r="A339" s="22" t="s">
+        <v>2023</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" ht="25">
+      <c r="A340" s="32" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B340" s="19" t="s">
+        <v>2032</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" ht="25">
+      <c r="A341" s="22" t="s">
+        <v>2025</v>
+      </c>
+      <c r="B341" s="19" t="s">
+        <v>2033</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E341" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5">
+      <c r="A342" s="32" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B342" s="19" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5">
+      <c r="A343" s="22" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B343" s="19" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5">
+      <c r="A344" s="31" t="s">
         <v>1587</v>
       </c>
-      <c r="B260" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D260" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5">
-      <c r="A261" s="1" t="s">
+      <c r="B344" s="19" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5">
+      <c r="A345" s="22" t="s">
         <v>1588</v>
       </c>
-      <c r="B261" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C261" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D261" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5">
-      <c r="A262" s="1" t="s">
+      <c r="B345" s="19" t="s">
+        <v>2039</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E345" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" ht="25">
+      <c r="A346" s="22" t="s">
         <v>1589</v>
       </c>
-      <c r="B262" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D262" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E262" s="1" t="s">
+      <c r="B346" s="19" t="s">
+        <v>2040</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5">
+      <c r="A347" s="32" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B347" s="19" t="s">
+        <v>2041</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" ht="25">
+      <c r="A348" s="22" t="s">
+        <v>2035</v>
+      </c>
+      <c r="B348" s="19" t="s">
+        <v>2042</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" ht="25">
+      <c r="A349" s="32" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B349" s="19" t="s">
+        <v>2043</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E349" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" ht="25">
+      <c r="A350" s="22" t="s">
+        <v>2037</v>
+      </c>
+      <c r="B350" s="19" t="s">
+        <v>2044</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E350" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -20891,7 +22854,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add text file to streaming assets add loading screen to start of game to indicate that the game is downloading new content and block the game until that is complete
</commit_message>
<xml_diff>
--- a/Assets/Resources/StringFile.xlsx
+++ b/Assets/Resources/StringFile.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8323" uniqueCount="2944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8343" uniqueCount="2952">
   <si>
     <t>XXXX</t>
   </si>
@@ -8866,6 +8866,30 @@
   </si>
   <si>
     <t>A citizen sends a picture showing three people vandalising bicycles though INSPEC2T</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_RETRIEVING_CONTENT</t>
+  </si>
+  <si>
+    <t>Retrieving Content…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking For New Content… </t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_CHECKING_NEW_CONTENT</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_NEW_CONTENT</t>
+  </si>
+  <si>
+    <t>New Content Found</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_NO_CONTENT</t>
+  </si>
+  <si>
+    <t>No New Content Found</t>
   </si>
 </sst>
 </file>
@@ -24761,10 +24785,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26474,6 +26498,74 @@
         <v>0</v>
       </c>
       <c r="E100" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="19" t="s">
+        <v>2944</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>2945</v>
+      </c>
+      <c r="C101" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="19" t="s">
+        <v>2947</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>2946</v>
+      </c>
+      <c r="C102" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="19" t="s">
+        <v>2948</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>2949</v>
+      </c>
+      <c r="C103" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="19" t="s">
+        <v>2950</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>2951</v>
+      </c>
+      <c r="C104" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="18" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>